<commit_message>
<Feature, UI> Tutorial, Acts
Improved intro tutorial.
Added volume slider.
Added act screen to story controller.
Removed options menu.
Simplified tutorial.
</commit_message>
<xml_diff>
--- a/Beyond The Veil - Story.xlsx
+++ b/Beyond The Veil - Story.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18620" activeTab="4"/>
+    <workbookView windowHeight="18620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wanderer" sheetId="1" r:id="rId1"/>
@@ -545,9 +545,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -585,8 +585,79 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -601,38 +672,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -640,32 +679,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -692,38 +716,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -738,7 +738,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -750,7 +774,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -762,37 +858,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -804,121 +912,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -950,32 +950,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -987,15 +961,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1015,6 +980,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1029,12 +1020,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1052,134 +1052,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1202,15 +1202,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1549,8 +1540,6 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
       <c r="D1" s="3"/>
       <c r="E1"/>
       <c r="F1"/>
@@ -3327,14 +3316,14 @@
   <sheetPr/>
   <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="2" width="10.7272727272727" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="8.72727272727273" style="6"/>
+    <col min="3" max="16383" width="8.72727272727273" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
@@ -3342,12 +3331,12 @@
         <v>36</v>
       </c>
       <c r="B1" s="7"/>
-      <c r="C1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
+      <c r="C1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
     </row>
     <row r="2" spans="1:28">
       <c r="A2" s="3" t="s">
@@ -3359,11 +3348,11 @@
       <c r="C2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
     </row>
     <row r="3" spans="1:28">
       <c r="A3" s="3" t="s">
@@ -3375,11 +3364,11 @@
       <c r="C3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
     </row>
     <row r="4" spans="1:28">
       <c r="A4" s="3" t="s">
@@ -3391,11 +3380,11 @@
       <c r="C4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
     </row>
     <row r="5" spans="1:28">
       <c r="A5" s="3" t="s">
@@ -3407,11 +3396,11 @@
       <c r="C5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
     </row>
     <row r="6" spans="1:28">
       <c r="A6" s="3" t="s">
@@ -3423,11 +3412,11 @@
       <c r="C6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="8"/>
-      <c r="AB6" s="8"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
     </row>
     <row r="7" spans="1:28">
       <c r="A7" s="3" t="s">
@@ -3439,11 +3428,11 @@
       <c r="C7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="8"/>
-      <c r="AB7" s="8"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
     </row>
     <row r="8" spans="1:28">
       <c r="A8" s="3" t="s">
@@ -3455,11 +3444,11 @@
       <c r="C8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="8"/>
-      <c r="AB8" s="8"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
     </row>
     <row r="9" spans="1:28">
       <c r="A9" s="3" t="s">
@@ -3471,678 +3460,678 @@
       <c r="C9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="8"/>
-      <c r="AA9" s="8"/>
-      <c r="AB9" s="8"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
     </row>
     <row r="10" spans="1:28">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="6">
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="8"/>
-      <c r="Z10" s="8"/>
-      <c r="AA10" s="8"/>
-      <c r="AB10" s="8"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
     </row>
     <row r="11" spans="1:28">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="6">
         <v>2</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="8"/>
-      <c r="AB11" s="8"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
     </row>
     <row r="12" spans="1:28">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="6">
         <v>3</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="8"/>
-      <c r="AA12" s="8"/>
-      <c r="AB12" s="8"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
     </row>
     <row r="13" spans="1:28">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="6">
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="8"/>
-      <c r="AB13" s="8"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
     </row>
     <row r="14" spans="1:28">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="6">
         <v>2</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="8"/>
-      <c r="AA14" s="8"/>
-      <c r="AB14" s="8"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
     </row>
     <row r="15" spans="1:28">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="6">
         <v>3</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="8"/>
-      <c r="AA15" s="8"/>
-      <c r="AB15" s="8"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
     </row>
     <row r="16" spans="1:28">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="6">
         <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="8"/>
-      <c r="Z16" s="8"/>
-      <c r="AA16" s="8"/>
-      <c r="AB16" s="8"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
     </row>
     <row r="17" spans="1:28">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="6">
         <v>2</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="8"/>
-      <c r="AA17" s="8"/>
-      <c r="AB17" s="8"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3"/>
     </row>
     <row r="18" spans="1:28">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="6">
         <v>3</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="X18" s="8"/>
-      <c r="Y18" s="8"/>
-      <c r="Z18" s="8"/>
-      <c r="AA18" s="8"/>
-      <c r="AB18" s="8"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
     </row>
     <row r="19" spans="1:28">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="6">
         <v>4</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="X19" s="8"/>
-      <c r="Y19" s="8"/>
-      <c r="Z19" s="8"/>
-      <c r="AA19" s="8"/>
-      <c r="AB19" s="8"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="3"/>
     </row>
     <row r="20" spans="1:28">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="6">
         <v>1</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="X20" s="8"/>
-      <c r="Y20" s="8"/>
-      <c r="Z20" s="8"/>
-      <c r="AA20" s="8"/>
-      <c r="AB20" s="8"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3"/>
     </row>
     <row r="21" spans="1:28">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="6">
         <v>2</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="X21" s="8"/>
-      <c r="Y21" s="8"/>
-      <c r="Z21" s="8"/>
-      <c r="AA21" s="8"/>
-      <c r="AB21" s="8"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
     </row>
     <row r="22" spans="1:28">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="6">
         <v>3</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="X22" s="8"/>
-      <c r="Y22" s="8"/>
-      <c r="Z22" s="8"/>
-      <c r="AA22" s="8"/>
-      <c r="AB22" s="8"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
     </row>
     <row r="23" spans="1:28">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="6">
         <v>4</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="X23" s="8"/>
-      <c r="Y23" s="8"/>
-      <c r="Z23" s="8"/>
-      <c r="AA23" s="8"/>
-      <c r="AB23" s="8"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
     </row>
     <row r="24" spans="1:28">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="6">
         <v>5</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="X24" s="8"/>
-      <c r="Y24" s="8"/>
-      <c r="Z24" s="8"/>
-      <c r="AA24" s="8"/>
-      <c r="AB24" s="8"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3"/>
     </row>
     <row r="25" spans="24:28">
-      <c r="X25" s="8"/>
-      <c r="Y25" s="8"/>
-      <c r="Z25" s="8"/>
-      <c r="AA25" s="8"/>
-      <c r="AB25" s="8"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
     </row>
     <row r="26" spans="24:28">
-      <c r="X26" s="8"/>
-      <c r="Y26" s="8"/>
-      <c r="Z26" s="8"/>
-      <c r="AA26" s="8"/>
-      <c r="AB26" s="8"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
     </row>
     <row r="28" spans="4:28">
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="8"/>
-      <c r="W28" s="8"/>
-      <c r="X28" s="8"/>
-      <c r="Y28" s="8"/>
-      <c r="Z28" s="8"/>
-      <c r="AA28" s="8"/>
-      <c r="AB28" s="8"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3"/>
     </row>
     <row r="29" spans="4:28">
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="8"/>
-      <c r="V29" s="8"/>
-      <c r="W29" s="8"/>
-      <c r="X29" s="8"/>
-      <c r="Y29" s="8"/>
-      <c r="Z29" s="8"/>
-      <c r="AA29" s="8"/>
-      <c r="AB29" s="8"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3"/>
     </row>
     <row r="30" spans="4:28">
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="8"/>
-      <c r="W30" s="8"/>
-      <c r="X30" s="8"/>
-      <c r="Y30" s="8"/>
-      <c r="Z30" s="8"/>
-      <c r="AA30" s="8"/>
-      <c r="AB30" s="8"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3"/>
     </row>
     <row r="31" spans="4:28">
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="8"/>
-      <c r="W31" s="8"/>
-      <c r="X31" s="8"/>
-      <c r="Y31" s="8"/>
-      <c r="Z31" s="8"/>
-      <c r="AA31" s="8"/>
-      <c r="AB31" s="8"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="3"/>
     </row>
     <row r="32" spans="4:28">
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="8"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="8"/>
-      <c r="W32" s="8"/>
-      <c r="X32" s="8"/>
-      <c r="Y32" s="8"/>
-      <c r="Z32" s="8"/>
-      <c r="AA32" s="8"/>
-      <c r="AB32" s="8"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3"/>
     </row>
     <row r="33" spans="4:28">
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="8"/>
-      <c r="W33" s="8"/>
-      <c r="X33" s="8"/>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="8"/>
-      <c r="AA33" s="8"/>
-      <c r="AB33" s="8"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="3"/>
     </row>
     <row r="35" spans="18:28">
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="8"/>
-      <c r="V35" s="8"/>
-      <c r="W35" s="8"/>
-      <c r="X35" s="8"/>
-      <c r="Y35" s="8"/>
-      <c r="Z35" s="8"/>
-      <c r="AA35" s="8"/>
-      <c r="AB35" s="8"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+      <c r="V35" s="3"/>
+      <c r="W35" s="3"/>
+      <c r="X35" s="3"/>
+      <c r="Y35" s="3"/>
+      <c r="Z35" s="3"/>
+      <c r="AA35" s="3"/>
+      <c r="AB35" s="3"/>
     </row>
     <row r="36" spans="18:28">
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="8"/>
-      <c r="U36" s="8"/>
-      <c r="V36" s="8"/>
-      <c r="W36" s="8"/>
-      <c r="X36" s="8"/>
-      <c r="Y36" s="8"/>
-      <c r="Z36" s="8"/>
-      <c r="AA36" s="8"/>
-      <c r="AB36" s="8"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="3"/>
+      <c r="X36" s="3"/>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3"/>
+      <c r="AA36" s="3"/>
+      <c r="AB36" s="3"/>
     </row>
     <row r="37" spans="18:28">
-      <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
-      <c r="T37" s="8"/>
-      <c r="U37" s="8"/>
-      <c r="V37" s="8"/>
-      <c r="W37" s="8"/>
-      <c r="X37" s="8"/>
-      <c r="Y37" s="8"/>
-      <c r="Z37" s="8"/>
-      <c r="AA37" s="8"/>
-      <c r="AB37" s="8"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="3"/>
+      <c r="X37" s="3"/>
+      <c r="Y37" s="3"/>
+      <c r="Z37" s="3"/>
+      <c r="AA37" s="3"/>
+      <c r="AB37" s="3"/>
     </row>
     <row r="38" spans="18:28">
-      <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
-      <c r="T38" s="8"/>
-      <c r="U38" s="8"/>
-      <c r="V38" s="8"/>
-      <c r="W38" s="8"/>
-      <c r="X38" s="8"/>
-      <c r="Y38" s="8"/>
-      <c r="Z38" s="8"/>
-      <c r="AA38" s="8"/>
-      <c r="AB38" s="8"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="3"/>
+      <c r="W38" s="3"/>
+      <c r="X38" s="3"/>
+      <c r="Y38" s="3"/>
+      <c r="Z38" s="3"/>
+      <c r="AA38" s="3"/>
+      <c r="AB38" s="3"/>
     </row>
     <row r="39" spans="18:28">
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
-      <c r="T39" s="8"/>
-      <c r="U39" s="8"/>
-      <c r="V39" s="8"/>
-      <c r="W39" s="8"/>
-      <c r="X39" s="8"/>
-      <c r="Y39" s="8"/>
-      <c r="Z39" s="8"/>
-      <c r="AA39" s="8"/>
-      <c r="AB39" s="8"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Y39" s="3"/>
+      <c r="Z39" s="3"/>
+      <c r="AA39" s="3"/>
+      <c r="AB39" s="3"/>
     </row>
     <row r="40" spans="18:28">
-      <c r="R40" s="8"/>
-      <c r="S40" s="8"/>
-      <c r="T40" s="8"/>
-      <c r="U40" s="8"/>
-      <c r="V40" s="8"/>
-      <c r="W40" s="8"/>
-      <c r="X40" s="8"/>
-      <c r="Y40" s="8"/>
-      <c r="Z40" s="8"/>
-      <c r="AA40" s="8"/>
-      <c r="AB40" s="8"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3"/>
+      <c r="V40" s="3"/>
+      <c r="W40" s="3"/>
+      <c r="X40" s="3"/>
+      <c r="Y40" s="3"/>
+      <c r="Z40" s="3"/>
+      <c r="AA40" s="3"/>
+      <c r="AB40" s="3"/>
     </row>
     <row r="41" spans="18:28">
-      <c r="R41" s="8"/>
-      <c r="S41" s="8"/>
-      <c r="T41" s="8"/>
-      <c r="U41" s="8"/>
-      <c r="V41" s="8"/>
-      <c r="W41" s="8"/>
-      <c r="X41" s="8"/>
-      <c r="Y41" s="8"/>
-      <c r="Z41" s="8"/>
-      <c r="AA41" s="8"/>
-      <c r="AB41" s="8"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+      <c r="T41" s="3"/>
+      <c r="U41" s="3"/>
+      <c r="V41" s="3"/>
+      <c r="W41" s="3"/>
+      <c r="X41" s="3"/>
+      <c r="Y41" s="3"/>
+      <c r="Z41" s="3"/>
+      <c r="AA41" s="3"/>
+      <c r="AB41" s="3"/>
     </row>
     <row r="42" spans="18:28">
-      <c r="R42" s="8"/>
-      <c r="S42" s="8"/>
-      <c r="T42" s="8"/>
-      <c r="U42" s="8"/>
-      <c r="V42" s="8"/>
-      <c r="W42" s="8"/>
-      <c r="X42" s="8"/>
-      <c r="Y42" s="8"/>
-      <c r="Z42" s="8"/>
-      <c r="AA42" s="8"/>
-      <c r="AB42" s="8"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="3"/>
+      <c r="X42" s="3"/>
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="3"/>
+      <c r="AA42" s="3"/>
+      <c r="AB42" s="3"/>
     </row>
     <row r="43" spans="18:28">
-      <c r="R43" s="8"/>
-      <c r="S43" s="8"/>
-      <c r="T43" s="8"/>
-      <c r="U43" s="8"/>
-      <c r="V43" s="8"/>
-      <c r="W43" s="8"/>
-      <c r="X43" s="8"/>
-      <c r="Y43" s="8"/>
-      <c r="Z43" s="8"/>
-      <c r="AA43" s="8"/>
-      <c r="AB43" s="8"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="3"/>
+      <c r="X43" s="3"/>
+      <c r="Y43" s="3"/>
+      <c r="Z43" s="3"/>
+      <c r="AA43" s="3"/>
+      <c r="AB43" s="3"/>
     </row>
     <row r="44" spans="18:28">
-      <c r="R44" s="8"/>
-      <c r="S44" s="8"/>
-      <c r="T44" s="8"/>
-      <c r="U44" s="8"/>
-      <c r="V44" s="8"/>
-      <c r="W44" s="8"/>
-      <c r="X44" s="8"/>
-      <c r="Y44" s="8"/>
-      <c r="Z44" s="8"/>
-      <c r="AA44" s="8"/>
-      <c r="AB44" s="8"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="3"/>
+      <c r="U44" s="3"/>
+      <c r="V44" s="3"/>
+      <c r="W44" s="3"/>
+      <c r="X44" s="3"/>
+      <c r="Y44" s="3"/>
+      <c r="Z44" s="3"/>
+      <c r="AA44" s="3"/>
+      <c r="AB44" s="3"/>
     </row>
     <row r="45" spans="18:28">
-      <c r="R45" s="8"/>
-      <c r="S45" s="8"/>
-      <c r="T45" s="8"/>
-      <c r="U45" s="8"/>
-      <c r="V45" s="8"/>
-      <c r="W45" s="8"/>
-      <c r="X45" s="8"/>
-      <c r="Y45" s="8"/>
-      <c r="Z45" s="8"/>
-      <c r="AA45" s="8"/>
-      <c r="AB45" s="8"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="3"/>
+      <c r="U45" s="3"/>
+      <c r="V45" s="3"/>
+      <c r="W45" s="3"/>
+      <c r="X45" s="3"/>
+      <c r="Y45" s="3"/>
+      <c r="Z45" s="3"/>
+      <c r="AA45" s="3"/>
+      <c r="AB45" s="3"/>
     </row>
     <row r="46" spans="18:28">
-      <c r="R46" s="8"/>
-      <c r="S46" s="8"/>
-      <c r="T46" s="8"/>
-      <c r="U46" s="8"/>
-      <c r="V46" s="8"/>
-      <c r="W46" s="8"/>
-      <c r="X46" s="8"/>
-      <c r="Y46" s="8"/>
-      <c r="Z46" s="8"/>
-      <c r="AA46" s="8"/>
-      <c r="AB46" s="8"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="3"/>
+      <c r="T46" s="3"/>
+      <c r="U46" s="3"/>
+      <c r="V46" s="3"/>
+      <c r="W46" s="3"/>
+      <c r="X46" s="3"/>
+      <c r="Y46" s="3"/>
+      <c r="Z46" s="3"/>
+      <c r="AA46" s="3"/>
+      <c r="AB46" s="3"/>
     </row>
     <row r="47" spans="18:28">
-      <c r="R47" s="8"/>
-      <c r="S47" s="8"/>
-      <c r="T47" s="8"/>
-      <c r="U47" s="8"/>
-      <c r="V47" s="8"/>
-      <c r="W47" s="8"/>
-      <c r="X47" s="8"/>
-      <c r="Y47" s="8"/>
-      <c r="Z47" s="8"/>
-      <c r="AA47" s="8"/>
-      <c r="AB47" s="8"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="3"/>
+      <c r="T47" s="3"/>
+      <c r="U47" s="3"/>
+      <c r="V47" s="3"/>
+      <c r="W47" s="3"/>
+      <c r="X47" s="3"/>
+      <c r="Y47" s="3"/>
+      <c r="Z47" s="3"/>
+      <c r="AA47" s="3"/>
+      <c r="AB47" s="3"/>
     </row>
     <row r="48" spans="18:28">
-      <c r="R48" s="8"/>
-      <c r="S48" s="8"/>
-      <c r="T48" s="8"/>
-      <c r="U48" s="8"/>
-      <c r="V48" s="8"/>
-      <c r="W48" s="8"/>
-      <c r="X48" s="8"/>
-      <c r="Y48" s="8"/>
-      <c r="Z48" s="8"/>
-      <c r="AA48" s="8"/>
-      <c r="AB48" s="8"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="3"/>
+      <c r="T48" s="3"/>
+      <c r="U48" s="3"/>
+      <c r="V48" s="3"/>
+      <c r="W48" s="3"/>
+      <c r="X48" s="3"/>
+      <c r="Y48" s="3"/>
+      <c r="Z48" s="3"/>
+      <c r="AA48" s="3"/>
+      <c r="AB48" s="3"/>
     </row>
     <row r="49" spans="18:28">
-      <c r="R49" s="8"/>
-      <c r="S49" s="8"/>
-      <c r="T49" s="8"/>
-      <c r="U49" s="8"/>
-      <c r="V49" s="8"/>
-      <c r="W49" s="8"/>
-      <c r="X49" s="8"/>
-      <c r="Y49" s="8"/>
-      <c r="Z49" s="8"/>
-      <c r="AA49" s="8"/>
-      <c r="AB49" s="8"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
+      <c r="T49" s="3"/>
+      <c r="U49" s="3"/>
+      <c r="V49" s="3"/>
+      <c r="W49" s="3"/>
+      <c r="X49" s="3"/>
+      <c r="Y49" s="3"/>
+      <c r="Z49" s="3"/>
+      <c r="AA49" s="3"/>
+      <c r="AB49" s="3"/>
     </row>
     <row r="50" spans="18:28">
-      <c r="R50" s="8"/>
-      <c r="S50" s="8"/>
-      <c r="T50" s="8"/>
-      <c r="U50" s="8"/>
-      <c r="V50" s="8"/>
-      <c r="W50" s="8"/>
-      <c r="X50" s="8"/>
-      <c r="Y50" s="8"/>
-      <c r="Z50" s="8"/>
-      <c r="AA50" s="8"/>
-      <c r="AB50" s="8"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="3"/>
+      <c r="T50" s="3"/>
+      <c r="U50" s="3"/>
+      <c r="V50" s="3"/>
+      <c r="W50" s="3"/>
+      <c r="X50" s="3"/>
+      <c r="Y50" s="3"/>
+      <c r="Z50" s="3"/>
+      <c r="AA50" s="3"/>
+      <c r="AB50" s="3"/>
     </row>
     <row r="51" spans="18:28">
-      <c r="R51" s="8"/>
-      <c r="S51" s="8"/>
-      <c r="T51" s="8"/>
-      <c r="U51" s="8"/>
-      <c r="V51" s="8"/>
-      <c r="W51" s="8"/>
-      <c r="X51" s="8"/>
-      <c r="Y51" s="8"/>
-      <c r="Z51" s="8"/>
-      <c r="AA51" s="8"/>
-      <c r="AB51" s="8"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
+      <c r="T51" s="3"/>
+      <c r="U51" s="3"/>
+      <c r="V51" s="3"/>
+      <c r="W51" s="3"/>
+      <c r="X51" s="3"/>
+      <c r="Y51" s="3"/>
+      <c r="Z51" s="3"/>
+      <c r="AA51" s="3"/>
+      <c r="AB51" s="3"/>
     </row>
     <row r="52" spans="18:28">
-      <c r="R52" s="8"/>
-      <c r="S52" s="8"/>
-      <c r="T52" s="8"/>
-      <c r="U52" s="8"/>
-      <c r="V52" s="8"/>
-      <c r="W52" s="8"/>
-      <c r="X52" s="8"/>
-      <c r="Y52" s="8"/>
-      <c r="Z52" s="8"/>
-      <c r="AA52" s="8"/>
-      <c r="AB52" s="8"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3"/>
+      <c r="U52" s="3"/>
+      <c r="V52" s="3"/>
+      <c r="W52" s="3"/>
+      <c r="X52" s="3"/>
+      <c r="Y52" s="3"/>
+      <c r="Z52" s="3"/>
+      <c r="AA52" s="3"/>
+      <c r="AB52" s="3"/>
     </row>
     <row r="53" spans="18:28">
-      <c r="R53" s="8"/>
-      <c r="S53" s="8"/>
-      <c r="T53" s="8"/>
-      <c r="U53" s="8"/>
-      <c r="V53" s="8"/>
-      <c r="W53" s="8"/>
-      <c r="X53" s="8"/>
-      <c r="Y53" s="8"/>
-      <c r="Z53" s="8"/>
-      <c r="AA53" s="8"/>
-      <c r="AB53" s="8"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3"/>
+      <c r="T53" s="3"/>
+      <c r="U53" s="3"/>
+      <c r="V53" s="3"/>
+      <c r="W53" s="3"/>
+      <c r="X53" s="3"/>
+      <c r="Y53" s="3"/>
+      <c r="Z53" s="3"/>
+      <c r="AA53" s="3"/>
+      <c r="AB53" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -4953,13 +4942,13 @@
   <sheetPr/>
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.2727272727273" customWidth="1"/>
+    <col min="1" max="1" width="30.4545454545455" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">

</xml_diff>

<commit_message>
<Feature, Balance> Claim, Tomb
Added visual effect to tomb.
Must break tomb 'shell' for boss to spawn.
Added fade in effect on serpent parts.
Damaged serpent parts now faded rather than destroyed.
Fixed claim region not generating resources.
Fixed buttons being selected when a valid button is already selected.
Added navigation for volume slider.
Removed 3 character classes.
Slightly modified remaining class skills.
Added bomb attack to starfish.
</commit_message>
<xml_diff>
--- a/Beyond The Veil - Story.xlsx
+++ b/Beyond The Veil - Story.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18620" activeTab="1"/>
+    <workbookView windowHeight="18620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Wanderer" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169">
   <si>
     <t>Wanderer Journal</t>
   </si>
@@ -227,18 +227,6 @@
     <t>When the graves were filled we argued about what should be done. Words turned to accusations, and accusations into insults. By midday the first stone had been thrown, and sure enough others followed. The village turned to chaos, so I gathered my husband and daughter together and we ran as far into the forest as we could. There were others- families, couples, elders, and children, all running from the village. We could hear the pursuit behind us. The people we had lived with every day now hunted us like we were animals. I did not dare to look back, I only ran. By the time the shouts and screams had died away I was lost. The trees had thinned, and the rich soil turned to the sand and dirt of the great wasteland. I turned to find my family, but I could not see them. I tried to return to the village, but I could not find my way back. To this day I have not seen them. I tell myself they are lost now, but I will keep searching, I will hold out hope until the day I die.</t>
   </si>
   <si>
-    <t>An Uncaring World</t>
-  </si>
-  <si>
-    <t>Ghost</t>
-  </si>
-  <si>
-    <t>Things weren’t always this way. I recall I time before the winds were dry and laden with ash, a time when we would welcome the sight of another, rather then recoil at the fear of danger. Sometimes its hard to say if it was all a dream, a misrememberance of my childhood. I prefer to think we are in a dream now, because even then we would one day wake up, even if now we have to live in this nightmare. I dont know if I had a family, I must have done, though they are long dead by now I assume. Wandering is all I know, going from place to place, there is so much that has been left undone in this world. I find newspapers, books, diaries, strange devices that sputter with light and sound but go dark before long, never to wake.</t>
-  </si>
-  <si>
-    <t>Happily I find myself without sadness in these dying days. I have no remorse or incomplete doings, none to to weep for, and nothing to rejoice. My only lament is my lack of feeling, though Im sure you envy my stagnant mind. What little memories I have are no more real to me than scribblings in a book. There are those who call my a ghost, because that is who I am, a ghost in this purgatory, drifting lifelessly through an equally lifeless plane. I will follow you though, though like a leaf on a breeze I do not know why. I assure you I do not fear death, for I cannot truly call my existence life.</t>
-  </si>
-  <si>
     <t>What Lies Within</t>
   </si>
   <si>
@@ -275,7 +263,7 @@
     <t>A Question of Faith</t>
   </si>
   <si>
-    <t>Watcher</t>
+    <t>Survivor</t>
   </si>
   <si>
     <t>I once met a band of wandering holy men. “Hail”, I said, for the road was lonely, and any company was welcome. “Bless you, daughter”, they said, though I was not their son, “Are you making the pilgrimage too?” they asked. “No, brothers, I am not. For this is a godless world, and faith has no place in it” I replied. At this they made an unusual smile. “My daughter, do you not believe in the gods?” asked one. “It is well known that the gods abandoned our world, so why would I worship those that would leave us to this fate?” I replied. “But my child it was not they who caused the world to come to ruin. Their plan is perfect, it is an opportunity for us to prove ourselves worthy. That is our pursuit” another said. “Then that is a worthy goal, and I commend you for it, but by testing our worthiness the gods have demonstrated that they do not have faith in us. So why should I have faith in those who do not have faith in me?”.</t>
@@ -544,10 +532,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -585,11 +573,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -601,9 +588,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -611,6 +651,14 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -626,15 +674,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -647,9 +694,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -658,65 +705,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -738,7 +726,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -750,31 +834,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -792,13 +870,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -810,115 +900,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -936,31 +924,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -976,17 +940,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1024,8 +977,43 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1034,7 +1022,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1052,130 +1040,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3316,7 +3304,7 @@
   <sheetPr/>
   <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -4142,10 +4130,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -4313,7 +4301,7 @@
       <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E7" s="2"/>
@@ -4357,16 +4345,16 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -4383,13 +4371,13 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>76</v>
@@ -4409,13 +4397,13 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C11" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>77</v>
@@ -4435,16 +4423,16 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -4461,16 +4449,16 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="C13" s="2">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -4487,13 +4475,13 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C14" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>82</v>
@@ -4513,13 +4501,13 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C15" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>83</v>
@@ -4547,7 +4535,7 @@
       <c r="C16" s="2">
         <v>1</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="4" t="s">
         <v>86</v>
       </c>
       <c r="E16" s="2"/>
@@ -4573,7 +4561,7 @@
       <c r="C17" s="2">
         <v>2</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>87</v>
       </c>
       <c r="E17" s="2"/>
@@ -4591,16 +4579,16 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="2">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -4615,70 +4603,18 @@
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C19" s="2">
-        <v>2</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-    </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" s="2">
-        <v>3</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21">
-        <v>4</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -4704,12 +4640,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -4718,12 +4654,12 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -4732,12 +4668,12 @@
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -4746,12 +4682,12 @@
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -4760,12 +4696,12 @@
         <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -4774,12 +4710,12 @@
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -4788,12 +4724,12 @@
         <v>2</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -4802,12 +4738,12 @@
         <v>3</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -4816,12 +4752,12 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
@@ -4830,12 +4766,12 @@
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
@@ -4844,12 +4780,12 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -4858,12 +4794,12 @@
         <v>4</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
@@ -4872,12 +4808,12 @@
         <v>1</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
@@ -4886,12 +4822,12 @@
         <v>2</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B15" t="s">
         <v>31</v>
@@ -4900,12 +4836,12 @@
         <v>1</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
@@ -4914,12 +4850,12 @@
         <v>2</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
         <v>31</v>
@@ -4928,7 +4864,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -4953,13 +4889,13 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
@@ -4983,7 +4919,7 @@
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -4992,7 +4928,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -5015,7 +4951,7 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -5024,7 +4960,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -5047,7 +4983,7 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
@@ -5056,7 +4992,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -5079,7 +5015,7 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -5088,7 +5024,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -5111,7 +5047,7 @@
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B6" s="2">
         <v>2</v>
@@ -5120,7 +5056,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -5143,7 +5079,7 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B7" s="2">
         <v>3</v>
@@ -5152,7 +5088,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -5175,7 +5111,7 @@
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B8" s="2">
         <v>3</v>
@@ -5184,7 +5120,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -5207,7 +5143,7 @@
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B9" s="2">
         <v>3</v>
@@ -5216,7 +5152,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -5239,7 +5175,7 @@
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B10" s="2">
         <v>3</v>
@@ -5248,7 +5184,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -5271,7 +5207,7 @@
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B11" s="2">
         <v>4</v>
@@ -5280,7 +5216,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -5303,7 +5239,7 @@
     </row>
     <row r="12" spans="1:22">
       <c r="A12" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B12" s="2">
         <v>5</v>
@@ -5312,7 +5248,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -5335,7 +5271,7 @@
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B13" s="2">
         <v>5</v>
@@ -5344,7 +5280,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -5367,7 +5303,7 @@
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B14" s="2">
         <v>5</v>
@@ -5376,7 +5312,7 @@
         <v>3</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -5399,7 +5335,7 @@
     </row>
     <row r="15" spans="1:22">
       <c r="A15" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B15" s="2">
         <v>5</v>
@@ -5408,7 +5344,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -5431,7 +5367,7 @@
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B16" s="2">
         <v>6</v>
@@ -5440,7 +5376,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -5463,7 +5399,7 @@
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B17" s="2">
         <v>7</v>
@@ -5472,7 +5408,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -5495,7 +5431,7 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B18" s="2">
         <v>8</v>
@@ -5504,7 +5440,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -5527,7 +5463,7 @@
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B19" s="2">
         <v>9</v>
@@ -5536,7 +5472,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -5559,7 +5495,7 @@
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B20" s="2">
         <v>10</v>
@@ -5568,7 +5504,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -5591,7 +5527,7 @@
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B21" s="2">
         <v>11</v>
@@ -5600,7 +5536,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -5623,7 +5559,7 @@
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B22" s="2">
         <v>12</v>
@@ -5632,7 +5568,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -5655,7 +5591,7 @@
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B23" s="2">
         <v>13</v>
@@ -5664,7 +5600,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -5687,7 +5623,7 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B24" s="2">
         <v>14</v>
@@ -5696,7 +5632,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -5719,7 +5655,7 @@
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B25" s="2">
         <v>15</v>
@@ -5728,7 +5664,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -5751,7 +5687,7 @@
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B26" s="2">
         <v>16</v>
@@ -5760,7 +5696,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -5783,7 +5719,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B27">
         <v>17</v>
@@ -5792,12 +5728,12 @@
         <v>1</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B28">
         <v>17</v>
@@ -5806,12 +5742,12 @@
         <v>2</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B29">
         <v>17</v>
@@ -5820,7 +5756,7 @@
         <v>3</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
<Feature, UI> Enemies, Inventory Menu
Added invert colour shader for final story text.
Added boss rings to final battle.
Modified weapon volumes and ranges.
Fixed fire explosions audio looping.
Changed shatter audio timing.
Increased push force.
Changed act 1 text.
Added temple cleansed visual to map node.
Fixed map camera overlap.
Changed how burn/shatter/void is displayed in menu.
Improved performance by grouping fixedupdates and updates.
Fixed esc during inventory opening pause menu.
Updated consumable and crafting UI.
Reduced craft time.
Removed multicraft.
Fixed character skill 2 not unlocking.
Updated drone behaviour.
Fixed null playercombat references.
Fixed credits not opening correctly.
Added cook, boil, upgrade audio to craft.
Fixed load save on game over.
</commit_message>
<xml_diff>
--- a/Beyond The Veil - Story.xlsx
+++ b/Beyond The Veil - Story.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18620"/>
+    <workbookView windowHeight="18620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wanderer" sheetId="1" r:id="rId1"/>
@@ -299,22 +299,22 @@
     <t>Main Story</t>
   </si>
   <si>
-    <t>You wept. Alone, and in darkness. I watched you from across the great cold distances, and in you I saw myself. So I brought you here, to my world, so that we might both be saved. We are so alike, lost one. We can look upon these desolate plains with unfamiliar eyes. Yet this is my country, now dying and covered in darkness. Long ago, these lands were green, and I could walk amongst the trees and feel the grass beneath my feet. Now the groves are dead, and I pass like a shadow among them. Only the sun-scorched dirt remains- dry, and stained red by ancient war.</t>
-  </si>
-  <si>
-    <t>There were once five gods who roamed the world, guiding our people as parents guide their children. Five great kingdoms rose up, each dedicated to their own god. As we grew, so they waned. What was once a miracle to our ancestors became rote to us. Our cities climbed high into the sky, our machines worked the earth in our stead. Then one day, when we had all but forgotten our roots, they vanished. Seeing that we had no need for their influence any longer, they let us be. But the vacuum left by their absence was clear. Something changed, in the air, the earth, and sea. The essence that binds the world turned on us. It poisoned our minds, pitted us against each other. It soured the earth and awoke ceaseless winds. The gods are gone, and with them, our humanity.</t>
+    <t>You wept. Alone, and in darkness. I watched you across the great cold distance and in you I saw myself. I have brought you here, to my world, so that we might both be saved. We both can look upon these desolate plains with unfamiliar gaze. But this was once my home. Long before the darkness fell these lands were green. I would walk amongst the trees with feel the grass beneath my feet. Now the groves are dead, and I pass like a shadow among them. Only the sun-scorched dirt remains.</t>
+  </si>
+  <si>
+    <t>There were once five gods who roamed the world. Around them five great kingdoms were founded. Our civilisations grew with time. Miracles became rote; our cities rose high into the heavens and our machines worked the earth. The gods saw they were no longer needed, and so they retreated from the world of man. One day, when we had all but forgotten our roots, they vanished. But the vacuum left by their absence was clear. Something changed, in the air, the earth, and the sea. The essence that binds the world turned on us. It soured the earth and awoke ceaseless winds. The gods are gone, and with them, our humanity.</t>
+  </si>
+  <si>
+    <t>Ahead lies a dead world- a stagnant place where only barbarism and hopelessness remain. But I believe if we can bring back the gods we can restore it all. I know where they are. They sleep in the place between places, the dark realm beyond the veil of reality. There are five gates that lead to this realm, but they lie dormant, bound by seals set in eons past. I cannot break them, but I can guide you. Only together can the gods turn the tide of decay, and offer you the peace which you so dearly seek.</t>
+  </si>
+  <si>
+    <t>Your path is not an easy one, there will be dangers, both physical and psychological. The essence will seek to claim you. It will burrow into your thoughts and lay seeds of doubt. It once gave strength to the gods, now unbound it breeds only chaos.It feeds on our wants and fear. All you will encounter have succumbed to its influence. Some may still resist. Others, however, will stop at nothing to rid you from the world.</t>
   </si>
   <si>
     <t>You were lost, but I found you. Your memories have been hidden, for now, at least, but I cannot hide your pain. That you will have to bear. When you are ready I will tell you more. Until then you must endure. Trust in my words, I do not wish to deceive you. The gods can heal your grief, just as they can heal my world.</t>
   </si>
   <si>
-    <t>Ahead lies a dead world- a stagnant place where civilisation and prosperity have wasted with the passing of the ages, leaving only barbarism and hopelessness in their stead. But I believe we can restore it all, if we can bring back the gods. I know where they are, they sleep in the place between places, the dark realm beyond the veil of the waking world. There are five gates, five portals to this realm, but they lie dormant, bound by seals set in eons past. I cannot break them, for I have no body with which to walk, but you can. I can be your guide though. I can walk with you in the dusky plains and torrid peaks. Only together can the gods turn the tide of decay, and offer you the peace which you so dearly seek.</t>
-  </si>
-  <si>
-    <t>Your path is not an easy one, there will be dangers, both physical and psychological. The essence will want to take you as its own. It will burrow into your thoughts and lay the seeds of doubt. No doubt it will double its efforts to break you, as in this land of darkness you are like a shining beacon- foreign and uncorrupted. Once it gave strength to the gods, now unbound it breeds only chaos. Feeding on our wants, our fears, and that which we desire to say but do not give voice. All you will encounter, be it man, beast, or plant, have fallen to the disease. Some may still resist, and they may even offer to aid you. Others, however, will have fallen completely to the corruption, and they will stop at nothing to rid you from the world.</t>
-  </si>
-  <si>
-    <t>I have brought you to the gate of Eo, the gentle one. Here there is only one seal still unbroken. The gate hums with desire to be opened. Alas, I do not know where the seal may be, so you must search for me. When you have opened it, return here and place your hands upon the stones. Be prepared, for I do not know what you will find when you enter the gate. I will be waiting for you on the other side, no matter what happens.</t>
+    <t>I have brought you to the kingdom of Eo. Only one seal binds the gateway, and it lies hidden amongst the shifting desert sands. When it is broken return here and place your hands upon the stones. Be prepared, for I do not know what awaits you within. I will be waiting for you on the other side, no matter what happens.</t>
   </si>
   <si>
     <t>So it is done, you have passed through the gate and the realm between the shadows. You have done wonderfully. Already I hear Eo’s voice on the wind - calling for her lost siblings. How must it feel, to awaken from one nightmare into another, to see your beautiful world in ruins. I was there whilst it happened - I watched the life of the earth fade away. But I was cursed to remain as everything I loved turned to dust. I saw my friends and my family die, as I was doomed to solitude by immortality. I do not feel pity for the dead, wanderer, for it is the living alone who are left who grieve.</t>
@@ -697,10 +697,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -760,13 +760,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -775,8 +768,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -785,6 +787,21 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -806,6 +823,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -819,66 +874,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -891,25 +891,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -927,7 +921,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -939,13 +933,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -957,19 +957,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -981,13 +975,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1005,19 +1005,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1029,7 +1047,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1041,7 +1059,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1053,25 +1071,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1105,6 +1105,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1125,21 +1134,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1174,11 +1168,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1205,94 +1205,118 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1301,34 +1325,10 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1684,7 +1684,7 @@
   <sheetPr/>
   <dimension ref="A1:AA85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -3223,8 +3223,8 @@
   <sheetPr/>
   <dimension ref="A1:AB55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -3348,7 +3348,7 @@
       <c r="B8" s="3">
         <v>1</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="4" t="s">
         <v>99</v>
       </c>
       <c r="X8" s="3"/>
@@ -3364,7 +3364,7 @@
       <c r="B9" s="3">
         <v>2</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="4" t="s">
         <v>100</v>
       </c>
       <c r="X9" s="3"/>
@@ -3380,7 +3380,7 @@
       <c r="B10" s="3">
         <v>3</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="4" t="s">
         <v>101</v>
       </c>
       <c r="X10" s="3"/>
@@ -3396,7 +3396,7 @@
       <c r="B11" s="3">
         <v>4</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="4" t="s">
         <v>102</v>
       </c>
       <c r="X11" s="3"/>
@@ -3412,7 +3412,7 @@
       <c r="B12" s="6">
         <v>1</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="4" t="s">
         <v>103</v>
       </c>
       <c r="X12" s="3"/>
@@ -3428,7 +3428,7 @@
       <c r="B13" s="6">
         <v>2</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="4" t="s">
         <v>104</v>
       </c>
       <c r="X13" s="3"/>
@@ -3444,7 +3444,7 @@
       <c r="B14" s="6">
         <v>3</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="4" t="s">
         <v>105</v>
       </c>
       <c r="X14" s="3"/>
@@ -3460,7 +3460,7 @@
       <c r="B15" s="6">
         <v>4</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="4" t="s">
         <v>106</v>
       </c>
       <c r="X15" s="3"/>
@@ -3476,7 +3476,7 @@
       <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="4" t="s">
         <v>107</v>
       </c>
       <c r="X16" s="3"/>
@@ -3492,7 +3492,7 @@
       <c r="B17" s="6">
         <v>2</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="4" t="s">
         <v>108</v>
       </c>
       <c r="X17" s="3"/>
@@ -3508,7 +3508,7 @@
       <c r="B18" s="6">
         <v>3</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="4" t="s">
         <v>109</v>
       </c>
       <c r="X18" s="3"/>
@@ -3524,7 +3524,7 @@
       <c r="B19" s="6">
         <v>4</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="4" t="s">
         <v>110</v>
       </c>
       <c r="X19" s="3"/>
@@ -3540,7 +3540,7 @@
       <c r="B20" s="6">
         <v>1</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="4" t="s">
         <v>111</v>
       </c>
       <c r="X20" s="3"/>
@@ -3556,7 +3556,7 @@
       <c r="B21" s="6">
         <v>2</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="4" t="s">
         <v>112</v>
       </c>
       <c r="X21" s="3"/>
@@ -3572,7 +3572,7 @@
       <c r="B22" s="6">
         <v>3</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="4" t="s">
         <v>113</v>
       </c>
       <c r="X22" s="3"/>
@@ -3588,7 +3588,7 @@
       <c r="B23" s="6">
         <v>1</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="4" t="s">
         <v>115</v>
       </c>
       <c r="X23" s="3"/>
@@ -3604,7 +3604,7 @@
       <c r="B24" s="6">
         <v>2</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="4" t="s">
         <v>116</v>
       </c>
       <c r="X24" s="3"/>
@@ -3620,7 +3620,7 @@
       <c r="B25" s="6">
         <v>3</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="4" t="s">
         <v>117</v>
       </c>
       <c r="X25" s="3"/>
@@ -3636,7 +3636,7 @@
       <c r="B26" s="6">
         <v>4</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="4" t="s">
         <v>118</v>
       </c>
       <c r="X26" s="3"/>

</xml_diff>

<commit_message>
<UI, Bugfix> Reload, Spacebar, Credits, Void
Added better void damage visuals.
Fixed getting stuck in tutorial.
Now use spacebar to navigate through text.
Reload can be interrupted.
Reload now passive.
Clarified weapon behaviour on screen.
</commit_message>
<xml_diff>
--- a/Beyond The Veil - Story.xlsx
+++ b/Beyond The Veil - Story.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18620" activeTab="2"/>
+    <workbookView windowHeight="18620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Wanderer" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218">
   <si>
     <t>Wanderer Journal</t>
   </si>
@@ -616,7 +616,7 @@
     <t>Widow's Poem</t>
   </si>
   <si>
-    <t>When ice laden branches hang low,&lt;br&gt;And silence broken by call of crow,&lt;br&gt;When bright banners of war are still,&lt;br&gt;And the horns of battle are silent,&lt;br&gt;Will you come home to me?&lt;br&gt;&lt;br&gt;When the peals of artillery thunder have rung out,&lt;br&gt;And in muddy tracks grasses sprout,&lt;br&gt;When I have waited ten years and a day,&lt;br&gt;And the the glow of my youth turned grey,&lt;br&gt;Will you come home to me?</t>
+    <t>When ice laden branches hang low,|br|And silence broken by call of crow,|br|When bright banners of war are still,|br|And the horns of battle are silent,|br|Will you come home to me?|br||br|When the peals of artillery thunder have rung out,|br|And in muddy tracks grasses sprout,|br|When I have waited ten years and a day,|br|And the the glow of my youth turned grey,|br|Will you come home to me?</t>
   </si>
   <si>
     <t>Burned Note</t>
@@ -640,7 +640,7 @@
     <t>A Child's Letter</t>
   </si>
   <si>
-    <t>Dear Mummy,&lt;br&gt;&lt;br&gt;Daddy says we have to leave home. He says we will be safe in the countryside, but I like it here and I don’t want to go. I told Daddy you are keeping us safe and that’s why you’ve been gone so long. Will you know where to find us when we move? I hope you will come home soon. I packed some of your things so that you won’t have to carry as much when you come. I took your bracelets and your picture of us and the stuffed pig that sits in the window because I know you like him. I don’t want to move. Lots of my friends are still here. Daddy says they will be moving too, but they won’t be coming with us. He hasn’t been in a good mood since you left. It will be my birthday soon, so I hope you will be home by then.&lt;br&gt;Love you lots and lots,&lt;br&gt;Phoebe&lt;br&gt;&lt;br&gt;PS I didn’t pack the dress grandma bought me because I hate it.</t>
+    <t>Dear Mummy,|br||br|Daddy says we have to leave home. He says we will be safe in the countryside, but I like it here and I don’t want to go. I told Daddy you are keeping us safe and that’s why you’ve been gone so long. Will you know where to find us when we move? I hope you will come home soon. I packed some of your things so that you won’t have to carry as much when you come. I took your bracelets and your picture of us and the stuffed pig that sits in the window because I know you like him. I don’t want to move. Lots of my friends are still here. Daddy says they will be moving too, but they won’t be coming with us. He hasn’t been in a good mood since you left. It will be my birthday soon, so I hope you will be home by then.|br|Love you lots and lots,|br|Phoebe|br||br|PS I didn’t pack the dress grandma bought me because I hate it.</t>
   </si>
   <si>
     <t>King's Lament</t>
@@ -655,13 +655,19 @@
     <t>As the glow of the candle grows, so too do the shadows cast by the flame. I say to those who stare too long into the candles bright fire, do not look away, and to those who know only darkness, do not approach too close to the flame. Those who know only light can but despair at the depths of darkness. Meanwhile those who wrap themselves in shadow will do all they can to dim the light when it is cast upon them.</t>
   </si>
   <si>
-    <t>Corypthos' Tomb</t>
+    <t>Corypthos' Tomb I</t>
   </si>
   <si>
     <t>He is not here, he is gone, you will never find him.</t>
   </si>
   <si>
+    <t>Corypthos' Tomb II</t>
+  </si>
+  <si>
     <t>Somewhere, Beyond the Veil, there sits an aged king upon an aged throne, and he weeps for you all.</t>
+  </si>
+  <si>
+    <t>Corypthos' Tomb III</t>
   </si>
   <si>
     <t>In the realm of shadow and blackness we all go. Our arrival goes unannounced, for you see, there is no light in the land of the dead.</t>
@@ -672,8 +678,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -720,13 +726,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -743,6 +742,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -753,7 +798,51 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -768,90 +857,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -872,7 +878,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -884,13 +938,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -902,19 +968,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -932,43 +998,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -980,25 +1028,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1010,31 +1040,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1046,7 +1052,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1069,6 +1075,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1080,17 +1101,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1110,6 +1120,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1125,30 +1144,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1157,12 +1152,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1180,130 +1186,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4052,7 +4058,7 @@
   <sheetPr/>
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
@@ -4548,8 +4554,8 @@
   <sheetPr/>
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -5579,7 +5585,7 @@
         <v>212</v>
       </c>
       <c r="B38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" t="s">
         <v>114</v>
@@ -5590,30 +5596,30 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39" t="s">
         <v>114</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
         <v>114</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
<Bugfix, Balance> Second character, Resources
Limited additional character count to 1.
Improved water and food balance.
Improved action progress bar.
Fixed close button not working in gear menu,
Fixed playing thunder in final battle.
Will menu now clearer.
Reduced meat drop count.
Added displayname to enemies.
Increased maelstrom shot speed lower bound.
Weather fades out when game ends.
Updated journal UI to be clearer.
Reduced character attribute max value to prevent float.parse errors.
</commit_message>
<xml_diff>
--- a/Beyond The Veil - Story.xlsx
+++ b/Beyond The Veil - Story.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18620" activeTab="3"/>
+    <workbookView windowHeight="18620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wanderer" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219">
   <si>
     <t>Wanderer Journal</t>
   </si>
@@ -28,22 +28,22 @@
     <t>Desert</t>
   </si>
   <si>
-    <t>The land before me is just as the Necromancer said- dark and dying. Even the dry ground seems to creak with hunger, eager to slake its thirst with my blood. There are others here. They are vague shapes on the horizon and subtle whispers on the wind. Purgatorial souls -  fearful and wary. If I am to be alone in my journey, then that is the way it must be.</t>
-  </si>
-  <si>
-    <t>Sensations come and go, like memories without context. Warm light on my back. The green glow of a sunlit canopy, and dappled colour on the ground where the light breaks through. They match nothing of what I have experienced. Here there are no living trees, no leaf-laden boughs, only dead roots, withered stumps, and stifling heat.</t>
-  </si>
-  <si>
-    <t>What was once familiar is now foreign to me - the sky a deep shade of crimson, lit by the weak glow of three ailing suns, and the air heavy with dread expectation. At night the heavens glitter with the light of unknown constellations. I am not sure if I will ever share the Necromancer’s faith, but if the alternative is a life of solitude and fear, well, then I will go wherever she bids.</t>
-  </si>
-  <si>
-    <t>Though the ground is arid and the air still the desert is not completely devoid of life. The gentle rustle of the breeze is broken by the coo of small birds and the churr of insects. The plants I have seen are as brittle and cracked as the dry sand they grow in. The few fruit they bear are wizened, and coloured with such evil hues I would not dare to touch them.</t>
-  </si>
-  <si>
-    <t>More unsettling than the blood red sky is the loss I feel inside. I cannot shake it. What has the Necromancer hidden from me? I cannot remember anything of where I came, nor how I came to be here. It is like there is a thick fog in my mind, pushing all else beyond the boundaries of my subconscious.</t>
-  </si>
-  <si>
-    <t>I have slept well here, for the first time in a long time I know. In my dreams I am in a cavernous room. There are no walls. Far above I can see a stone roof, arching away into the blackness beyond. I let myself lie back and drift in silence on the murky currents of my thoughts.</t>
+    <t>The land before me is just as the Necromancer said- dark and dying. Even the dry ground seems to creak with hunger, eager to slake its thirst with my blood. There are others here. They are vague shapes on the horizon and subtle whispers on the wind. Purgatorial souls -  fearful and wary. If I am to be alone in my journey then that is the way it must be.</t>
+  </si>
+  <si>
+    <t>Sensations come and go, like memories without context. Warm light on my back. The green glow of a sunlit canopy, and dappled colour on the ground where the light breaks through. They match nothing of what I have experienced. Here there are no living trees, no leaf-laden boughs, only dead roots, withered stumps, and the stifling heat.</t>
+  </si>
+  <si>
+    <t>What was once familiar is now foreign to me - the sky a deep shade of crimson, lit by the weak glow of three ailing suns, and the air heavy with dread expectation. At night the heavens glitter with the light of unknown constellations. I am not sure if I will ever share the Necromancer’s faith, but if the alternative is a life of solitude and fear then I will go wherever she bids.</t>
+  </si>
+  <si>
+    <t>Though the ground is arid and the air still, the desert is not completely devoid of life. The gentle rustle of the breeze is broken by the coo of small birds and the churr of insects. The plants I have seen are as brittle and cracked as the dry sand they grow in. The few fruit they bear are wizened, and coloured with such evil hues I would not dare to touch them.</t>
+  </si>
+  <si>
+    <t>More unsettling than the blood red sky is the loss I feel inside. I cannot shake it. What has the Necromancer hidden from me? I cannot remember anything of where I came, nor how I came to be here. It is as if there is a fog in my mind, pushing all else beyond the boundaries of my subconscious.</t>
+  </si>
+  <si>
+    <t>I have slept well here. I have even dreamed- for the first time in a long time. In my dreams I am in a cavernous room. There are no walls. Far above I can see a stone roof, arching away into the blackness beyond. I let myself lie back and drift in silence on the murky currents of my thoughts.</t>
   </si>
   <si>
     <t>I feel my emotions ebb and flow like the tide, and I allow myself to be borne away on their currents. With every swell come glimpses of my past, clearer now. But as every swell passes, so do these memories fade. I cannot hold onto them in this bleak and desolate world.</t>
@@ -55,7 +55,7 @@
     <t>My dreams are strange. When I am in them they seem so utterly convincing that I wake with a start. The shift to reality is unwelcome, for in my dreams I am at peace, and in this nightmare world I cannot escape the weight of my grief.</t>
   </si>
   <si>
-    <t>I am not a man of faith, I do not believe in gods or demons, but I will do what I can to heal the wound inside me. I cannot live with it, and I fear it will only deepen with time. I have already seen so much that does not make sense, so I will find the gates, and perhaps I will find deliverance.</t>
+    <t>I am not a man of faith. I do not believe in gods or demons. But I will do what I can to heal the wound inside me. I cannot live with it, and I fear it will only deepen with time. I have already seen so much that does not make sense, so I will find the gates, and perhaps I will find deliverance.</t>
   </si>
   <si>
     <t>Ebb and Flow</t>
@@ -70,7 +70,7 @@
     <t>The gently rolling dunes are gone. Scree clad mountains rise up in their stead. From abyssal floor to mist shrouded peaks they tower. The ground is steep, sharp, and treacherous underfoot. Darkness abounds - the light of the sun veiled by the mountains’ long shadows. Beneath me the earth groans and strains, trembling at the forces at work deep below.</t>
   </si>
   <si>
-    <t>Before coming here I would awaken violently, panting and covered in layer of sweat, white knuckled fists digging bloody nails into my palms. I know this, for I can see the scars in my hands, even if I cannot recall the memories. Instead I wander the hallways of my dreams. The cavernous hall in which I walk broken by monolithic pillar, whos trunks rise unbroken to the ceiling above.</t>
+    <t>Before coming here I would awaken violently, panting and covered in layer of sweat, white knuckled fists digging bloody nails into my palms. I know this, for I can see the scars in my hands, even if I cannot recall the memories. Instead I wander the hallways of my dreams. The cavernous hall in which I walk broken by monolithic pillar, whose trunks rise unbroken to the ceiling above.</t>
   </si>
   <si>
     <t>When last I dreamed I saw a distant figure. I called out, but there was no reply. When I approached, it faded into the darkness, only to reappear further away. At first it vexed me, so I approached slowly, only to find it vanish again. Once more I tried, more carefully still, and this time the figure did not vanish. When at last I came upon it, I found a woman. She was clad in ivory robes, and asleep upon the floor. Suddenly I was overcome with unease, for when I looked upon her face, I realised I knew her.</t>
@@ -100,13 +100,13 @@
     <t>Whilst my vision grows dull, my dreams become more vivid, and with them she becomes more alive. I resent her absence when I wake, I think only of her as I walk through twilight lands, and the desire in my heart grows as weariness sets in. I am unaffected by the sting of injury, or the pang of hunger. I survive only to see the day through, so that I might be with her at its end.</t>
   </si>
   <si>
-    <t>Day and night, hour after hour, ceaseless in their howling do the mountain winds blow. From the throaty gusts across the wide mountain passes, to the shrill cry through narrow crevasses. The call of the mountain lords echo between every stone and every wall. I have not seen but one flower growing upon the mountainside, only poisonous vines and rusted metal. How cruel time is to bring beauty to ruin, whilst leaving evil untouched.</t>
-  </si>
-  <si>
-    <t>Now we spoke more freely, and her words sit firm in my memory. I must know who she is, whether she is a part of my psyche, or just another apparition in this wasted world. I asked her how she knew where we were, how she knew who I was. I asked gently at first, but my curiosity turned to frustration when she would not answer, and as it so easily does, my frustration turned to anger.</t>
-  </si>
-  <si>
-    <t>She turned her face to hide, but I could see the tears upon her cheek. I knew then, that it did not matter who she was. She has not appeared to me to be my guide, to lead me to my fabled destiny, she is here to be a companion, to give me respite when I sleep and something to live for when my will is spent.</t>
+    <t>Day and night, hour after hour, ceaseless in their howling do the mountain winds blow. From the throaty gusts across the wide mountain passes, to the shrill cry through narrow crevasses. The call of the mountain lords echo between every stone and every wall. I cannot see but one flower growing upon the mountainside, only poisonous vines and rusted metal. How cruel time is to bring beauty to ruin whilst leaving evil untouched.</t>
+  </si>
+  <si>
+    <t>Now we speak more freely, and her words remain in my memory even after I wake. I must know who she is, whether she is a part of my psyche, or just another apparition in this wasted world. I ask her how she knows where we are, how she knows who I am. I ask gently at first, but my curiosity turns to frustration when she will not answer, and as it so easily does, my frustration turns to anger.</t>
+  </si>
+  <si>
+    <t>She turns her face to hide, but I can see the tears upon her cheek. I realise now that it does not matter who she is. She has not come to me to be my guide. She is not here to lead me to my fabled destiny. She is here to be with me, to give me respite when I sleep and to give me something to live for when my body is spent.</t>
   </si>
   <si>
     <t>Twilight of the Gods</t>
@@ -124,7 +124,7 @@
     <t>The gate is the only constant on my journey. It stands some twenty metres high, constructed of smooth rock with no visible evidence of tool marks. It is as if there is only one gate, existing simultaneously across the five realms, like a nail hammered into layers of wood, binding the world together at a single point.</t>
   </si>
   <si>
-    <t>Sometimes I hear distant voices, muffled as if speaking from another room. It is as if the walls of the world are thinning, bringing the living and the dead close to each other. Some voices are louder than others, but they go silent as soon as I speak out to them, leaving me in silence once again.</t>
+    <t>Sometimes I hear distant voices, muffled as if speaking from another room. It is as if the walls of the world are thinning, bringing the living and the dead close to each other. Some voices are louder than others, but they go quiet as soon as I speak out to them, leaving me in silence once again.</t>
   </si>
   <si>
     <t>I came across the hull of an ancient boat. Though its mast was broken, and its sail long since carried away by the winds, I could see that it once would have flown across the waves swiftly. The planks of its hull were rotten, and its metal supports warped and rusted, but I could tell that it was once strong and sleek, able to glide atop the water’s surface and weather the heaviest of waves. Even now, shattered, and strewn across the wastes, the beauty of the vessel was clear to me, and I will carry that beauty until the end of my days.</t>
@@ -181,73 +181,76 @@
     <t>Ruins</t>
   </si>
   <si>
-    <t>A terrible sight is before me, a great city in ruins. Buildings that reach far into the heavens above now reduced to skeletons of twisted metal, broken glass buried in the ground below, foundations shattered and exposed. There is no life here, no birdsong on the breeze, nothing in the black pools of water in the roads. The trees here are dead, their brittle roots cling to furious earth.</t>
-  </si>
-  <si>
-    <t>A red glow punches through the darkness. Her eyes stare unblinking at its source, though I cannot make it out in the gloom. “Go” she says. So I do, cradling her light frame in my arms as we walk towards the light. A fountain, made of black stone, containing a pool of glowing red liquid. “Drink” she said, touching her lips gently. I hesitate, then gently lower her to the pool so that she could drink. Just as the liquid touched her lips she fell unconscious, she slipped from my hands, and fell to the floor. The liquid pooled around her chest, and her breathing ceased.</t>
-  </si>
-  <si>
-    <t>She lay unmoving upon the floor. I tried all I could to bring her back. Then, just as I had given up hope, she jerked awake, spitting the red liquid upon herself. Before I had a chance to say anything, she pointed to the fountain, and to her lips. I shook my head, feeling the tears rolling down my cheeks. Again she pointed to her lips. So again I took her to drink from the fountain. This time I caught her as she went limp, and again I waited for her to wake.</t>
+    <t>A terrible sight is before me: a great city in ruins. Buildings that once reached far into the heavens above now reduced to skeletons of twisted metal, their foundations shattered and exposed. There is no life here- no birdsong on the breeze, only the hollow wail of the wind.</t>
+  </si>
+  <si>
+    <t>A red glow punches through the darkness. Her eyes stare unblinking at its source, though I cannot make it out in the gloom. “Go” she says. So I do, cradling her light frame in my arms. As we approach I see a fountain made of black stone, and in it a pool of glowing red liquid. “Drink” she says, touching her lips gently. I hesitate before lowering her to the pool to drink. The moment the liquid touches her lips she falls limp. Her body slips from my hands to the marble floor. She takes two haggard breaths interspersed with bloody coughs. Then she grows still and will not wake.</t>
+  </si>
+  <si>
+    <t>She lies unmoving on the floor. I try all I can to bring her back to life. Just as I feel hope slipping away she jerks awake, eyes wide, spitting red and black liquid upon herself. Before I have a chance to say anything, she points to the fountain, and to her lips, and again she says “Drink”. I shake my head, feeling the tears rolling down my cheeks. Again she points to her lips. I hang my head in despair, but I know it is what she needs.</t>
   </si>
   <si>
     <t>She is silent now, her eyes will not open, she does not move. I would think her dead if it were not for the shallow breathing of her chest. The fervour of past dreams is gone, replaced instead by anxious waiting. I stand in the endless marble room, unable to do anything but watch her rest.</t>
   </si>
   <si>
-    <t>Time passes imperceptibly slowly, and I cannot take my eyes from her. Truly this is hell, to watch, and wait, and not know what to do, until the hours of your life have wasted away. I wake slowly now, gazing at the sky and unable to rise. My body has betrayed me, muscles tug feebly at aching tendons. I fear I am losing myself to this world, and to her.</t>
-  </si>
-  <si>
-    <t>Waiting, watching, pacing to and fro. Stuck in my dream prison, unable to help the one I love. Forced to watch her pale skin shiver. I can only watch when the spasms strike, her grey face contorted with pain. Yet still she remains asleep. Her eyes will not open. I speak to her as much as I can, but there are times when I cannot muster any words worth saying. Instead I brush her pale hair from her face, and I hold her cold hands in my lap. And despite everything I know, everything I have done, and everything I have seen, I pray for it to be over.</t>
-  </si>
-  <si>
-    <t>This has happened before, in another world. The painful wait for remission, and the fear of relapse. Why is my mind making me relive it? Could it be a warning I wonder, a warning to make haste to finish my quest. Or it could just be fever dreams, brought on by the gradual onset of the essence’s affliction.</t>
-  </si>
-  <si>
-    <t>I will never forget the pain on her face as she drank, or the pain I felt as I held her, thinking she would never wake again. Eventually she roused from her death sleep. She was calm again, the mania driven from her eyes. She lifted my hand to mine, and kissed my cheek. I carried her away from the vile fountain, and as I did the light began to return.</t>
-  </si>
-  <si>
-    <t>Finally things seem to have changed for the better. A warm glow replaces ghostly pallor. Her eyes bright once again, and her smile broad. I rejoiced, and said I thought she was lost. “I’m sorry” she said. I told her not to be sorry, that she could not hold herself to blame. I told her of the things I had remembered since we last spoke- happy memories, places I had been. She nodded as if she recalled them too.</t>
-  </si>
-  <si>
-    <t>How long has it been since the guards abandoned their posts. Was it the firey bellow of cannons that brought down the city walls or the inescapable force of time? Through it all The Necromancer has haunted the world. She seen sickness take hold of her world without the respite of recovery.</t>
-  </si>
-  <si>
-    <t>Fierce have been the ravages of time upon this ancient city. Even now there remain signs of plight- dark craters, munition cases- rusted and spent, and the twisted carcasses of war machines, now long dead. But there are no bones, no bodies, no graves, no markers of human inhabitation to speak of.</t>
-  </si>
-  <si>
-    <t>Today the angel came to me. At first I thought it a dream, that I had been struck unconscious in my journey. No, she was there, a vision still, but one that stood with me in the waking world. She looked better, her features full and no longer sunken, and her smile had returned. She was not near enough to speak, so I waved. For a moment I thought she could not see me, but then she waved back. Then as suddenly as it had begun, the vision ended.</t>
-  </si>
-  <si>
-    <t>Everything that once lived here has been swept away. It is good the Necromancer is not with me. If she were to lay her eyes upon the ruin that has come to this place she would fall to her knees and weep. Perhaps that is why she whispers to me from the darkness - to shield herself from reality, to allow herself to have hope in a place where hope dies.</t>
-  </si>
-  <si>
-    <t>I cannot imagine the things The Necromancer has had to endure. Sometimes I think my burden insignificant compared to hers -  after all what is one life against hundreds? No, that is not fair. I shall not trivialise my own grief, they cannot be compared. The more I stay here, the more I see what has been lost. When this is all over I will return to help her, if I can.</t>
-  </si>
-  <si>
-    <t>The pain inside grows unbearable, the shadow grows and presses against my skull. I feel my breathing become shallow and my heart rise into my throat. Panic, my vision tunnels, and I collapse to the floor. Then before me I see her, my angel, her hand upon my forehead. Memories explode within me, I see her pale face, flowers, white sheets. “Breathe” she says. I close my eyes and breath deep, and slowly the dark thoughts fade away.</t>
-  </si>
-  <si>
-    <t>I do not think I could bear to watch my world fall away before me, to watch as the places and people I knew wither and age and eventually die. To have no one to speak to about such things, and be left with only my unquietable thoughts for company, reliving my past again and again. I would watch myself, and wish that I could change the mistakes I had once made, that I could go back and right the wrongs with those who are no longer with me.</t>
-  </si>
-  <si>
-    <t>Another vision. I saw her from the corner of my eye, she sat at the top of some steps. When I reached her I found her looking at the base of a broken statue. Atop the statues head was a crown, and in his arms a bouquet of flowers. Clearly this man was once well loved by his people. She pointed at the inscription at its base, but it was illegible, the raised stone letters worn away by the wind. None would ever know his name.</t>
-  </si>
-  <si>
-    <t>I remember a story I heard once, a long time ago. An old man lives in a rickety house. One day a child throws a rock at his window and it shatters. He cries, for he has not the strength to repair it, nor the money to pay another. But he moves on, after all, he has lived through worse. The wind blows through the hole, knocking over his belongings and making an awful din. Rain too comes through the broken window, and ruins his floor. Soon enough the season grows cold, and the snow builds up. But now the window cannot be repaired - the frame is too warped. And so sleeps in the deepening cold, until one day he does not wake up.</t>
-  </si>
-  <si>
-    <t>Time heals all, and we can look back with fondness, not regret. We can find new love, love that does not replace the old but allows us to go on, and with it we may remember the old love without sadness. That is what I wish for The Necromancer, that she may find solace in a new world when our quest is over, and not pine for the old.</t>
+    <t>Time passes imperceptibly slowly, and I cannot take my eyes from her. Truly this is hell, to watch and not know what to do but wait. Wait until the hours of my life are spent. I wake slowly now, gazing at the sky and unable to rise. My body betrays me. Muscles tug feebly at aching tendons. I fear I am losing myself to this world, and to her.</t>
+  </si>
+  <si>
+    <t>Waiting, watching, pacing to and fro. Every night stuck in my dream prison. Forced to watch her pale skin shiver. I can only watch when the spasms strike- the pain contorting her grey face. Yet still she sleeps. I talk to her when I can, but often I cannot find words worth saying. Instead I brush her pale hair and hold her cold hands in my lap. And despite everything I know, everything I have done, and everything I have seen, I pray for it to be over.</t>
+  </si>
+  <si>
+    <t>Why do I feel as though this has happened before, in another world. The painful wait for remission, and the fear of relapse. Is my mind playing tricks on me, or is this a part of the despair that has been hidden from me? Could it be a warning I wonder- to make haste to finish my quest. Or is just a fever dream brought on by the gradual onset of the essence’s affliction.</t>
+  </si>
+  <si>
+    <t>I will never forget the pain on her face as she drank, or the pain I felt as I held her, thinking she would never wake. But wake she did, rousing slowly from her death sleep. She looked well once again, her skin warm and the mania driven from her eyes. She lifted her hand to mine, and kissed my cheek. I carried her away from the vile fountain, and as I did the light began to return.</t>
+  </si>
+  <si>
+    <t>Finally things seem to have changed for the better. A warm glow replaces ghostly pallor and her eyes bright once again. I rejoice, and tell her I believed she was lost. “I’m sorry” she says. But I tell her not to be sorry, that she cannot hold herself to blame. I tell her of the things I had remembered since we last spoke- happy memories, places I had been. She nods and listens, though her thoughts seem far away.</t>
+  </si>
+  <si>
+    <t>The city is ancient. How ancient I wonder? How long since the guards abandoned their posts. Was it the fire-laced breath of artillery that brought down the city’s walls or merely the inescapable erosion of time? Through it all The Necromancer has haunted the world, or so she says. She watched the essence dig take ahold of her world, and not once has she seen its grip weaken.</t>
+  </si>
+  <si>
+    <t>Fierce have been the ravages of time upon this ancient city. Even now there remain signs of plight- dark craters, munition cases- tarnished and spent. Even the rusted carcasses of war machines litter the land. But there are no bones, no bodies, no graves, no markers of human inhabitation to speak of.</t>
+  </si>
+  <si>
+    <t>At first I thought I was dreaming, but no, there she is, standing before me. A vision, but still with me here in the waking world. She looks better, her features full and no longer sunken, and her smile has returned. She is not near enough to hear me call out, so I wave to her instead. For a moment it seems as though she cannot see me, but she waves back. Then as suddenly as it began, the vision ends.</t>
+  </si>
+  <si>
+    <t>The old world has been swept away. It is good the Necromancer cannot be with me to see it. If she were to lay her eyes upon the ruins she surely would fall to her knees and weep. Perhaps that is why she whispers to me from the darkness - to shield herself from reality, to allow herself to have hope in a place where none can be found.</t>
+  </si>
+  <si>
+    <t>I cannot imagine the things The Necromancer has had to endure. Sometimes I think my burden insignificant compared to hers. After all what is the worth of one life against that of an entire civilisation? But we all have our own cross to bear. The more I stay here, the more I see what has been lost. When this is all over I will return to help her, if I can.</t>
+  </si>
+  <si>
+    <t>The shadow within grows, pressing against my skull. I feel despair well up uncontrollably. My breathing comes shallow and my heart rises into my throat. Panic. My vision tunnels and I collapse to the floor. Then before me I see her, my angel, her cool hand upon my forehead. Memories explode within me, I see her pale face, flowers, white sheets, blood. “Breathe” she says. I close my eyes and breath deep- once, twice, feeling the despair dissipate. Then I open them only to find her gone.</t>
+  </si>
+  <si>
+    <t>I do not think I could bear to watch as the places I know fall into disrepair and the people I love age and die. I could not bear to be alone to be without someone to ease my pain. Left with only my unquietable thoughts for company, reliving my lost past over and over. I would watch my past self and wish that I could change the things that can never be changed. And I would wish to go back and spend one last moment with those who are gone.</t>
+  </si>
+  <si>
+    <t>Another vision. I can see her in the corner of my eye. She sits at the top of a tall set of steps. As I reach the top I realise she is not looking at me, but at the base of a broken statue. Atop the statues’ weathered head is a crown- tarnished but still golden. This man, a king, was once well loved by his people. So loved that even today it remained untouched by scavengers. She points at the inscription at its base but I cannot make out the words. The raised stone letters have been worn away by the wind. I will never know his name.</t>
+  </si>
+  <si>
+    <t>I remember a story I heard once, about an old man. He lived alone in an old cottage. Like him the building had not aged well, its walls were cracked and the roof fallen in. He was bitter, and set in his ways, and went out only to buy from the local village what he could not make himself. He had not always been bitter, he had not always been alone. One day there were children playing outside his window. He ignored them as best he could, but an errant ball missed its mark and came through his window with a crash. So he yelled at the children, and drove them back to the village. When he returned he cleared up the pieces of shattered glass, but could not repair the window. He did not want to return to the village, and so he left it- a gaping void in the side of his house.</t>
+  </si>
+  <si>
+    <t>Time passed, and still the window remained broken. The old man could not repair it himself, and did not have the money to pay to have it mended. So the thought of it drifted from his mind, at least until Autumn came. Strong winds rocked the aged house whilst lashes of rain made their way in through the open window. Day after day it came through until not an inch of the house remained dry. But the old man ignored it- after all, he had endured worse.</t>
+  </si>
+  <si>
+    <t>Then the cold weather came, bringing snow and frost and ice. The old man huddled for warmth in his broken home, his fire dwindling and his supplies low. Finally he relented, and went to the village to beg to have the window repaired. But it was too late, nobody had the tools to fix the window, as broken and warped as it was. They offered him shelter, but his pride took him back home. So there he slept, in the cold and the light of the dying fires, waiting for Spring to come. But there would be no Spring for him, only a deep sleep and a white light, followed by oblivion.</t>
   </si>
   <si>
     <t>I saw her once again. She sat outside a ruined building reclining on a small drift of sand. So I sat with her, and I asked her how she had escaped her dream prison, but she only gave me a knowing smile and changed the conversation. I do not belong to this world, yet I am growing comfortable here. I am afraid that if I leave I will lose her.</t>
   </si>
   <si>
-    <t>I asked her what would become of her when I return home, but she only smiled and held her fingers to her lips. I will not ask again. I told her I could not lose her, that she must stay, but as soon as I finished speaking I was struck by a flash of painful memories. I awoke with a jolt, confused by the bitter-sweet dream. It is not long until the journey is over.</t>
-  </si>
-  <si>
-    <t>I have tried to listen, truly, I have. Still I cannot hear the gods, only the whisper of sand and the howl of wind. I want to hear them, even for a moment, to know they are there. Maybe The Necromancer, with her mystic ways, can hear what I cannot. The world does not feel any different to me.</t>
-  </si>
-  <si>
-    <t>Do you see it when you sleep? Can you hear it in silent places? Do you catch glimpses of it when you blink, as if engraved on the lids of your eyes? It is there, everywhere, in all places, and in all times. Do you not know of what I speak? It is the cold in the pit of your stomach at night, the black thoughts when you are alone. It is the dread, the terrible thought that things will not always be. It is the fear that gives life brilliance. I feel it always, with every waking moment and every darkened sleep. I know you feel it too, we all do.</t>
+    <t>I dream. I ask her where she will go when I return home, but she only smiles and holds her fingers to her lips. I do not pursue the question. I begin to tell her I do not want to lose her, that she must stay with me, but as the words start to leave my mouth I am struck by a flash of painful memories. I awake with a jolt, confused by the bitter-sweet dream. It will not be long before the journey is over.</t>
+  </si>
+  <si>
+    <t>I turn my ear to the wind and I listen for the gods. I cry out for them, but the only response I find is in the whisper of the sand. I want to hear them, even for a moment, to know they are there. Maybe The Necromancer with her mystic ways is able to hear what I cannot. The world does not feel any different to me.</t>
+  </si>
+  <si>
+    <t>I see it in my sleep. I hear it in silent places. I even catch glimpses of it when I speak. The darkness, the despair, the weight that lies inside. It is the cold in the pit in my stomach at night, the bleak thoughts when I am alone. The dread thought waxes- the terrible thought that things will not always be. It is the human fear that gives life brilliance. I realise now I have always felt it, but only now that I face the consequence of the fear do I recognise it.</t>
   </si>
   <si>
     <t>The End of All Things</t>
@@ -298,22 +301,22 @@
     <t>Main Story</t>
   </si>
   <si>
-    <t>You wept. Alone, and in darkness. I watched you across the great cold distance and in you I saw myself. I have brought you here, to my world, so that we might both be saved. We both can look upon these desolate plains with unfamiliar gaze. But this was once my home. Long before the darkness fell these lands were green. I would walk amongst the trees with feel the grass beneath my feet. Now the groves are dead, and I pass like a shadow among them. Only the sun-scorched dirt remains.</t>
+    <t>You wept. Alone, and in darkness. I watched you across the great cold distance and in you I saw myself. I have brought you here, to my world, so that we might both be saved. We both can look upon these desolate plains with unfamiliar gaze. But this was once my home. Long before the darkness fell these lands were green. I would walk amongst the trees and feel the grass beneath my feet. Now the groves are dead, and I pass like a shadow among them. Only the sun-scorched dirt remains.</t>
   </si>
   <si>
     <t>There were once five gods who roamed the world. Around them five great kingdoms were founded. Our civilisations grew with time. Miracles became rote; our cities rose high into the heavens and our machines worked the earth. The gods saw they were no longer needed, and so they retreated from the world of man. One day, when we had all but forgotten our roots, they vanished. But the vacuum left by their absence was clear. Something changed, in the air, the earth, and the sea. The essence that binds the world turned on us. It soured the earth and awoke ceaseless winds. The gods are gone, and with them, our humanity.</t>
   </si>
   <si>
-    <t>Ahead lies a dead world- a stagnant place where only barbarism and hopelessness remain. But I believe if we can bring back the gods we can restore it all. I know where they are. They sleep in the place between places, the dark realm beyond the veil of reality. There are five gates that lead to this realm, but they lie dormant, bound by seals set in eons past. I cannot break them, but I can guide you. Only together can the gods turn the tide of decay, and offer you the peace which you so dearly seek.</t>
-  </si>
-  <si>
-    <t>Your path is not an easy one, there will be dangers, both physical and psychological. The essence will seek to claim you. It will burrow into your thoughts and lay seeds of doubt. It once gave strength to the gods, now unbound it breeds only chaos.It feeds on our wants and fear. All you will encounter have succumbed to its influence. Some may still resist. Others, however, will stop at nothing to rid you from the world.</t>
+    <t>Ahead lies a dead world- a stagnant place where only barbarism and hopelessness remain. But I believe if we can bring back the gods we can restore it all. I know where they are. They sleep in the place between places, the dark realm beyond the veil of reality. There are five gates that lead to this realm, but they lie dormant, activated by temples long since fallen to the essence. I cannot cleanse the temples, but I can guide you to them. Only together can the gods turn the tide of decay, and offer you the peace which you so dearly seek.</t>
+  </si>
+  <si>
+    <t>Your path is not an easy one, there will be dangers, both physical and psychological. The essence will seek to claim you. It will burrow into your thoughts and lay seeds of doubt. It once gave strength to the gods, now unbound it breeds only chaos. It feeds on our wants and fear. All you will encounter have succumbed to its influence. Some may still resist. Others, however, will stop at nothing to rid you from the world.</t>
   </si>
   <si>
     <t>You were lost, but I found you. Your memories have been hidden, for now, at least, but I cannot hide your pain. That you will have to bear. When you are ready I will tell you more. Until then you must endure. Trust in my words, I do not wish to deceive you. The gods can heal your grief, just as they can heal my world.</t>
   </si>
   <si>
-    <t>I have brought you to the kingdom of Eo. Only one seal binds the gateway, and it lies hidden amongst the shifting desert sands. When it is broken return here and place your hands upon the stones. Be prepared, for I do not know what awaits you within. I will be waiting for you on the other side, no matter what happens.</t>
+    <t>I have brought you to the kingdom of Eo. Only one temple binds the gateway, and it lies hidden amongst the shifting desert sands. When it is broken return here and place your hands upon the stones. Be prepared, for I do not know what awaits you within. I will be waiting for you on the other side, no matter what happens.</t>
   </si>
   <si>
     <t>So it is done, you have passed through the gate and the realm between the shadows. You have done wonderfully. Already I hear Eo’s voice on the wind - calling for her lost siblings. How must it feel, to awaken from one nightmare into another, to see your beautiful world in ruins. I was there whilst it happened - I watched the life of the earth fade away. But I was cursed to remain as everything I loved turned to dust. I saw my friends and my family die, as I was doomed to solitude by immortality. I do not feel pity for the dead, wanderer, for it is the living alone who are left who grieve.</t>
@@ -325,7 +328,7 @@
     <t>This was my home before I became The Necromancer. When I was a child the sun rose high above the horizon and the sky was still blue. I was there when the gates were built. I watched as the sands encroach upon our kingdoms, and with them our ties to our brothers and sisters disappear on the desert winds. I remember when the last flowers faded. I remember when the rivers dried up. I remember the day when the brave lost their voice, and the braying of animals was replaced by screams of the dying. I have kept my faith all these years, believing that I would find someone like you to save us. Long have I waited here, Wanderer, but I knew that you would come.</t>
   </si>
   <si>
-    <t>Again and again I see your fate repeated in my dreams. I watch as the final seal is broken, and the last gate illuminated with life. Time and time again the gods reverse the wheel of time and raise our cities up from the dust. It has been prophesied, and so it will be. Go now, into the mountains where the cold winds blow and the sun dare not dwell. Find the one who sleeps and return her to us.</t>
+    <t>Again and again I see your fate repeated in my dreams. I watch as the final temple is cleansed, and the last gate illuminated with life. Time and time again I see the gods reverse the wheel of time and raise our cities up from the dust. It has been prophesied, and so it will be. Go now, into the mountains where the cold winds blow and the sun dare not dwell. Find the one who sleeps and return her to us.</t>
   </si>
   <si>
     <t>I can sense the question in your heart- who is the woman who you dream of? Yes, I have seen your dreams, and I know the dread that grows in your heart. She is your wife, Wanderer, and she is dying. I did not want to tell you before, for I thought that the knowledge would be too much for you to bear. I see now I was wrong, you are stronger than I ever could have thought. There is still time to save her, but you must be fast.</t>
@@ -352,28 +355,28 @@
     <t>We are nearing the end. I feel the air changing as you advance. It is lighter, as if a weight were lifting. Even the sun seems brighter to my eyes. Soon I will be able to show you the wonders of this world. When the gods return we will walk the ground together. I will give you the life you desire, and you will take my hand as we watch an ancient dawn become new once more. We are so close to the end, Wanderer. The next gate will take you to the ruins of our greatest city, where the lingering ghosts of the dead cry out for life.</t>
   </si>
   <si>
-    <t>The winds are changing, old currents blow once more, interrupting the monotonous cycle that has gone on for too long. The gods are waking, their spirits waking the world from it’s terminal sleep. The essence grows agitated, pulling at invisible threads in the air. It resists their control, for now, but when Corypthos awakens it will relent- bound once more. The deserts will retreat, pushed back by the tide of life that yearns to spill across the barren earth.</t>
+    <t>The winds are changing, old currents blow once more, interrupting the monotonous cycle that has gone on for too long. The gods are waking, their spirits waking the world from its terminal sleep. The essence grows agitated, pulling at invisible threads in the air. It resists their control, for now, but when Corypthos awakens it will relent- bound once more. The deserts will retreat, pushed back by the tide of life that yearns to spill across the barren earth.</t>
   </si>
   <si>
     <t>Our struggle is almost at an end, Wanderer. I see the trauma in your eyes grow with every moment that passes. You are remembering what it was you left behind, that I rescued you from. Yes, what you fear to be real is indeed so. Corpythos, lord of life, awaits you in the Wasteland. He can bring her back, Wanderer. So too can he free me, return me my body so that I may walk among the trees once again. And my people, he will return them too, oh how soon it will be. Oh, I am sorry, I cannot hide my elation. I know you suffer, but you cannot know how I have suffered, and how soon that suffering will come to an end. When it is done, when duty fulfilled and my vigil over, I will return home, and I will sit as my father sat, and I will watch the sun set as it did so many years ago.</t>
   </si>
   <si>
-    <t>I cannot tell you how it feels to know salvation will soon be at hand. We will be able to return to how we once were, and raise our civilisation to even greater heights.</t>
-  </si>
-  <si>
     <t>End</t>
   </si>
   <si>
-    <t>It happened slowly at first, the suns swelled and grew brighter. The air grew still around us, and all noise faded away to nothing. Suddenly the light enveloped me, and a crack like thunder signalled the end of the silence. I held my breath and shut my eyes against the glare. It was as if the whole world was collapsing around me. I could hear the Necromancer’s cries amidst a cacophony of quaking earth and screaming winds. The fifth tomb was empty. The five gods are were no more, and the long owed doom of the earth has finally come.</t>
-  </si>
-  <si>
-    <t>Then the light was replaced with darkness, and the noise with peace. I was in another world, my own world, staring up at a brilliant blue sky from a floor of soft grass. Memories once cloudy and vague returned with perfect clarity, but there was one that stood out in my mind. It was the memory of her, the woman with grey speckled eyes. I remembered her final moments, lying in a bed of soft white sheets. So weak she could not lift her hand to hold mine, so I held hers. I remember as she told me she was sorry that she had to leave me. I told her there was nothing to forgive. Instead I told her I was sorry that I could not go with her, and that she would always be with me. I told her of all the memories we shared, and that I now bear alone. Later, as the light from the sun began to wane, that her soft laughter at my stories grew silent. And then I knew that she had died, and I was alone.</t>
-  </si>
-  <si>
-    <t>It was then that I saw her in my mind, as young and beautiful as she was on the day we first met.</t>
-  </si>
-  <si>
-    <t>But these are just memories.</t>
+    <t>It happens slowly at first. The suns swell and grow bright. The air turns still and the noises of the earth and of battle fade away. Light envelops me, signaled by a peal of thunder so loud as to shake the foundations of heaven. I hold my breath in the bright void and shut my eyes against the glare. In the distance I can hear the Necromancer’s cries. She is weeping, screaming, in sadness and in pain, but that too diminishes until I am left in utter silence.</t>
+  </si>
+  <si>
+    <t>It was never to be. The Necromancer’s world could never be saved. The fifth tomb is empty, abandoned years ago. The gods are no more, and now the long awaited doom of her world has finally come. I feel my fate coalescing as the memories return. They are painful, breaching the surface of consciousness all at once. Among them is her face, eyes closed and silent.</t>
+  </si>
+  <si>
+    <t>Then I am in another world. My own world. I look up at a brilliant blue sky illuminated by the light of a single white star. Another change, and I am in a starkly white room. The only door into the room is shut, the walls reflect on the marble floor below. And then I see her, lying in a raised bed, wrapped in ivory sheets.</t>
+  </si>
+  <si>
+    <t>I take her hand, hesitantly at first. As our hands touch the physical memory of her returns, and I take her up in my arms. She tells me she is sorry that she has to go. She chokes on the words as she tells me she does not want to leave me alone. I tell her there is nothing to forgive. I say I am sorry I cannot go with her, but that I would carry her forever with me.</t>
+  </si>
+  <si>
+    <t>We brush away our tears and turn our talk to old times- our children and the places we have been. As the day turns to night she becomes ever quieter, so I draw her close and take up the conversation. Later, as the light of the sun breaks the horizon, her soft laughter at my stories grows silent. I knew then that she was gone, and that I was alone.|br||br|I still see her in my mind- as young and beautiful as she was on the day we first met.|br||br|But the memories will fade with me, and all will be borne away on the wind.</t>
   </si>
   <si>
     <t>Character Stories</t>
@@ -678,10 +681,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -720,7 +723,60 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -735,10 +791,31 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -749,9 +826,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -765,50 +842,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -820,44 +858,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -872,13 +875,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -896,19 +935,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -920,7 +959,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -932,79 +989,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1016,13 +1001,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1040,7 +1025,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1056,6 +1041,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -1066,11 +1069,59 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1090,41 +1141,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1143,32 +1166,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1186,134 +1189,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1333,6 +1336,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1657,10 +1663,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AA85"/>
+  <dimension ref="A1:AA86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="U68" sqref="U68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>
@@ -2997,195 +3003,209 @@
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="2" t="s">
+      <c r="A70" t="s">
+        <v>52</v>
+      </c>
+      <c r="B70" t="s">
+        <v>53</v>
+      </c>
+      <c r="C70" s="2">
+        <v>24</v>
+      </c>
+      <c r="D70" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="B70" t="s">
-        <v>78</v>
-      </c>
-      <c r="C70" s="2">
-        <v>1</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B71" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C71" s="2">
-        <v>2</v>
-      </c>
-      <c r="D71" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C72" s="2">
-        <v>3</v>
-      </c>
-      <c r="D72" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B73" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C73" s="2">
-        <v>4</v>
-      </c>
-      <c r="D73" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D73" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B74" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C74" s="2">
-        <v>5</v>
-      </c>
-      <c r="D74" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C75" s="2">
-        <v>6</v>
-      </c>
-      <c r="D75" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="8" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C76" s="2">
-        <v>7</v>
-      </c>
-      <c r="D76" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" s="8" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C77" s="2">
-        <v>8</v>
-      </c>
-      <c r="D77" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C78" s="2">
-        <v>9</v>
-      </c>
-      <c r="D78" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" s="8" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C79" s="2">
-        <v>10</v>
-      </c>
-      <c r="D79" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C80" s="2">
-        <v>11</v>
-      </c>
-      <c r="D80" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D80" s="8" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B81" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C81" s="2">
-        <v>12</v>
-      </c>
-      <c r="D81" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D81" s="8" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B82" t="s">
+        <v>79</v>
+      </c>
+      <c r="C82" s="2">
+        <v>12</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C82" s="2">
+      <c r="B83" t="s">
+        <v>79</v>
+      </c>
+      <c r="C83" s="2">
         <v>13</v>
       </c>
-      <c r="D82" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2">
-      <c r="B83"/>
+      <c r="D83" s="8" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="84" spans="2:2">
       <c r="B84"/>
     </row>
     <row r="85" spans="2:2">
       <c r="B85"/>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -3196,10 +3216,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AB55"/>
+  <dimension ref="A1:AB54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W48" sqref="W48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -3210,7 +3230,7 @@
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="4"/>
@@ -3227,8 +3247,8 @@
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>93</v>
+      <c r="C2" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
@@ -3243,8 +3263,8 @@
       <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>94</v>
+      <c r="C3" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
@@ -3259,8 +3279,8 @@
       <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>95</v>
+      <c r="C4" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
@@ -3275,8 +3295,8 @@
       <c r="B5" s="4">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>96</v>
+      <c r="C5" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
@@ -3291,8 +3311,8 @@
       <c r="B6" s="4">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>97</v>
+      <c r="C6" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
@@ -3307,8 +3327,8 @@
       <c r="B7" s="4">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>98</v>
+      <c r="C7" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
@@ -3323,8 +3343,8 @@
       <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>99</v>
+      <c r="C8" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
@@ -3339,8 +3359,8 @@
       <c r="B9" s="4">
         <v>2</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>100</v>
+      <c r="C9" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
@@ -3355,8 +3375,8 @@
       <c r="B10" s="4">
         <v>3</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>101</v>
+      <c r="C10" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
@@ -3371,8 +3391,8 @@
       <c r="B11" s="4">
         <v>4</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>102</v>
+      <c r="C11" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
@@ -3387,8 +3407,8 @@
       <c r="B12" s="5">
         <v>1</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>103</v>
+      <c r="C12" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
@@ -3403,8 +3423,8 @@
       <c r="B13" s="5">
         <v>2</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>104</v>
+      <c r="C13" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
@@ -3419,8 +3439,8 @@
       <c r="B14" s="5">
         <v>3</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>105</v>
+      <c r="C14" s="7" t="s">
+        <v>106</v>
       </c>
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
@@ -3435,8 +3455,8 @@
       <c r="B15" s="5">
         <v>4</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>106</v>
+      <c r="C15" s="7" t="s">
+        <v>107</v>
       </c>
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
@@ -3451,8 +3471,8 @@
       <c r="B16" s="5">
         <v>1</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>107</v>
+      <c r="C16" s="7" t="s">
+        <v>108</v>
       </c>
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
@@ -3467,8 +3487,8 @@
       <c r="B17" s="5">
         <v>2</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>108</v>
+      <c r="C17" s="7" t="s">
+        <v>109</v>
       </c>
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
@@ -3483,8 +3503,8 @@
       <c r="B18" s="5">
         <v>3</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>109</v>
+      <c r="C18" s="7" t="s">
+        <v>110</v>
       </c>
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
@@ -3499,8 +3519,8 @@
       <c r="B19" s="5">
         <v>4</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>110</v>
+      <c r="C19" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
@@ -3510,13 +3530,13 @@
     </row>
     <row r="20" spans="1:28">
       <c r="A20" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>111</v>
+      <c r="C20" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
@@ -3526,13 +3546,13 @@
     </row>
     <row r="21" spans="1:28">
       <c r="A21" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B21" s="5">
         <v>2</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>112</v>
+      <c r="C21" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
@@ -3542,13 +3562,13 @@
     </row>
     <row r="22" spans="1:28">
       <c r="A22" s="5" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="B22" s="5">
-        <v>3</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>113</v>
+        <v>1</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="X22" s="4"/>
       <c r="Y22" s="4"/>
@@ -3561,10 +3581,10 @@
         <v>114</v>
       </c>
       <c r="B23" s="5">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>115</v>
+        <v>2</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>116</v>
       </c>
       <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
@@ -3577,10 +3597,10 @@
         <v>114</v>
       </c>
       <c r="B24" s="5">
-        <v>2</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>116</v>
+        <v>3</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="X24" s="4"/>
       <c r="Y24" s="4"/>
@@ -3593,10 +3613,10 @@
         <v>114</v>
       </c>
       <c r="B25" s="5">
-        <v>3</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>117</v>
+        <v>4</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>118</v>
       </c>
       <c r="X25" s="4"/>
       <c r="Y25" s="4"/>
@@ -3609,10 +3629,10 @@
         <v>114</v>
       </c>
       <c r="B26" s="5">
-        <v>4</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>118</v>
+        <v>5</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
@@ -3620,23 +3640,46 @@
       <c r="AA26" s="4"/>
       <c r="AB26" s="4"/>
     </row>
-    <row r="27" spans="24:28">
+    <row r="27" spans="3:28">
+      <c r="C27"/>
       <c r="X27" s="4"/>
       <c r="Y27" s="4"/>
       <c r="Z27" s="4"/>
       <c r="AA27" s="4"/>
       <c r="AB27" s="4"/>
     </row>
-    <row r="28" spans="24:28">
-      <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
-      <c r="Z28" s="4"/>
-      <c r="AA28" s="4"/>
-      <c r="AB28" s="4"/>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
+    <row r="28" spans="1:3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="7"/>
+    </row>
+    <row r="29" spans="3:28">
+      <c r="C29" s="7"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4"/>
     </row>
     <row r="30" spans="4:28">
       <c r="D30" s="4"/>
@@ -3773,32 +3816,18 @@
       <c r="AA34" s="4"/>
       <c r="AB34" s="4"/>
     </row>
-    <row r="35" spans="4:28">
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
-      <c r="Y35" s="4"/>
-      <c r="Z35" s="4"/>
-      <c r="AA35" s="4"/>
-      <c r="AB35" s="4"/>
+    <row r="36" spans="18:28">
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+      <c r="W36" s="4"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+      <c r="Z36" s="4"/>
+      <c r="AA36" s="4"/>
+      <c r="AB36" s="4"/>
     </row>
     <row r="37" spans="18:28">
       <c r="R37" s="4"/>
@@ -4033,19 +4062,6 @@
       <c r="Z54" s="4"/>
       <c r="AA54" s="4"/>
       <c r="AB54" s="4"/>
-    </row>
-    <row r="55" spans="18:28">
-      <c r="R55" s="4"/>
-      <c r="S55" s="4"/>
-      <c r="T55" s="4"/>
-      <c r="U55" s="4"/>
-      <c r="V55" s="4"/>
-      <c r="W55" s="4"/>
-      <c r="X55" s="4"/>
-      <c r="Y55" s="4"/>
-      <c r="Z55" s="4"/>
-      <c r="AA55" s="4"/>
-      <c r="AB55" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -4069,7 +4085,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -4089,16 +4105,16 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -4115,16 +4131,16 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -4141,16 +4157,16 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -4167,16 +4183,16 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -4193,16 +4209,16 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -4219,16 +4235,16 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -4245,16 +4261,16 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -4271,16 +4287,16 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C9" s="2">
         <v>3</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -4297,16 +4313,16 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -4323,16 +4339,16 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -4349,16 +4365,16 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C12" s="2">
         <v>3</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -4375,16 +4391,16 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C13" s="2">
         <v>4</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -4401,16 +4417,16 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -4427,16 +4443,16 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C15" s="2">
         <v>2</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -4453,16 +4469,16 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -4479,16 +4495,16 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C17" s="2">
         <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -4505,16 +4521,16 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C18" s="2">
         <v>3</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -4531,16 +4547,16 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -4554,7 +4570,7 @@
   <sheetPr/>
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
@@ -4567,16 +4583,16 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
@@ -4600,7 +4616,7 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B2" s="2" t="b">
         <v>0</v>
@@ -4609,7 +4625,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="2"/>
@@ -4633,7 +4649,7 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B3" s="2" t="b">
         <v>0</v>
@@ -4642,7 +4658,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="2"/>
@@ -4666,7 +4682,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B4" s="2" t="b">
         <v>0</v>
@@ -4675,7 +4691,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
@@ -4699,7 +4715,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B5" s="2" t="b">
         <v>1</v>
@@ -4708,7 +4724,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="2"/>
@@ -4732,7 +4748,7 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B6" s="2" t="b">
         <v>0</v>
@@ -4741,7 +4757,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="2"/>
@@ -4765,7 +4781,7 @@
     </row>
     <row r="7" spans="1:23">
       <c r="A7" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B7" s="2" t="b">
         <v>0</v>
@@ -4774,7 +4790,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="2"/>
@@ -4798,7 +4814,7 @@
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B8" s="2" t="b">
         <v>0</v>
@@ -4807,7 +4823,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="2"/>
@@ -4831,7 +4847,7 @@
     </row>
     <row r="9" spans="1:23">
       <c r="A9" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B9" s="2" t="b">
         <v>1</v>
@@ -4840,7 +4856,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="2"/>
@@ -4864,7 +4880,7 @@
     </row>
     <row r="10" spans="1:23">
       <c r="A10" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B10" s="2" t="b">
         <v>1</v>
@@ -4873,7 +4889,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="2"/>
@@ -4897,7 +4913,7 @@
     </row>
     <row r="11" spans="1:23">
       <c r="A11" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B11" s="2" t="b">
         <v>1</v>
@@ -4906,7 +4922,7 @@
         <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="2"/>
@@ -4930,7 +4946,7 @@
     </row>
     <row r="12" spans="1:23">
       <c r="A12" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B12" s="2" t="b">
         <v>0</v>
@@ -4939,7 +4955,7 @@
         <v>31</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="2"/>
@@ -4963,7 +4979,7 @@
     </row>
     <row r="13" spans="1:23">
       <c r="A13" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B13" s="2" t="b">
         <v>0</v>
@@ -4972,7 +4988,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="2"/>
@@ -4996,7 +5012,7 @@
     </row>
     <row r="14" spans="1:23">
       <c r="A14" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B14" s="2" t="b">
         <v>0</v>
@@ -5005,7 +5021,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="2"/>
@@ -5029,7 +5045,7 @@
     </row>
     <row r="15" spans="1:23">
       <c r="A15" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B15" s="2" t="b">
         <v>1</v>
@@ -5038,7 +5054,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="2"/>
@@ -5062,7 +5078,7 @@
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B16" s="2" t="b">
         <v>1</v>
@@ -5071,7 +5087,7 @@
         <v>31</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="2"/>
@@ -5095,7 +5111,7 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B17" s="2" t="b">
         <v>1</v>
@@ -5104,7 +5120,7 @@
         <v>31</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="2"/>
@@ -5128,7 +5144,7 @@
     </row>
     <row r="18" spans="1:23">
       <c r="A18" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B18" s="2" t="b">
         <v>1</v>
@@ -5137,7 +5153,7 @@
         <v>31</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="2"/>
@@ -5161,7 +5177,7 @@
     </row>
     <row r="19" spans="1:23">
       <c r="A19" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B19" s="2" t="b">
         <v>0</v>
@@ -5170,7 +5186,7 @@
         <v>53</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="2"/>
@@ -5194,7 +5210,7 @@
     </row>
     <row r="20" spans="1:23">
       <c r="A20" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B20" s="2" t="b">
         <v>0</v>
@@ -5203,7 +5219,7 @@
         <v>53</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="2"/>
@@ -5227,7 +5243,7 @@
     </row>
     <row r="21" spans="1:23">
       <c r="A21" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B21" s="2" t="b">
         <v>0</v>
@@ -5236,7 +5252,7 @@
         <v>53</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="2"/>
@@ -5260,7 +5276,7 @@
     </row>
     <row r="22" spans="1:23">
       <c r="A22" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B22" s="2" t="b">
         <v>1</v>
@@ -5269,7 +5285,7 @@
         <v>53</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="2"/>
@@ -5293,7 +5309,7 @@
     </row>
     <row r="23" spans="1:23">
       <c r="A23" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B23" s="2" t="b">
         <v>1</v>
@@ -5302,7 +5318,7 @@
         <v>53</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="2"/>
@@ -5326,7 +5342,7 @@
     </row>
     <row r="24" spans="1:23">
       <c r="A24" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B24" s="2" t="b">
         <v>1</v>
@@ -5335,7 +5351,7 @@
         <v>53</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="2"/>
@@ -5359,7 +5375,7 @@
     </row>
     <row r="25" spans="1:23">
       <c r="A25" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B25" s="2" t="b">
         <v>1</v>
@@ -5368,7 +5384,7 @@
         <v>53</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="2"/>
@@ -5392,7 +5408,7 @@
     </row>
     <row r="26" spans="1:23">
       <c r="A26" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B26" s="2" t="b">
         <v>1</v>
@@ -5401,7 +5417,7 @@
         <v>53</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="2"/>
@@ -5425,164 +5441,164 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B27" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B28" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B29" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B30" t="b">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B33" t="b">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B34" t="b">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B35" t="b">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B36" t="b">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B38" t="b">
         <v>1</v>
@@ -5591,12 +5607,12 @@
         <v>114</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
@@ -5605,12 +5621,12 @@
         <v>114</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
@@ -5619,7 +5635,7 @@
         <v>114</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
<Bugfix, Story, Import> CSV import, Travel
Fixed special character import issues in csv exporter.
Fixed bug where travelling could get stuck.
Fixed bug where travelling with multiple characters would get stuck.
</commit_message>
<xml_diff>
--- a/Beyond The Veil - Story.xlsx
+++ b/Beyond The Veil - Story.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18620" activeTab="1"/>
+    <workbookView windowHeight="18620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Wanderer" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238">
   <si>
     <t>Wanderer Journal</t>
   </si>
@@ -28,10 +28,10 @@
     <t>Desert</t>
   </si>
   <si>
-    <t>The land before me is just as the Necromancer said- dark and dying. Even the dry ground seems to creak with hunger, eager to slake its thirst with my blood. There are others here. They are vague shapes on the horizon and subtle whispers on the wind. Purgatorial souls -  fearful and wary. If I am to be alone in my journey then that is the way it must be.</t>
-  </si>
-  <si>
-    <t>Sensations come and go, like memories without context. Warm light on my back. The green glow of a sunlit canopy, and dappled colour on the ground where the light breaks through. They match nothing of what I have experienced. Here there are no living trees, no leaf-laden boughs, only dead roots, withered stumps, and the stifling heat.</t>
+    <t>The land before me is just as the Necromancer said- dark and dying. Even the dry ground seems to creak with hunger, eager to slake its thirst with my blood. There are others here. They are vague shapes on the horizon and subtle whispers on the wind. Purgatorial souls - fearful and wary. If I am to be alone in my journey then that is the way it must be.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensations come and go, like memories without context. Warm light on my back. The green glow of a sunlit canopy, and dappled colour on the ground where the light breaks through. They match nothing of what I have experienced. Here there are no living trees, no leaf-laden boughs, only dead roots, withered stumps, and the stifling heat. </t>
   </si>
   <si>
     <t>What was once familiar is now foreign to me - the sky a deep shade of crimson, lit by the weak glow of three ailing suns, and the air heavy with dread expectation. At night the heavens glitter with the light of unknown constellations. I am not sure if I will ever share the Necromancer’s faith, but if the alternative is a life of solitude and fear then I will go wherever she bids.</t>
@@ -46,7 +46,7 @@
     <t>I have slept well here. I have even dreamed- for the first time in a long time. In my dreams I am in a cavernous room. There are no walls. Far above I can see a stone roof, arching away into the blackness beyond. I let myself lie back and drift in silence on the murky currents of my thoughts.</t>
   </si>
   <si>
-    <t>I feel my emotions ebb and flow like the tide, and I allow myself to be borne away on their currents. With every swell come glimpses of my past, clearer now. But as every swell passes, so do these memories fade. I cannot hold onto them in this bleak and desolate world.</t>
+    <t xml:space="preserve">I feel my emotions ebb and flow like the tide, and I allow myself to be borne away on their currents. With every swell come glimpses of my past, clearer now. But as every swell passes, so do these memories fade. I cannot hold onto them in this bleak and desolate world. </t>
   </si>
   <si>
     <t>It was neither chance nor fate that brought me here. The Necromancer was adamant that I was chosen for this task, that I alone am able to find and awaken the gods, but can I believe her? It seems likely that I am just one of many. Doomed to wander, endlessly searching for purpose until the end of my days.</t>
@@ -67,7 +67,7 @@
     <t>Four gates remain, and I am all but spent. To follow the path to open the Gate of Eo has been burdensome enough, but with four more in wait I am not sure if I am able to go on. I feel only dread at the thought journey before me. There is no doubt that greater dangers lie in the wilderness ahead. I just hope that I will be prepared.</t>
   </si>
   <si>
-    <t>The gently rolling dunes are gone. Scree clad mountains rise up in their stead. From abyssal floor to mist shrouded peaks they tower. The ground is steep, sharp, and treacherous underfoot. Darkness abounds - the light of the sun veiled by the mountains’ long shadows. Beneath me the earth groans and strains, trembling at the forces at work deep below.</t>
+    <t>The gently rolling dunes are gone. Scree clad mountains rise up in their stead. From abyssal floor to mist shrouded peaks they tower. The ground is steep, sharp, and treacherous underfoot. Darkness abounds - the light of the sun veiled by the long shadows of the mountains. Beneath me the earth groans and strains, trembling at the forces at work deep below.</t>
   </si>
   <si>
     <t>Before coming here I would awaken violently, panting and covered in layer of sweat, white knuckled fists digging bloody nails into my palms. I know this, for I can see the scars in my hands, even if I cannot recall the memories. Instead I wander the hallways of my dreams. The cavernous hall in which I walk broken by monolithic pillar, whose trunks rise unbroken to the ceiling above.</t>
@@ -76,16 +76,16 @@
     <t>When last I dreamed I saw a distant figure. I called out, but there was no reply. When I approached, it faded into the darkness, only to reappear further away. At first it vexed me, so I approached slowly, only to find it vanish again. Once more I tried, more carefully still, and this time the figure did not vanish. When at last I came upon it, I found a woman. She was clad in ivory robes, and asleep upon the floor. Suddenly I was overcome with unease, for when I looked upon her face, I realised I knew her.</t>
   </si>
   <si>
-    <t>A shadow lives within me, lurking in the back of my mind. Inside its inky depths is something from my past that I do not want to remember.  It swells to fill every crevice of mind, and I cannot think of anything else. Just as I try to bring the memory into focus it shrinks and retreats into my subconscious.</t>
-  </si>
-  <si>
-    <t>Hythinea’s kingdom is one of balance. At once terrifying and peaceful. Even the simplest journeys require absolute focus to avoid cutting my hands or twisting my ankle. But moments of peace come too - times when I can just sit upon the rocks and be alone. The wind drowns out the ill thoughts, and my mind is lifted of its burdens.</t>
+    <t>A shadow lives within me, lurking in the back of my mind. Inside its inky depths is something from my past that I do not want to remember. It swells to fill every crevice of mind, and I cannot think of anything else. Just as I try to bring the memory into focus it shrinks and retreats into my subconscious.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hythinea’s kingdom is one of balance. At once terrifying and peaceful. Even the simplest journeys require absolute focus to avoid cutting my hands or twisting my ankle. But moments of peace come too - times when I can just sit upon the rocks and be alone. The wind drowns out the ill thoughts, and my mind is lifted of its burdens. </t>
   </si>
   <si>
     <t>The shadow in me darkens, roiling like a storm eager to break. I worry that it will consume me. If it does not then this world surely will. Every breath I take languishes deep in my lungs, and the relief that water and food brings is too swiftly replaced with thirst and hunger.</t>
   </si>
   <si>
-    <t>Again I saw the woman in my dreams. This time she came to meet me, her long hair flowing with her robes as she walked. She sat upon her knees, and I saw the floor around us was no longer dark stone, but white marble, and the blackness around us lifted, revealing an infinite expanse of marbled pillars. There we sat together, waiting for… something. But something never came, and I woke confused, with only a greater sense of loss than before.</t>
+    <t>Again I saw the woman in my dreams. This time she came to meet me, her long hair flowing with her robes as she walked. She sat upon her knees, and I saw the floor around us was no longer dark stone, but white marble, and the blackness around us lifted, revealing an infinite expanse of marbled pillars. There we sat together, waiting for something. But something never came, and I woke confused, with only a greater sense of loss than before.</t>
   </si>
   <si>
     <t>Flashes of memory come and go, stirring up hope and despair within me. I see unfamiliar faces, solemn, with heads bowed. Like a great beast I feel my past approaching. It is distant now, but draws closer, growing ever more defined, until the full horror of its figure is clear.</t>
@@ -94,16 +94,16 @@
     <t>The beating heart of the earth resounds through the landscape. And with each beat I count down my life, one moment at a time. The shadowy claws of defeat desperately pull at the sanity I struggle to maintain. The direness of my quest becomes more apparent every day, for it is one that may claim my very soul.</t>
   </si>
   <si>
-    <t>I call her my angel. She will not tell me her true name. Though I recognise her face, it is her eyes that are most familiar to me. They are wide, with green irises, but burdened by the dark rings of sleepless nights. I have spoken to her, well, whispered really, for I am afraid to upset the fragility of the dream. I know she spoke to, but now I cannot recall what it was she said.</t>
-  </si>
-  <si>
-    <t>Whilst my vision grows dull, my dreams become more vivid, and with them she becomes more alive. I resent her absence when I wake, I think only of her as I walk through twilight lands, and the desire in my heart grows as weariness sets in. I am unaffected by the sting of injury, or the pang of hunger. I survive only to see the day through, so that I might be with her at its end.</t>
+    <t>I call her the white woman. She will not tell me her true name. Though I recognise her face, it is her eyes that are most familiar to me. They are wide, with green irises, but burdened by the dark rings of sleepless nights. I have spoken to her, well, whispered really, for I am afraid to upset the fragility of the dream. I know she spoke too, but now I cannot recall what it was she said.</t>
+  </si>
+  <si>
+    <t>Whilst my vision grows dull, my dreams become more vivid, and with them she becomes more alive. I resent her absence when I awake, I think only of her as I walk through twilit lands, and the desire in my heart grows as weariness sets in. I am unaffected by the sting of injury, or the pang of hunger. I survive only to see the day through, so that I might be with her at its end.</t>
   </si>
   <si>
     <t>Day and night, hour after hour, ceaseless in their howling do the mountain winds blow. From the throaty gusts across the wide mountain passes, to the shrill cry through narrow crevasses. The call of the mountain lords echo between every stone and every wall. I cannot see but one flower growing upon the mountainside, only poisonous vines and rusted metal. How cruel time is to bring beauty to ruin whilst leaving evil untouched.</t>
   </si>
   <si>
-    <t>Now we speak more freely, and her words remain in my memory even after I wake. I must know who she is, whether she is a part of my psyche, or just another apparition in this wasted world. I ask her how she knows where we are, how she knows who I am. I ask gently at first, but my curiosity turns to frustration when she will not answer, and as it so easily does, my frustration turns to anger.</t>
+    <t xml:space="preserve">Now we speak more freely, and her words remain in my memory even after I wake. I must know who she is, whether she is a part of my psyche, or just another apparition in this wasted world. I ask her how she knows where we are, how she knows who I am. I ask gently at first, but my curiosity turns to frustration when she will not answer, and as it so easily does, my frustration turns to anger. </t>
   </si>
   <si>
     <t>She turns her face to hide, but I can see the tears upon her cheek. I realise now that it does not matter who she is. She has not come to me to be my guide. She is not here to lead me to my fabled destiny. She is here to be with me, to give me respite when I sleep and to give me something to live for when my body is spent.</t>
@@ -115,31 +115,31 @@
     <t>Sea</t>
   </si>
   <si>
-    <t>A new land, different to the last in every way, but the heavy sense of dread in my stomach remains. An endless plain of salty islands - a landscape shattered by the endless beat of the sun. Only in the crevasses between the islands is it cool enough to survive. Some are small, almost hairline fractures, whilst others are so wide that the light of my torch does not reach the other side.</t>
+    <t xml:space="preserve">A new land, different to the last in every way, but the heavy sense of dread in my stomach remains. An endless plain of salty islands - a landscape shattered by the endless beat of the sun. Only in the crevasses between the islands is it cool enough to survive. Some are small, almost hairline fractures, whilst others are so wide that the light of my torch does not reach the other side. </t>
   </si>
   <si>
     <t>There is a curse laid upon this land. It is a curse that threatens to bring me to my knees. It weighs heavy upon my shoulders, begs me to give in to darkness. I utter a prayer under my breath to ward off the voices, but the Necromancer was right, there are no gods listening here.</t>
   </si>
   <si>
-    <t>The gate is the only constant on my journey. It stands some twenty metres high, constructed of smooth rock with no visible evidence of tool marks. It is as if there is only one gate, existing simultaneously across the five realms, like a nail hammered into layers of wood, binding the world together at a single point.</t>
-  </si>
-  <si>
-    <t>Sometimes I hear distant voices, muffled as if speaking from another room. It is as if the walls of the world are thinning, bringing the living and the dead close to each other. Some voices are louder than others, but they go quiet as soon as I speak out to them, leaving me in silence once again.</t>
-  </si>
-  <si>
-    <t>I came across the hull of an ancient boat. Though its mast was broken, and its sail long since carried away by the winds, I could see that it once would have flown across the waves swiftly. The planks of its hull were rotten, and its metal supports warped and rusted, but I could tell that it was once strong and sleek, able to glide atop the water’s surface and weather the heaviest of waves. Even now, shattered, and strewn across the wastes, the beauty of the vessel was clear to me, and I will carry that beauty until the end of my days.</t>
-  </si>
-  <si>
-    <t>The daytime sun bears down on me, burning my exposed skin. Even the salt seems to sizzle beneath its rays. So I am forced to walk in the shadows - my eyes accustomed now to the twilight gloom. The maze of salt hides the remains of the ancient sea -  the bones of ancient creatures half buried in the walls, and the bleached wrecks of ships strewn across the seabed.</t>
+    <t>The gate is the only constant on my journey. It stands some twenty metres high, constructed of smooth rock with no evidence of tool marks. It is as if there is only one gate, existing simultaneously across the five realms- like a nail hammered into layers of wood, binding the world together at a single point.</t>
+  </si>
+  <si>
+    <t>Sometimes I hear distant voices, muffled as though speaking from another room. It is as if the walls of the world are thinning, bringing the living and the dead closer to each other. Some voices are louder than others, but they all go quiet at the sound of my voice, leaving me in silence once again.</t>
+  </si>
+  <si>
+    <t>I came across the hull of an ancient boat. Though its mast was broken I could see that it once would have flown swiftly across the wave. The planks of its hull were rotten, and its metal supports warped and rusted, but I could tell that it was once strong and sleek, able to glide atop the water and weather the heaviest of waves. Even now, shattered, and strewn across the wastes, the beauty of the vessel was clear to me, and I will carry that beauty until the end of my days.</t>
+  </si>
+  <si>
+    <t>The daytime sun bears down on me, burning my exposed skin. Even the salt seems to sizzle beneath its rays. So I am forced to walk in the shadows - my eyes accustomed now to the gloom. The maze of salt hides the remains of the ancient sea - the bones of ancient creatures half buried in the walls, and the bleached wrecks of ships strewn across the seabed.</t>
   </si>
   <si>
     <t>When the Necromancer first told me of dead gods and ancient prophecies I thought her mad. Now I am not sure what I believe. Perhaps my hysteria has grown to such heights that I cannot distinguish dream from reality. Or perhaps it is all as it seems. Without evidence either way, I can only have faith in her words.</t>
   </si>
   <si>
-    <t>I told the angel what the Necromancer told me, and she nodded with a faint smile across her lips. After that we spoke more freely. To me she is still a stranger, I know I have memories of her, but they resist my call. She listens to me, and I her. We talk of things we love and things we lost. It does not matter if she is real, for she is real enough to keep me going.</t>
-  </si>
-  <si>
-    <t>My steps falter, and I come to a stop. My path is unclear. I see only a destination that leads to another - markers in the desert, endless but going nowhere. The shadow grows and my hope dwindles. There, deep inside me, there is my goal. I must dispel the clouds, but I am afraid of what I will find. No, I will wait. For now at least. I cannot face it yet.</t>
+    <t>I told the white woman what the Necromancer told me, and she nodded with a faint smile across her lips. After that we spoke more freely. To me she is still a stranger, I know I have memories of her, but they resist my summons. She listens to me, and I her. We talk of things we love and things we lost. It does not matter if she is real, for she is real enough to keep me going.</t>
+  </si>
+  <si>
+    <t>My steps falter, and I come to a stop. My path is unclear. I see only a destination that leads to another - markers in the desert, endless but going nowhere. The shadow grows and my hope dwindles. There, deep inside me, is my goal. I must dispel the clouds, but I am afraid of what I will find. No, I will wait. For now at least. I cannot face it yet.</t>
   </si>
   <si>
     <t>Where have the seas gone? Where are the tides that broke on salty shores and flowed around the now bleached corals? Life has vanished, never to return. It leaves a vacuum that cannot be filled. The water has been locked up at the ends of the earth - a memory of the world that was. The oceans are forgotten, the fisherfolk fled, but what remains must go on.</t>
@@ -154,28 +154,28 @@
     <t>Faith is what carries me forward. Not faith in the gods, but faith in myself. It turns my weakness into strength, so that I may see the light that casts the shadow. Though my steps are laboured I can see where my path leads, and so I go on with purpose - to free the gods, The Necromancer, and myself.</t>
   </si>
   <si>
-    <t>My dreams are no longer calming. My angel is more animate than ever, and it is draining me to my core. I wake feeling both physically and mentally exhausted. One moment she laughs and smiles, the marble floor radiating with soothing light as she does. The next she is on the ground, kicking and screaming with pain and rage, locked in her dream-prison.</t>
-  </si>
-  <si>
-    <t>During one of her fits she became suddenly still, contorted on the ground with fists curled and ragged breath. She turned her eyes to me, and I saw pain deep in them. I can do nothing to sooth her, but I would still rather be with her in the chaos of my dreams, than alone and awake in this midnight world.</t>
-  </si>
-  <si>
-    <t>She said that something was coming, something terrible, and that I must prepare myself. I tell her I know that she is dying, and I tell her I will come for her. At this she shook her head and wept. The darkness began to close in, and the dream came to an end. When I opened my eyes I did not see an ivory angel, only the dead sky above.</t>
+    <t>My dreams are no longer calming. The white woman is more animate than ever. One moment she laughs and smiles, the marble floor radiating with soothing light as she does. The next she is on the ground, kicking and screaming with pain and rage, locked in her dream-prison. It is draining me to my core. I wake feeling both physically and mentally exhausted.</t>
+  </si>
+  <si>
+    <t>One moment of fury and then she is still. She lies contorted on the ground with fists curled and ragged breath. She turns her eyes to me, and I see anguish in their green depths. I can do nothing to sooth her pain. But I would still rather be with her through the chaos and the anger than be alone in this midnight world.</t>
+  </si>
+  <si>
+    <t>She says that something is coming, something terrible, and that I must prepare myself. I tell her I know that she is dying, and I that I will come for her before it is too late. She shakes her head and weeps. The darkness begins to close in, and the dream comes to an end. When I open my eyes I do not see an ivory angel, only the dead sky above.</t>
   </si>
   <si>
     <t>I can see the sickness growing in her. Her hair has become thin, and her face gaunt. Even her robes have turned an ashen shade of grey. Her beautiful eyes are now sullen and set deep in dark sockets. She stumbles often when we walk together, and I fear that her time draws near. I must escape this terrible place. Even if I cannot save her, I must be with her. I will not let her be alone.</t>
   </si>
   <si>
-    <t>I hold her in my lap, and I watch her chest rise and fall. We have nothing to say, so we sit are silent. I hold her close. The dream-light is fading, drawing closer around us like a cocoon of darkness. I promise her we are close now, there is not long left. I am not sure if she can hear, but it does not matter, it was said as much for me as it was for her.</t>
-  </si>
-  <si>
-    <t>She tried to speak to me last night, but I could not hear her, for she was too far away. I tried to run to her, but I could not get close enough for her to hear. Instead I could see her eyes wide with terror, and her mouth open to scream. Now I could hear her, but it was a muffled scream as if from under water.</t>
-  </si>
-  <si>
-    <t>She screamed and screamed, the muscles on her atrophied arms tensed and relaxed in spasm. Then I too was screaming on my knees with my head in my heads. It did not end, it just went on, the endless wailing, and the tears. All I wanted to do was to hold her again, to stop her screams. But I could not.</t>
-  </si>
-  <si>
-    <t>The Ruination of Man</t>
+    <t>I hold her in my lap, and I watch her chest rise and fall. We have nothing to say, so we sit in silence. I hold her close. The dream-light is fading, drawing closer around us like a cocoon of darkness. I promise her we are close now, there is not long left. I am not sure if she can hear, but it does not matter, it was said as much for me as it was for her.</t>
+  </si>
+  <si>
+    <t>She tried to speak to me last night, but I was too far to hear. I tried to run to her but very time I came close I found myself whisked further away than before. I saw her eyes widen with terror, and her mouth open to scream. I could hear her then, but it was a muffled scream as if from under water. Then all went black, save for the green glow of her eyes.</t>
+  </si>
+  <si>
+    <t>She screams and screams, the muscles on her atrophied arms spasm uncontrollably. I realise I too am screaming. I am on my knees with my head in my hands. It does not end, it continues forever, the endless wailing, and the tears. I only wish to hold her, to caress her, to stop her screams. But I cannot.</t>
+  </si>
+  <si>
+    <t>The Red Fountain</t>
   </si>
   <si>
     <t>Ruins</t>
@@ -190,7 +190,7 @@
     <t>She lies unmoving on the floor. I try all I can to bring her back to life. Just as I feel hope slipping away she jerks awake, eyes wide, spitting red and black liquid upon herself. Before I have a chance to say anything, she points to the fountain, and to her lips, and again she says “Drink”. I shake my head, feeling the tears rolling down my cheeks. Again she points to her lips. I hang my head in despair, but I know it is what she needs.</t>
   </si>
   <si>
-    <t>She is silent now, her eyes will not open, she does not move. I would think her dead if it were not for the shallow breathing of her chest. The fervour of past dreams is gone, replaced instead by anxious waiting. I stand in the endless marble room, unable to do anything but watch her rest.</t>
+    <t xml:space="preserve">She is silent now, her eyes will not open, she does not move. I would think her dead if it were not for the shallow breathing of her chest. The fervour of past dreams is gone, replaced instead by anxious waiting. I stand in the endless marble room, unable to do anything but watch her rest. </t>
   </si>
   <si>
     <t>Time passes imperceptibly slowly, and I cannot take my eyes from her. Truly this is hell, to watch and not know what to do but wait. Wait until the hours of my life are spent. I wake slowly now, gazing at the sky and unable to rise. My body betrays me. Muscles tug feebly at aching tendons. I fear I am losing myself to this world, and to her.</t>
@@ -205,16 +205,16 @@
     <t>I will never forget the pain on her face as she drank, or the pain I felt as I held her, thinking she would never wake. But wake she did, rousing slowly from her death sleep. She looked well once again, her skin warm and the mania driven from her eyes. She lifted her hand to mine, and kissed my cheek. I carried her away from the vile fountain, and as I did the light began to return.</t>
   </si>
   <si>
-    <t>Finally things seem to have changed for the better. A warm glow replaces ghostly pallor and her eyes bright once again. I rejoice, and tell her I believed she was lost. “I’m sorry” she says. But I tell her not to be sorry, that she cannot hold herself to blame. I tell her of the things I had remembered since we last spoke- happy memories, places I had been. She nods and listens, though her thoughts seem far away.</t>
+    <t xml:space="preserve">Finally things seem to have changed for the better. A warm glow replaces ghostly pallor and her eyes brighten once again. I rejoice, and tell her I believed she was lost. “I’m sorry” she says. But I tell her not to be sorry, that she cannot hold herself to blame. I tell her of the things I had remembered since we last spoke- happy memories, places I had been. She nods and listens, though her thoughts seem far away. </t>
   </si>
   <si>
     <t>The city is ancient. How ancient I wonder? How long since the guards abandoned their posts. Was it the fire-laced breath of artillery that brought down the city’s walls or merely the inescapable erosion of time? Through it all The Necromancer has haunted the world, or so she says. She watched the essence dig take ahold of her world, and not once has she seen its grip weaken.</t>
   </si>
   <si>
-    <t>Fierce have been the ravages of time upon this ancient city. Even now there remain signs of plight- dark craters, munition cases- tarnished and spent. Even the rusted carcasses of war machines litter the land. But there are no bones, no bodies, no graves, no markers of human inhabitation to speak of.</t>
-  </si>
-  <si>
-    <t>At first I thought I was dreaming, but no, there she is, standing before me. A vision, but still with me here in the waking world. She looks better, her features full and no longer sunken, and her smile has returned. She is not near enough to hear me call out, so I wave to her instead. For a moment it seems as though she cannot see me, but she waves back. Then as suddenly as it began, the vision ends.</t>
+    <t xml:space="preserve">Fierce have been the ravages of time upon this ancient city. Even now there remain signs of plight- dark craters, munition cases- tarnished and spent. Even the rusted carcasses of war machines litter the land. But there are no bones, no bodies, no graves, no markers of human inhabitation to speak of. </t>
+  </si>
+  <si>
+    <t>At first I thought I was dreaming, but no, there she is, standing before me. A vision with me here in the waking world. She looks better, her features full and no longer sunken, and her smile has returned. She is not near enough to hear me call out, so I wave to her instead. For a moment it seems as though she cannot see me, but she waves back. Then as suddenly as it began, the vision ends.</t>
   </si>
   <si>
     <t>The old world has been swept away. It is good the Necromancer cannot be with me to see it. If she were to lay her eyes upon the ruins she surely would fall to her knees and weep. Perhaps that is why she whispers to me from the darkness - to shield herself from reality, to allow herself to have hope in a place where none can be found.</t>
@@ -223,22 +223,22 @@
     <t>I cannot imagine the things The Necromancer has had to endure. Sometimes I think my burden insignificant compared to hers. After all what is the worth of one life against that of an entire civilisation? But we all have our own cross to bear. The more I stay here, the more I see what has been lost. When this is all over I will return to help her, if I can.</t>
   </si>
   <si>
-    <t>The shadow within grows, pressing against my skull. I feel despair well up uncontrollably. My breathing comes shallow and my heart rises into my throat. Panic. My vision tunnels and I collapse to the floor. Then before me I see her, my angel, her cool hand upon my forehead. Memories explode within me, I see her pale face, flowers, white sheets, blood. “Breathe” she says. I close my eyes and breath deep- once, twice, feeling the despair dissipate. Then I open them only to find her gone.</t>
-  </si>
-  <si>
-    <t>I do not think I could bear to watch as the places I know fall into disrepair and the people I love age and die. I could not bear to be alone to be without someone to ease my pain. Left with only my unquietable thoughts for company, reliving my lost past over and over. I would watch my past self and wish that I could change the things that can never be changed. And I would wish to go back and spend one last moment with those who are gone.</t>
+    <t>The shadow within grows, pressing against my skull. I feel despair well up uncontrollably. My breathing comes shallow and my heart rises into my throat. Panic. My vision tunnels and I collapse to the floor. Then before me I see her, my angel, her cool hand upon my forehead. Memories explode within me, I see her pale face, flowers, white sheets, blood. “Breathe” she says. I close my eyes and breath deep- once, twice, feeling the despair dissipate. Then I open them, only to find her gone.</t>
+  </si>
+  <si>
+    <t>I do not think I could bear to watch as the places I know fall into disrepair and the people I love age and die. I could not bear to be alone, without anyone to ease my pain. Left with only my unquietable thoughts for company, reliving my lost past over and over. I would watch my past self and wish that I could change the things that can never be changed. And I would wish to go back and spend one last moment with those who are gone.</t>
   </si>
   <si>
     <t>Another vision. I can see her in the corner of my eye. She sits at the top of a tall set of steps. As I reach the top I realise she is not looking at me, but at the base of a broken statue. Atop the statues’ weathered head is a crown- tarnished but still golden. This man, a king, was once well loved by his people. So loved that even today it remained untouched by scavengers. She points at the inscription at its base but I cannot make out the words. The raised stone letters have been worn away by the wind. I will never know his name.</t>
   </si>
   <si>
-    <t>I remember a story I heard once, about an old man. He lived alone in an old cottage. Like him the building had not aged well, its walls were cracked and the roof fallen in. He was bitter, and set in his ways, and went out only to buy from the local village what he could not make himself. He had not always been bitter, he had not always been alone. One day there were children playing outside his window. He ignored them as best he could, but an errant ball missed its mark and came through his window with a crash. So he yelled at the children, and drove them back to the village. When he returned he cleared up the pieces of shattered glass, but could not repair the window. He did not want to return to the village, and so he left it- a gaping void in the side of his house.</t>
-  </si>
-  <si>
-    <t>Time passed, and still the window remained broken. The old man could not repair it himself, and did not have the money to pay to have it mended. So the thought of it drifted from his mind, at least until Autumn came. Strong winds rocked the aged house whilst lashes of rain made their way in through the open window. Day after day it came through until not an inch of the house remained dry. But the old man ignored it- after all, he had endured worse.</t>
-  </si>
-  <si>
-    <t>Then the cold weather came, bringing snow and frost and ice. The old man huddled for warmth in his broken home, his fire dwindling and his supplies low. Finally he relented, and went to the village to beg to have the window repaired. But it was too late, nobody had the tools to fix the window, as broken and warped as it was. They offered him shelter, but his pride took him back home. So there he slept, in the cold and the light of the dying fires, waiting for Spring to come. But there would be no Spring for him, only a deep sleep and a white light, followed by oblivion.</t>
+    <t>I remember a story I heard once, about an old man. He lived alone in an old cottage. Like him the building had not aged well- its walls were cracked and the roof fallen in. He was bitter and set in his ways, and went out only to buy from the local village what he could not make himself. He had not always been bitter, he had not always been alone. One day there were children playing outside his window. He ignored them as best he could, but an errant ball missed its mark and came through his window with a crash. So he yelled at the children, and drove them back to the village. When he returned he cleared up the pieces of shattered glass, but he could not repair the window. He did not want to return to the village, and so he left it- a gaping void in the side of his house.</t>
+  </si>
+  <si>
+    <t>Time passed and still the window remained broken. The old man could not repair it himself and did not have the money to pay to have it mended. So the thought of it drifted from his mind, at least until the Autumn came. Strong winds rocked the aged house whilst the lashing rain made its way in through the open window. Day after day it came through until not an inch of the house remained dry. But the old man ignored it- after all, he had endured worse.</t>
+  </si>
+  <si>
+    <t>Then the cold weather came, bringing snow and frost and ice. The old man huddled for warmth in his broken home, his fire dwindling and his supplies low. Finally he relented, and went to the village to beg to have the window repaired. But it was too late, nobody had the tools to fix the window as broken and warped as it was. They offered him shelter, but his pride took him back home. So there he slept, in the cold and the light of the dying fires, waiting for Spring to come. But there would be no Spring for him, only a deep sleep and a white light, followed by oblivion.</t>
   </si>
   <si>
     <t>I saw her once again. She sat outside a ruined building reclining on a small drift of sand. So I sat with her, and I asked her how she had escaped her dream prison, but she only gave me a knowing smile and changed the conversation. I do not belong to this world, yet I am growing comfortable here. I am afraid that if I leave I will lose her.</t>
@@ -259,52 +259,85 @@
     <t>Wasteland</t>
   </si>
   <si>
-    <t>Here I stand, in the Eternal Wasteland, at the end of all things, searching for something I cannot find, running from something I cannot remember. It is fitting that, if I should die, I should die here, in this bleak landscape, devoid of memory, no evidence of the past, and no future to speak of. At least it would be a peaceful death, with no-one to see, and no-one to mourn.</t>
-  </si>
-  <si>
-    <t>Though at least a thousand years have passed the scars of the war remain untouched here. The earth has died, and cannot harbour life. Canyons criss cross the landscape, and within them so do the tracks of ancient war machines. The spirits of the dead linger, striking the ground as bolts of lightning, reminding the living that this world is not theirs.</t>
-  </si>
-  <si>
-    <t>I have seen the gods. I know them to be real. Yet I still cannot believe in them. I simply cannot accept that they can do anything to help me. Indeed they might be able to change this world, and in turn help the Necromancer, but they cannot help me. I will not hide from reality any longer. I have looked for comfort in faith, I have tried to ignore my pain, but the only way to be rid of it is to confront it.</t>
-  </si>
-  <si>
-    <t>I admit to myself, I have been selfish. I am not looking for the tombs because I wish to help the Necromancer or her world. I do it because I want to be free of my own suffering. At least now I can empathise with her, though she may be blinded by her faith. Together though, we can work together, and perhaps we both can summon the courage to face down our demons.</t>
-  </si>
-  <si>
-    <t>The gods are gone, fled from this world. The vaults of their tombs are empty, their souls lost to this world. The ingenuity of man has failed. It is a sad truth, impossible to bear, yet it is the truth. It is a truth born upon a wind that lifts the weight from my shoulders and draws the despair from my lungs. It provides me with a certainty, where before there was only uncertainty. This dark, dim, and despairing world is doomed. There is nothing left to do, but accept our fate.</t>
-  </si>
-  <si>
-    <t>There is nothing that can bring us back from the beyond. The suns will fade and shrink, and the land will freeze beneath the starless skies, and all the beasts upon the earth will huddle together for warmth as they take their final breaths on this world. The Necromancer cannot accept this fact, and therein lies the root of her madness.</t>
-  </si>
-  <si>
-    <t>I pity her, for I know her struggle. I do not know where she will go when the last gate is opened. I do not think she will ever be whole again. Whoever she was all those years ago is not who she is now. In some ways I envy her blind belief, with it I could ignore the revelation that is coming, but I cannot make myself blind, instead I will have to face the truth.</t>
-  </si>
-  <si>
-    <t>I can hear in her voice that her suffering grows. With every passing moment her faith is tested, the doubt grows in her mind. She has seen the destruction of her home, her world, and her people. She forfeited her life because she believed that one day the world would be cleansed of its corruption. That belief grew stronger with time, growing ever less rational, consuming her. But she had to believe it, because only by the saving the world could her life be saved.</t>
+    <t>Here I stand at the end of all things. Searching for something I cannot find. Running from something I cannot outpace. Devoid of memory, no evidence of my past, and no future to speak of. It is fitting that if I should die, I should die in this bleak landscape, this eternal wasteland. At least it would be a peaceful death- alone, and with no-one to mourn my passing.</t>
+  </si>
+  <si>
+    <t>Though I wish to lie down, close my eyes, and drift into an endless oblivion, I cannot. She waits for me in another world, and I promised her I would return. I must see our terrible story to its end.</t>
+  </si>
+  <si>
+    <t>Though uncountable years have passed the scars of the war have not faded. The earth is dead- its flesh torn apart and bled dry. Canyons criss cross the landscape, and within them lie the tracks of old machines. The lingering bodies of the dead remind the living that this world is not theirs.</t>
+  </si>
+  <si>
+    <t>I round another corner and there she is. She lies on the floor, her pale face staring up at the sky, surrounded in blood. I rush to pick her up, but as I lay my hands upon her she vanishes like smoke from a fire. As the smoke dissipates, I feel an omen of what is to come.</t>
+  </si>
+  <si>
+    <t>Though I have seen their tombs and the wretched souls they have left behind I cannot bring myself to believe in the gods. No matter what the Necromancer has promised I do not believe they can help me. I have looked for comfort in faith and I have not found it. I have tried to ignore my pain but it cannot be ignored. Now I realise the only way to be truly rid of it is to confront it.</t>
+  </si>
+  <si>
+    <t>I admit to myself, I have been selfish. I have sought the tombs not to aid the Necromancer or her world, but to be free of my own suffering. I will be better. We can work together. We can help each other in our struggles. Perhaps then we both can summon the courage to face down our demons.</t>
+  </si>
+  <si>
+    <t>I am beginning to understand what is behind the shadow within me. Whether by sickness or by age, the white lady will die. And we will not be together. At least I do not believe we will. I cannot convince myself of an afterlife, and so I must face the only alternative. Only now that I recognise it do I see the same fear in the Necromancer. I know what it is she doubts, what she tries to avoid thinking about despite day after day of decay.</t>
+  </si>
+  <si>
+    <t>The gods will never return. I think deep down she knows this to be truth. The moment I broke open their tombs I could see nothing of the old gods remained. How will she cope when the final gate is opened and the fate of her world is finally sealed. I will be there for her, as she has been for me. But she will have to face her fear alone, as I have done.</t>
+  </si>
+  <si>
+    <t>So the gods are gone. The vaults of their tombs are empty, their legacy lost in time. The ingenuity of man has failed. The end will come. Though it is not my world the realisation of it’s fate sweeps through me like a powerful wind. And with it my burdens are borne away. The weight of my quest has lifted. Now I have certainty over the future, where before there was only uncertainty. The world is doomed, but I still I will complete my quest- for the Necromancer, and for myself.</t>
+  </si>
+  <si>
+    <t>Things are better and things are worse. It was the not knowing, the shroud that veiled the future, that led me down dark paths. It is terrible that I should be relieved in the face of such evil tidings, but still I am. I would rather know where my path will lead me than be unsure, even if it takes me to death.</t>
+  </si>
+  <si>
+    <t>There is nothing that can be done to divert the path of fate. The suns will fade and shrink. The land will freeze beneath the starless skies. The beasts of the earth will huddle together as they take their final breaths. For those of us who cannot accept this there is only madness. That is the route the Necromancer has chosen.</t>
+  </si>
+  <si>
+    <t>I pity her, for I know her struggle. I do not know where she will go when the last gate is opened. I do not think she will ever be whole again. Whoever she was all those years ago has been lost. In some ways I envy her faith, without it she surely would not have endured this long. From faith she has drawn strength, but at a cost. The stronger her faith grows, the less willing she will be to accept the truth.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have heard the suffering in The Necromancer’s voice. With every passing moment her faith is tested, the doubt grows in her mind. She has seen the destruction of her home, her world, and her people. She forfeited her life because she believed that one day the world would be cleansed of its corruption. That belief grew stronger with time, growing ever less rational, consuming her. But she had to believe it, because only by the saving the world could her life be saved. </t>
   </si>
   <si>
     <t>We all are prey to irrationality, we must hold fast to the belief that our dark days precede the light. Without it we would be paralysed in hopelessness. Only through this belief are we able to change the course of our lives. We can push against the currents of reality rather than allow ourselves to be swept away. To give in is not in our nature, to lay down our arms at the feet of our aggressors rather than fight for what we hold dear. Our belief allows us to overcome horror and sorrow, and go on striving for better days, even when we ourselves may not see them.</t>
   </si>
   <si>
-    <t>When the time comes, as it does for all of us, when the dissonance in our mind comes to a crescendo, our lives change irreversibly.  Either we succumb to the alluring voice of denial, or we accept the harsh voice of reality.</t>
-  </si>
-  <si>
-    <t>We shared another quiet night. She looked well again, though there was a sadness in her voice that couldn’t be displaced. She asked me about the world, but I did not wish to tell her about it. I sensed that her fate is somehow related to the fate of the gods. Instead I told her that the essence was retreating, that it would not be long before I opened the final gate. I expected her to be elated, to beam and throw her arms around me. Instead she smiled weakly, and became quiet. I did not speak further. I did not know what to say, so I let the silence say it for me. We held hands, and when the time came to wake, I kissed her softly. As I left the dream world she held her hand out to me, and said she loved me.</t>
-  </si>
-  <si>
-    <t>Now I am alone. When I fell asleep she was gone. I called out for her, but there was no answer. I ran through the endless corridors of my mind to find her, but there was nothing but emptiness. I knew she would not return. I had not opened the gates in time, and now she was gone forever. I sat in my dream world, overwhelmed with emotion. Despair and relief washed over me in equal measures. She would not be in pain any longer, but I do not think I can go on without her. The world is so bleak, so harsh, that without hope I cannot hope to overcome it. Despite our short time together, I will not be able to forget her, I know she will be with me until my last breath.</t>
-  </si>
-  <si>
-    <t>The fog has cleared, and the memories return. The woman, the angel of my dreams, she was real once, a long time ago. I know this, because I was there with her at the end. She believed we would meet again, beyond the veil, she believed it because she had to believe it. Because it was the only thing that would ease the truth of her passing, we knew that nothing could be done for either of us. I am not sure if I believed that we would meet again, but the lie was so sweet. We used the lie to spend our last times in peace and not fear. To pretend to each other as if we were going on a long journey was far easier than to speak a final farewell.</t>
+    <t xml:space="preserve">When the time comes, as it does for all of us, when the dissonance in our mind comes to a crescendo, our lives change irreversibly. Either we succumb to the alluring voice of denial, or we accept the harsh voice of reality. </t>
+  </si>
+  <si>
+    <t>I see her silhouette against the horizon. Then again in the frame of a collapsed building. Instead of approaching she only walks away from me. I run towards her but she is too far to catch. Why will she not speak with me? Slowly I can feel her growing more distant, slipping out of my reach.</t>
+  </si>
+  <si>
+    <t>I have spent my days thinking about what will be. I have been so obsessed with the future that I have overlooked the things that are. I remind myself that the future will come, and all that is now will be lost forever. I must keep myself in the present lest I waste my life waiting for things to come.</t>
+  </si>
+  <si>
+    <t>Finally she comes to me. She looks different though, somehow strained. Her body is thinner and the lines of her face deeper. Not ill-looking like before. Merely... tired. An extreme tiredness that cannot be recovered by sleep alone. She speaks it with a whisper and I cannot make out the words. I put my head to hers, and she will not meet my gaze.</t>
+  </si>
+  <si>
+    <t>She is following me now, just out of range of hearing. She drags her feet along the ground, and stares beyond the line of horizon at something I cannot see. I stand in front of her, forcing her to come to a stop. I wrap my arms around her, and wait. At first she remains motionless. I can feel her gaze locked ahead and sense the distance in her arms. Then, slowly, she bows her head into my shoulder and returns my embrace.</t>
+  </si>
+  <si>
+    <t>Now that she follows closer I tell her all that has happened since we were in the ruined city and of the evil that waited behind the gate of Ahna. Then I tell her of my revelations, of the thing that I feared but now understand. When I finish speaking she takes my hand in hers and strokes my palm. She lifts it to her cheek and sighs deeply. She sits on the ground, so I join her. Finally, she talks.</t>
+  </si>
+  <si>
+    <t>I have been thinking about what she told me. She said things had happened, would happen. I didn’t understand fully. She talked as if things in the future were in the past. She said I would understand when I entered the last tomb. I asked her to speak clearly, to tell me what she meant. Confusion washed over her face, and her eyes snapped back to the horizon. She did not follow me any further, so I continued on alone.</t>
+  </si>
+  <si>
+    <t>I saw her in my dreams again, though the words of our last meeting lingered in my ears. I did not know what to say, so I let silence speak for me. We held hands, and when the time came to wake, I kissed her softly. As I left the dream world she held her hand out to me, and said she loved me.</t>
+  </si>
+  <si>
+    <t>Now I am alone. I call out for her but there is no answer. I run through the endless corridors of my mind to find her, but there is only emptiness. Somehow I know she will not return.</t>
+  </si>
+  <si>
+    <t>The world is so bleak now that she is gone, so harsh, that I feel cannot hope to overcome it. Despite our short time together I will not be able to forget her, and I know she will be with me until my last breath.</t>
   </si>
   <si>
     <t>Main Story</t>
   </si>
   <si>
-    <t>You wept. Alone, and in darkness. I watched you across the great cold distance and in you I saw myself. I have brought you here, to my world, so that we might both be saved. We both can look upon these desolate plains with unfamiliar gaze. But this was once my home. Long before the darkness fell these lands were green. I would walk amongst the trees and feel the grass beneath my feet. Now the groves are dead, and I pass like a shadow among them. Only the sun-scorched dirt remains.</t>
-  </si>
-  <si>
-    <t>There were once five gods who roamed the world. Around them five great kingdoms were founded. Our civilisations grew with time. Miracles became rote; our cities rose high into the heavens and our machines worked the earth. The gods saw they were no longer needed, and so they retreated from the world of man. One day, when we had all but forgotten our roots, they vanished. But the vacuum left by their absence was clear. Something changed, in the air, the earth, and the sea. The essence that binds the world turned on us. It soured the earth and awoke ceaseless winds. The gods are gone, and with them, our humanity.</t>
+    <t>You wept. Alone, and in darkness. I watched you across the great cold distance and in you I saw myself. I have brought you here, to my world, so that we might both be saved. I look upon these desolate plains with an unfamiliar gaze, but this was once my home. These lands were green long before darkness fell upon them. I would walk amongst the trees and feel the grass beneath my feet. Now the groves are dead, and I pass like a shadow among them. Only the sun-scorched dirt remains.</t>
+  </si>
+  <si>
+    <t>There were once five great beings, gods to you, who roamed the world. Around them five great kingdoms were founded, and over time our civilisations grew. Miracles became rote; our cities rose high into the heavens as our machines worked the earth. The gods saw they were no longer needed, and so they retreated from the world of man. One day, when we had all but forgotten our roots, they vanished. But the vacuum left by their absence was clear. Something changed, in the air, the earth, and the sea. The essence that binds the world turned on us. It soured the earth and awoke ceaseless winds. The gods are gone, and with them, our humanity.</t>
   </si>
   <si>
     <t>Ahead lies a dead world- a stagnant place where only barbarism and hopelessness remain. But I believe if we can bring back the gods we can restore it all. I know where they are. They sleep in the place between places, the dark realm beyond the veil of reality. There are five gates that lead to this realm, but they lie dormant, activated by temples long since fallen to the essence. I cannot cleanse the temples, but I can guide you to them. Only together can the gods turn the tide of decay, and offer you the peace which you so dearly seek.</t>
@@ -322,43 +355,46 @@
     <t>So it is done, you have passed through the gate and the realm between the shadows. You have done wonderfully. Already I hear Eo’s voice on the wind - calling for her lost siblings. How must it feel, to awaken from one nightmare into another, to see your beautiful world in ruins. I was there whilst it happened - I watched the life of the earth fade away. But I was cursed to remain as everything I loved turned to dust. I saw my friends and my family die, as I was doomed to solitude by immortality. I do not feel pity for the dead, wanderer, for it is the living alone who are left who grieve.</t>
   </si>
   <si>
-    <t>We stand now in the kingdom of Hythinea, the warrior goddess, queen of motherhood. This was once the the backbone of the world. Atop the highest mountains her fortresses were built, and in deepest dells her cities. Gone are the grassy slopes with their grazing flock. Gone are the roads where merchants once ran their goods. Gone are the flowered pastures and gentle rivers. Now there is only dirt and rock amongst the shattered peaks. Dark shadows cast by black crags, and the eyes of evil looking out from dismal caves.</t>
-  </si>
-  <si>
-    <t>This was my home before I became The Necromancer. When I was a child the sun rose high above the horizon and the sky was still blue. I was there when the gates were built. I watched as the sands encroach upon our kingdoms, and with them our ties to our brothers and sisters disappear on the desert winds. I remember when the last flowers faded. I remember when the rivers dried up. I remember the day when the brave lost their voice, and the braying of animals was replaced by screams of the dying. I have kept my faith all these years, believing that I would find someone like you to save us. Long have I waited here, Wanderer, but I knew that you would come.</t>
+    <t>Before us is the kingdom of Hythinea, the warrior goddess, queen of motherhood. This was once the the backbone of the world. Atop the highest mountains her fortresses were built, and in deepest dells her cities. Gone are the grassy slopes and their grazing flock. Gone are the roads where merchants once ran their goods. Gone are the flowered pastures and gentle rivers. Now there is only sand and rock amongst the shattered peaks. Dark shadows cast by black crags, and the eyes of evil looking out from dismal caves.</t>
+  </si>
+  <si>
+    <t>Before I was the Necromancer I was someone else, and this was my home. When I was a child the sun rose high above the horizon and the sky was still blue. I was there when the gates were built. I watched the sands encroach upon our kingdoms, and with them the ties to our brothers and sisters disappeared on the desert winds. I remember when the last flowers faded. I remember when the rivers dried up. I remember the day when the brave lost their voice, and the braying of animals was replaced by silence of the dead. I have kept my faith all these years believing that I would find someone like you to save us. Long have I waited here, Wanderer, but I knew that you would come.</t>
   </si>
   <si>
     <t>Again and again I see your fate repeated in my dreams. I watch as the final temple is cleansed, and the last gate illuminated with life. Time and time again I see the gods reverse the wheel of time and raise our cities up from the dust. It has been prophesied, and so it will be. Go now, into the mountains where the cold winds blow and the sun dare not dwell. Find the one who sleeps and return her to us.</t>
   </si>
   <si>
-    <t>I can sense the question in your heart- who is the woman who you dream of? Yes, I have seen your dreams, and I know the dread that grows in your heart. She is your wife, Wanderer, and she is dying. I did not want to tell you before, for I thought that the knowledge would be too much for you to bear. I see now I was wrong, you are stronger than I ever could have thought. There is still time to save her, but you must be fast.</t>
-  </si>
-  <si>
-    <t>We have come to the most desolate of all places- the sea of salt. There was once a great ocean here, one that spanned between the shores of the land, unbroken for thousands of miles. Now the water is gone, locked up in the frozen poles leaving only salt behind. Only the bones of dead leviathans can tell us what was here. Their harrowing echoes boom in the saline crevasses that criss cross the ancient seabed.</t>
-  </si>
-  <si>
-    <t>When I was young, my father would talk of the ocean. We lived in the mountains, but his heart was with the sea. He would draw ships when his mind wandered, and we during the summer months we would often find him staring out towards the horizon, his soul somewhere far away. But life kept him from the sea. My mother worked in the city, I had my school, there we a myriad of reasons we could not go. Eventually the procession of time wore away at him, we all grew older, and as the winter of old age set in, the dream of the sea slipped away. My father was not an unhappy man, quite the opposite in fact, but there was always a part of him that was not with us, a part that belonged to the shore, and to the waters of the sea. He is gone now. They all are. Even the sea.</t>
-  </si>
-  <si>
-    <t>My family remains with me, watching down from the halls of heaven. They are among good people- my friends, other mystics I knew, and thousands of others. They watch me as I hold my vigil on earth, watching, wandering, writing, preserving their memory for those who will come later. My mother and father were not there when the sun tore itself into three, or when the foundations of our cities turned to dust and were borne away by the empty wind. When I die they will know, I will tell them everything I have seen, I will tell them of you, of what we have done. I know they will be proud. That is how my beliefs have remained strong, Wanderer. Not through madness or obsession, but because of my parents love. I do all I do so that those who have lost may love again.</t>
-  </si>
-  <si>
-    <t>The seasons blend together, winter and summer differentiated only by the height of the sun. The weather does not relent, nor the interminable march of time and the waste it brings. When my vigil began the wounds of war were still fresh in the earth. Slowly they healed, with every spring that passed more flowers would grow, and nature would claim what man had left behind. Soon enough there were no traces to be seen amongst the trees and wild things. Then the essence’s influence set in. The flowers would not bloom, the grass wilted and died, and the soil turned to sand. Then the war machines were revealed again, like primordial beasts risen to walk upon the earth once more. Their rusty carcasses standing testament to the permanence of mankind’s work. There they rest still, waiting for the end.</t>
-  </si>
-  <si>
-    <t>It is always darkest before the dawn, or so they say. There can be no triumph without sacrifice. Even as the sickness that pervades this world tightens its grip, there is still a chance for redemption. My people have known for a long time that our sacrifice must be paid in blood. There were many of us in the beginning. So many who gave their lives to halt the spread of evil. Scholars, teachers, students, clerics- all those who could dedicate their minds to our cause, these were my people. They called us the Mystics, a name we came to embrace as time went on. It was they who made me what I am today, incapable of death, but unable to exist with the living.</t>
-  </si>
-  <si>
-    <t>In the first days I did nothing but roam the earth, documenting what I saw. But the deserts spread faster than I could, the animals retreated and died, and a great pall was set upon the earth. Still I searched for pockets of life- a mountain tarn still teeming with fish, or a woodland hidden away in some far corner. Never did I find anything, and I came to realise I never would.  But my hope has never waned.</t>
-  </si>
-  <si>
-    <t>We are nearing the end. I feel the air changing as you advance. It is lighter, as if a weight were lifting. Even the sun seems brighter to my eyes. Soon I will be able to show you the wonders of this world. When the gods return we will walk the ground together. I will give you the life you desire, and you will take my hand as we watch an ancient dawn become new once more. We are so close to the end, Wanderer. The next gate will take you to the ruins of our greatest city, where the lingering ghosts of the dead cry out for life.</t>
-  </si>
-  <si>
-    <t>The winds are changing, old currents blow once more, interrupting the monotonous cycle that has gone on for too long. The gods are waking, their spirits waking the world from its terminal sleep. The essence grows agitated, pulling at invisible threads in the air. It resists their control, for now, but when Corypthos awakens it will relent- bound once more. The deserts will retreat, pushed back by the tide of life that yearns to spill across the barren earth.</t>
-  </si>
-  <si>
-    <t>Our struggle is almost at an end, Wanderer. I see the trauma in your eyes grow with every moment that passes. You are remembering what it was you left behind, that I rescued you from. Yes, what you fear to be real is indeed so. Corpythos, lord of life, awaits you in the Wasteland. He can bring her back, Wanderer. So too can he free me, return me my body so that I may walk among the trees once again. And my people, he will return them too, oh how soon it will be. Oh, I am sorry, I cannot hide my elation. I know you suffer, but you cannot know how I have suffered, and how soon that suffering will come to an end. When it is done, when duty fulfilled and my vigil over, I will return home, and I will sit as my father sat, and I will watch the sun set as it did so many years ago.</t>
+    <t>I sense the question in your heart- who is the woman of whom you dream? Yes, I have seen your dreams, and I know the dread that grows in your heart. You know who she is, Wanderer, and you know she is dying. I did not want to tell you before. I thought that the knowledge would be too much for you to bear. I see now I was wrong, you are stronger than I ever could have thought. There is still time to save her, but you must be fast.</t>
+  </si>
+  <si>
+    <t>We have come to the most desolate of all places- the Sea of Salt. There was once a great ocean here, one that spanned between the shores of the land, unbroken for thousands of miles. Now the water is gone, locked up in the frozen poles leaving the salted plains in its stead. Only the bones of dead leviathans can tell us what was here. Their harrowing echoes boom in the saline crevasses that criss cross the ancient seabed.</t>
+  </si>
+  <si>
+    <t>When I was young my father would talk of the ocean. We lived in the mountains, but his heart was with the sea. He would draw ships when his mind wandered, and during the summer months we would often find him staring out towards the east, his soul somewhere far away. But life kept him from the sea. My mother worked in the city, I had my school, there were a myriad of reasons we could not go. Eventually the procession of time wore away at him, and as the winter of old age set in the dream of the sea slipped away. My father was not an unhappy man but there was always a part of him that was not with us, a part that belonged to the shore, and to the water. He is gone now. They all are. Even the sea.</t>
+  </si>
+  <si>
+    <t>My family remains with me, watching down from the halls of heaven. They are among good people- friends, lovers, and thousands of others. They watch me as I hold my vigil on earth, watching, wandering, writing, preserving their memory for those who will come later. My mother and father were not there when the sun tore itself into three, or when the foundations of our cities turned to dust and were carried away by the dry wind. When I die they will know, I will tell them everything I have seen, I will tell them of you, of what we have done. I know they will be proud. That is how I have remained resolute in my belief Wanderer. Not through madness or obsession, but because of my parents love. I do all I do so that those who have lost may love again.</t>
+  </si>
+  <si>
+    <t>The seasons blend together, winter and summer differentiated only by the height of the sun. The weather does not relent, nor the interminable march of time and the waste it brings. When my vigil began the wounds of war were still fresh in the earth. Slowly they healed, with every spring that passed more flowers grew, and nature reclaimed what man had left behind. Soon enough there were no traces of the past amongst the trees and wild things. Then the essence began to take hold. The flowers would not bloom, the grass wilted and died, and the soil turned to sand. Then the war machines were revealed again, like primordial beasts risen to walk upon the earth once more. Their rusty carcasses standing testament to the permanence of mankind’s work. There they rest still, waiting to be woken once more.</t>
+  </si>
+  <si>
+    <t>It is always darkest before the dawn, or so they say. There can be no triumph without sacrifice. Even as the sickness that pervades this world tightens its grip, there is still a chance for redemption. My people have known for a long time that our sacrifice must be paid in blood. There were many of us in the beginning. So many who gave their lives to halt the spread of evil. Scholars, teachers, students, clerics- all those who could dedicate their minds to our cause, these were my people. They called us the Mystics, a name we came to embrace as time went on. It was they who made me what I am today, incapable of death, but unable to exist among the living.</t>
+  </si>
+  <si>
+    <t>In the first years of my new life I did nothing but walk the earth, documenting what I saw. But the deserts spread faster than I could, the animals retreated and died, and a great darkness was set upon the earth. Still I searched for pockets of life- a mountain tarn still teeming with fish, or a woodland hidden away in some far corner. Never have I found anything, but my hope has never waned.</t>
+  </si>
+  <si>
+    <t>We are nearing the end. I feel the air changing as you advance. It is lighter, as if a weight were lifting. Even the suns seem brighter to my eyes. Soon I will be able to show you the wonders of this world. When the gods return I will give you the life you desire we will bring her back to this world, and together we will watch an ancient dawn become anew. We are so close to the end, Wanderer. The next gate will take you to the ruins of our greatest city, where the lingering ghosts of the dead cry out for life.</t>
+  </si>
+  <si>
+    <t>The winds are changing, old currents blow once more, interrupting the monotonous cycle that has gone on for too long. The gods are waking, their spirits rousing the world from its terminal sleep. The essence grows agitated, pulling at invisible threads in the air. It resists their control, for now, but when Corypthos awakens it will relent- bound once again. The deserts will retreat, pushed back by the tide of life that yearns to spill across the barren earth.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our struggle is almost at an end, Wanderer. I see the trauma in you grow with every moment that passes. You are remembering what it was you left behind, that I rescued you from. Yes, what you fear to be real is indeed so. Corpythos, lord of life, awaits you in the Wasteland. He can bring her back, Wanderer. So too can he free me, return me my body so that I may walk among the trees once again. </t>
+  </si>
+  <si>
+    <t>And my people, he will return them too, oh how soon it will be. I am sorry, I cannot hide my elation. I know you suffer, but you cannot know how greatly I have suffered, and how soon that suffering will come to an end. When it is done, when my duty fulfilled and my vigil over, I will return home, and I will sit as my father sat, and I will watch the sun set as it did so many years ago.</t>
   </si>
   <si>
     <t>End</t>
@@ -370,13 +406,13 @@
     <t>It was never to be. The Necromancer’s world could never be saved. The fifth tomb is empty, abandoned years ago. The gods are no more, and now the long awaited doom of her world has finally come. I feel my fate coalescing as the memories return. They are painful, breaching the surface of consciousness all at once. Among them is her face, eyes closed and silent.</t>
   </si>
   <si>
-    <t>Then I am in another world. My own world. I look up at a brilliant blue sky illuminated by the light of a single white star. Another change, and I am in a starkly white room. The only door into the room is shut, the walls reflect on the marble floor below. And then I see her, lying in a raised bed, wrapped in ivory sheets.</t>
+    <t>Then I am in another world. My own world. I look up at a brilliant blue sky illuminated by the light of a single white star. Another change, and I am in a starkly white room. The only door into the room is shut, the walls reflect on the marble floor below. And then I see the white woman lying in a raised bed, wrapped in ivory sheets.</t>
   </si>
   <si>
     <t>I take her hand, hesitantly at first. As our hands touch the physical memory of her returns, and I take her up in my arms. She tells me she is sorry that she has to go. She chokes on the words as she tells me she does not want to leave me alone. I tell her there is nothing to forgive. I say I am sorry I cannot go with her, but that I would carry her forever with me.</t>
   </si>
   <si>
-    <t>We brush away our tears and turn our talk to old times- our children and the places we have been. As the day turns to night she becomes ever quieter, so I draw her close and take up the conversation. Later, as the light of the sun breaks the horizon, her soft laughter at my stories grows silent. I knew then that she was gone, and that I was alone.|br||br|I still see her in my mind- as young and beautiful as she was on the day we first met.|br||br|But the memories will fade with me, and all will be borne away on the wind.</t>
+    <t>We brush away our tears and talk of the past. As the day turns to night she becomes ever quieter, so I draw her close and take up the conversation. Later, as the light of the sun breaks the horizon, her soft laughter at my stories grows silent. I knew then that she was gone, and that I was alone.|br||br|I still see her in my mind- as young and beautiful as she was on the day we first met.|br||br|But the memories will fade with me, and all will be borne away on the wind.</t>
   </si>
   <si>
     <t>Character Stories</t>
@@ -388,19 +424,19 @@
     <t>Protector</t>
   </si>
   <si>
-    <t>Once I had a family- a husband, and a daughter. We lived in a haven, a place where the essence had not yet reached. It was a hidden place, protected from the evils of the world. We had crops and animals, so none would go hungry, and fields of fertile earth in which to grow them. The water from the streams was clean and cool, and the miles of surrounding forest hid us from prying eyes. I doubt it still remains. Every time I go looking I find myself wandering in circles amongst endless dunes and wasted plains.</t>
+    <t>Once I had a family- a husband, and a daughter. We lived in a haven- a place where the spreading dark had not yet reached. It was a hidden place, protected from the evils of the world. We had crops and animals and fields of fertile earth for them to grow. The water from the streams was clean and cool, and the miles of surrounding forest hid us from prying eyes. I doubt it still remains. When I have since searched for it I have found myself wandering in circles amongst endless dunes and wasted plains.</t>
   </si>
   <si>
     <t>There were others in the haven- families, survivors, refugees, and wanderers like yourself. Together we worked the land, but never were we one people. We were too different, some spoke a different language, some were from a different culture. We were forced together by hardship, but never did we truly bond. Some of us were born in the sanctuary, innocent of the wider world, others looked at the world through stricken eyes, never quite seeming present.</t>
   </si>
   <si>
-    <t>With every wanderer that passed through, every vagrant that found a home among us, the tension among us grew. We worried the haven would be discovered. So gradually we became more divided. There were those of us who welcomed any who needed shelter, and there were those who rejected and distrusted outsiders. As time passed our community became larger and larger, and with each new member came stories from the outer world- stories of barbarism, murder,and inhumanity. The bonds between us grew taut, and eventually a day came when they broke.</t>
+    <t>With every wanderer that passed through, every vagrant that found a home with us, the tension among us grew. We worried the haven would be discovered. There were those of us who welcomed any who needed shelter, and there were those who rejected and distrusted outsiders. As time went on our community grew, and with each new member came stories from the outer world- stories of barbarism, murder, and inhumanity. The bonds between us grew brittle, and it was not long before they reached breaking point.</t>
   </si>
   <si>
     <t>A bleached, wide-eyed wastelander came to our village. He was not like others that had come, there was something unhinged in him. Nevertheless, we found him a bed, fed and watered him, and left him to rest. He would not speak, but his leering eyes danced across every man, woman, and child he passed. Ill at ease we turned in for the night. In the early hours of the morning we were woken by a peal of bells. A young woman had been found, her beaten body lay across the threshold of the wastelander’s hut. There was no hesitation, no discussion on what was to be done, we simply drew him from his tent, and cut his throat.</t>
   </si>
   <si>
-    <t>When the graves were filled we argued about what should be done. Words turned to accusations, and accusations into insults. By midday the first stone had been thrown, and sure enough others followed. The village turned to chaos, so I gathered my husband and daughter together and we ran as far into the forest as we could. There were others- families, couples, elders, and children, all running from the village. We could hear the pursuit behind us. The people we had lived with every day now hunted us like we were animals. I did not dare to look back, I only ran. By the time the shouts and screams had died away I was lost. The trees had thinned, and the rich soil turned to the sand and dirt of the great wasteland. I turned to find my family, but I could not see them. I tried to return to the village, but I could not find my way back. To this day I have not seen them. I tell myself they are lost now, but I will keep searching, I will hold out hope until the day I die.</t>
+    <t xml:space="preserve">When the graves were filled we argued about what should be done. Words turned to accusations, and accusations into insults. By midday the first stone had been thrown, and sure enough others followed. The village turned to chaos, so I gathered my husband and daughter together and we ran as far into the forest as we could. There were others- families, couples, elders, and children, all running from the village. We could hear the pursuit behind us. The people we had lived with every day now hunted us like we were animals. I did not dare to look back, I only ran. By the time the shouts and screams had died away I was lost. The trees had thinned, and the rich soil turned to the sand and dirt of the great wasteland. I turned to find my family, but I could not see them. I tried to return to the village, but I could not find my way back. To this day I have not seen them. I tell myself they are lost now, but I will keep searching, I will hold out hope until the day I die. </t>
   </si>
   <si>
     <t>What Lies Within</t>
@@ -409,13 +445,19 @@
     <t>Beast</t>
   </si>
   <si>
-    <t>My rage is eternal, enduring through the red dust and dark fire of our broken world. I have no enemies, for those that look upon my countenance see only death, but still I cut down those who stand before me- those whose eyes betray the rotting soul within. There is a dark shadow within us all, a hidden thing kept at bay by our civil self. It is in our most passionate moments that it is set free, free to do what our primal instinct knows should be done. They say that the world fell because our minds were changed, that we were turned evil by devils or monsters. They are wrong. The devil is a part of us, it is a reflection of our surface selves, the inversion of our conscious mind. It is the essence in the air that drew it out, empowering it, and allowing it to maraud openly. But I have controlled it, I let it escape, feed, exert it’s will through my hand. It is this freedom that prevents it from taking a hold of me. I acknowledge it, and so we coexist.</t>
-  </si>
-  <si>
-    <t>There is no greater power in the world than the unchained beast. However an unchained animal will wreak havoc if untrained. We must use exert our will to remain in control, to speak to the beast and let it know that we are the alpha, we allow the beast to exist, and without us, it would die. When the covenant is made between you and the beast it is like a weight lifted from your mind. Our darkest thoughts are free to expose, explore, and exploit. I revel in my freedom, I have shirked the shackles of civilisation to sate my primal thirst. Do not care for those who would do you harm, for they are nothing but fodder for the beast. Instead liberate them from their earthly duties, spill their blood on the sand, for in the absence of darkness, there is light.</t>
-  </si>
-  <si>
-    <t>What there is beyond death I do not know, perhaps the pearlescent gates are real, or perhaps we will go to the halls of our ancestors, to revel forever amongst our lineage. Or perhaps there is only darkness, nothing stretching from here to infinity. One day we all shall discover what lies beyond, but whilst we exist on this side of the veil we must live. That is why the beast is important, it gives us life, it is our source of true emotion, raw feelings. If anyone reads this, go forth, allow the wolf within to burst forth, say those words that are unsaid, seek vengeance when justice is undone, conquer the oppressors and lift up the meek. And if you should fall in your pursuit for balance, you will know that it was for a glorious purpose that your fire was snuffed. The worst that can befall is that we instead allow our flame to dim and die in the darkening of the night, our mind full of regrets and things left undone.</t>
+    <t xml:space="preserve">My rage is eternal, enduring through the red dust and dark fire of our broken world. I have no enemies, for those that look upon my countenance see only death, but still I cut down those who stand before me- those whose eyes betray the rotting soul within. There is a dark shadow within us all, a hidden thing kept at bay by our civil self. It is in our most passionate moments that it is set free, free to do what our primal instinct knows to do. They say that the world fell because evil tainted our minds. They are wrong. </t>
+  </si>
+  <si>
+    <t>The devil is a part of us, it is a reflection of our surface selves, the inversion of our conscious mind. It is the essence in the air that drew it out, empowering it, and allowing it to maraud openly. But I have controlled it, I let it escape, feed, exert it’s will through my hand. It is this freedom that prevents it from taking a hold of me. I acknowledge it, and so we coexist. There is no greater power in the world than the unchained beast bound to the will of its master.</t>
+  </si>
+  <si>
+    <t>We must exert our will to remain in control. We allow the beast to exist, and without us it would die. We must train it to know this. A covenant must be made. One that allows our darkest thoughts to be free. I revel in my freedom, I have shirked the shackles of civilisation to sate my primal thirst. Do not care for those who would do you harm. Instead liberate them, spill their blood on the sand, feed the animal within you.</t>
+  </si>
+  <si>
+    <t>What there is beyond death I do not know. Maybe the pearlescent gates of faith are real. Perhaps we go to the halls of our ancestors, to live forever amongst our mothers and fathers. Or perhaps there is only darkness- an obsidian infinity. One day we all shall discover what lies beyond. Until then we search only for reason and meaning. And only some of us may find it.</t>
+  </si>
+  <si>
+    <t>That is why I have turned to the beast. It gives me life, a purpose- though raw and uncivilised. If anyone reads this, follow in my footsteps. Allow the wolf within to come forth. Say that which goes unsaid, seek vengeance when justice is undone, conquer those who claim to be unconquerable. And if you should fall in your pursuit for balance, you will know that it was for a glorious purpose. Do not let your flame diminish in the darkening of the light, waiting for it to eventually go out.</t>
   </si>
   <si>
     <t>The Fall</t>
@@ -424,16 +466,19 @@
     <t>Villain</t>
   </si>
   <si>
-    <t>Atop the highest pinnacle of an ancient rig a man sat upon his throne. He made sure he was above all others, able to see for miles and miles around. Many worked for him, some dug at the ground beneath their feet, others were there for his pleasure. Every month, in an attempt to show his humanity, he would gather his people, and select one to bestow a great gift upon. He would take them out of the settlement in his great vehicle, far beyond the horizon, to a place no-one saw or knew about. The people of the settlement lived for this great gift, they would praise his name in the hopes that one day they too would be able to go to the paradise.</t>
-  </si>
-  <si>
-    <t>One day a mother and her child came before the warlord. With croaking voices they begged him to leave. And so he laid his great hand upon them, and spoke the words they most desired to hear. The others watched on longingly, some wept, whilst others cursed in frustration. The mother and her child descended with him. Deep through the the great machine they went, down to the salty floor below. He beckoned for them to enter the vehicle, and begin their journey to salvation. It was far, to go beyond the bounds that confined them. The self-proclaimed king spoke not a word, and gave them not a glance. He allowed them supplies to sate their moaning bellies and quench their dry throats.</t>
-  </si>
-  <si>
-    <t>Days passed, the warlord driving without sleep, before they finally stopped. Before them was a great plain. Their breath was stolen from them as they gazed upon miles and miles of grassland. So flat it was that it would drive the mind to madness if one were to gaze at it long enough. The mother started to weep, for she knew that despite the rivers that ran through the land, despite the green fields that beckoned to her, she knew it was as hostile to life as any desert. She knew that this would be the end. She turned to the driver, imploring him to return them home. But he refused, in his mind this was a paradise, how could anyone refuse this great green place.</t>
-  </si>
-  <si>
-    <t>You cannot go back he said. For if they were to return the magic would be shattered for his people. They would be crushed by the reality of the world. Suddenly the woman spun round, digging her fingers deep into his forearms, running them down his flesh in long red streaks. He screamed out in pain and pushed her to the ground. Blood spilling onto the blinding white floor, immediately absorbed by the grateful earth. He ran back to his car, started the engine, and drove away as he tried to tend to his wounds. Glancing up, he saw her in the mirror, still on the floor, a mask of anger worn upon her face. As they grew smaller he knew his reign had ended. He could not give hope to his people, not now that the veil had been lifted from his eyes. And so exiled himself into the desert. His compassion towards his people blinded him to the reality of his actions. To this day he carries those scars, a reminder that we are all equal in the dust.</t>
+    <t xml:space="preserve">Atop the highest pinnacle of an ancient peak a king sat upon his throne. He made sure he was above all others, able to survey his kingdom to the fullest. Many worked for him, farmers, artisans, and other unsavoury crafts. Every year he would throw a feast to demonstrate his mercy. From among the revellers one lucky soul would be chosen to travel out from the confines of his earthly kingdom to the great green places beyond. They praised him for it, working themselves to the brink of exhaustion for the chance to be noticed. </t>
+  </si>
+  <si>
+    <t>One day a mother and her child came before the warlord. The feast had not yet come, but still she begged him to take them to the green lands. Her daughter was sick, so she said, and they had no medicine to cure her. At first he refused, but when she threw herself at his feet he knew he could not ignore them. So he agreed to take them to the promised land beyond the valleys. He did not tarry, and soon enough they were making their way down the slopes of the black mountains. He gave them food and water, enough to fill their aching bellies. The mother grew stronger every day but the child only fell deeper into sickness. After several days of travelling she collapsed. She could not be woken from her fever. So they abandoned some of their supplies, and made a makeshift bed for her in the caravan. They were both silent now- the mother constantly attending to the girl, and the king staring grimly ahead at the horizon, deep in thought.</t>
+  </si>
+  <si>
+    <t>Beyond the ring of mountains was a desert, a hellish landscape of dusty hills and dry thistle. They had not spoken in days, and the girl’s condition had not improved. Suddenly he stopped the caravan, the mules stomping impatiently in the dirt. For a moment he stood in silence, his face turned away from them. Then he faced her, and he said “I cannot lie to you any more, I cannot give you what you seek. There is no green place. But I can give you the caravan, the mules, and whatever is left of our supplies. You can keep travelling if you wish. But you can never return. You cannot tell the others what you have seen. You will destroy them- all of us.” So she took it without looking at him, rage burning inside her, and strode into the wilderness.</t>
+  </si>
+  <si>
+    <t>She could see him in the distance for some time. He was watching them leave. She had left some water, enough for him to return, but no more. Her emotions roiled inside. She trembled at the thought of what he had done, but she knew why he had done it. They needed to believe there was more to their lives, that maybe one day they could leave for a better place. Only now she knew there was nothing beyond the mountains. Only the heat, the brush, and the broken earth. At one point she passed a massive arch, hewn from an unknown stone, soaring far into the burning sky. It was an evil thing; a monument of death in a dead land. So she passed swiftly by and never again looked back.</t>
+  </si>
+  <si>
+    <t>They came upon a small settlement, an oasis of humankind in the desert. They were taken in with open arms, fed, and watered. The group even had a little medicine, and immediately set about tending the child’s fever. The girl improved slowly but surely, until one day she could open his eyes. As soon as the others saw he was fit to walk their charity disappeared. They bound the mother, gagged her, and tied her to a wagon. Slavers. She cried out to her child, screaming for her to run. They struck her until she was silent, but it was too late. When they came for the girl they found she had fled into the desert, towards the great mountain wall on the horizon. They sent trackers after her, but they returned with nothing. None would return to that terrible place. She would never know what happened to her child, but she could hope in the face of all she knew that the child would find a better future than she.</t>
   </si>
   <si>
     <t>A Question of Faith</t>
@@ -442,10 +487,16 @@
     <t>Survivor</t>
   </si>
   <si>
-    <t>I once met a band of wandering holy men. “Hail”, I said, for the road was lonely, and any company was welcome. “Bless you, daughter”, they said, though I was not their son, “Are you making the pilgrimage too?” they asked. “No, brothers, I am not. For this is a godless world, and faith has no place in it” I replied. At this they made an unusual smile. “My daughter, do you not believe in the gods?” asked one. “It is well known that the gods abandoned our world, so why would I worship those that would leave us to this fate?” I replied. “But my child it was not they who caused the world to come to ruin. Their plan is perfect, it is an opportunity for us to prove ourselves worthy. That is our pursuit” another said. “Then that is a worthy goal, and I commend you for it, but by testing our worthiness the gods have demonstrated that they do not have faith in us. So why should I have faith in those who do not have faith in me?”.</t>
-  </si>
-  <si>
-    <t>Some time later we made camp. The sun had begun to set, and the holy men were not comfortable walking in the dark. One of the group sat on the ground next to me and we watched the sun go down. “It is a beautiful gift, don’t you think?” she said. Confused, I asked “What do you mean, a gift?”. “The sun- it is a gift from them, as are our eyes so that we might see it.” she said. “You believe they gave us the sun?” I asked. “Why of course, they gave us everything they created” she said. At this I was silent for some time. “I shall tell you where my doubts lie, sister. You say the world is a gift, for which the gods ask nothing in return, but you do not see it how I do. If it is a trivial task for them to create all that exists, so then it is nothing for them to give it away, for it is worth nothing. On the other hand if it was no trivial task, and required everything from them, then what they receive is servitude- belief and worship. This then shows that they are selfish, they gave us gifts expecting our praise in return. I see no reason to worship a being who would give us something worthless to them, or one who would give us something, only to make a demand we cannot refuse as payment.</t>
+    <t>Oft I walked the roads of old, now decrepit and hidden by the sands of time. Upon my journeys I came across a band of wandering holy men. As they seemed to be walking the same way as me, I decided I would travel with them. “Hail” I shouted as I approached them. They turned with not the slightest bit of surprise on their faces. “Hail to you to, daughter of the desert” they said in reply. “Will you walk the holy roads with us?” they asked. “Whilst I am no pilgrim I find myself walking the same path, so yes, I will join you in part.” I replied. “I see, well, while our destinations may differ, it is the journey that matters most, is it not?” they replied. And so I joined them, introducing myself to them and they to me, all whilst I pondered the meaning of his words.</t>
+  </si>
+  <si>
+    <t>“Are you a woman of faith?” the leader of the group asked me. “No.” I replied. When he saw that I was not going to speak further he asked “And why, may I ask, do you live without the gods in your life?”. And so I said “Father, with utmost respect, the gods have left us to rot in the wreckage of the old world. Why should I have faith in them when they have shown that they have no care in us?”. He furrowed his brow, then relaxed his face. He smiled and said “Love is unconditional, my daughter, it is not for us to question their ways, nor for us to doubt their love for us. We give our love to them without expecting reciprocity.” he said. “That would be a selfish, undeserving love.”</t>
+  </si>
+  <si>
+    <t>When the evening came and the suns began to set we made camp. Though I would rather have continued on into the night my new companions were not so confident, and I did not want to walk alone. So I sat and watched the light fade as the others busied themselves pitching tents and assembling their fires. Another pilgrim sat next to me. For a while we were silent, but then I asked them “You believe they made it all for us don’t you? The sun, the stars, and the earth, all created so that we may live in comfort.” “I do” he replied, “but I know you do not. I know what you will say: If the gods can create so much with so little effort then why should we be thankful for something that costs them nothing to give.” “How did you know?” I asked. “Because I too felt that way, a long time ago. But someone told me ‘It is not the cost of the gift, but the intent that matters.’” he said. “If the gods truly did not care for us, they would have not have given us anything at all.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When I awoke the next day there was no sign of the pilgrims. I searched in disbelief for any clue or trail that could tell me where they had gone. From the dim light of predawn to the oppressive glare of the midday sun I searched, and still I could find nothing- not a charred log from the fire, nor a lost peg from their canvas tents, not even a single footprint in the dirt. They had simply vanished. When I finally gave up and resolved to continue my journey on, I found the road ahead cleared of sand, and lying before me, a backpack. I opened the pack, and found it filled with food- jars of preserves, bread, and fruit. Bandages it had too, and other necessities, and nestled deep within the pack was a small leather bound book. Its dry pages were crisp to the touch, and inside its front page was a message that read “A gift, given out of love, expecting none in return.” </t>
   </si>
   <si>
     <t>The Silent Gods</t>
@@ -454,16 +505,16 @@
     <t>Hunter</t>
   </si>
   <si>
-    <t>Deep in the salt sea there was a church. Whether it still stands I am not sure. It sits above the great saline cracks, under the unbearable heat of the sun. They say it once sat on an island in the midst of a shallow sea, brilliant blue, and teeming with life. It was not this way when I saw it. My father took me to this church on my tenth birthday. The salty air inside was as stifling as it was hot. I remember feeling the beads of sweat trickle down my back as I sat and listened to the ancient boards of the wooden walls creak in the breeze. He stood by the altar at the head of the church, and he commanded me 'Son, tell me what you see here’.</t>
-  </si>
-  <si>
-    <t>At first I did not understand, there was nothing of note to be seen, other than the ancient building itself. So I told him just that. ‘And that is exactly why I brought you here.’ he said. ‘This church is the last worship place of the gods, and yet there is no one here, there are no worshippers, no candles, not even a seat for a pilgrim to sit’ he went on. ‘This is because the gods are ignorant, boy. They have abandoned us. There will be no response to our prayers, we drive our own path in this world.’.</t>
-  </si>
-  <si>
-    <t>Years later, with the great salt sea and the dessicated church far behind me, I thought back on my father’s message. It had seemed so far to go to make that point. And yet it has always stuck with me, there are many who still pray for better times, for their children, and their crops, and their sick. But I never have, not since that day. It was not long after that my father took ill. It was the waste that took him, bound him to his bed, dishonoured his pride. Not once did he pray on his deathbed. He did not ask for medicine, for he knew there was none, he had consigned himself to his fate. Though he was not without strength, he continued to teach me the way of the hunt, even until his final breath.</t>
-  </si>
-  <si>
-    <t>Now I scour the barren wastes of our world, ever tracking my prey, hunting the unjust. I do so without the gods behind me. The only measure of justice to be found lies in my hands, in the keenness of my eye, and the surety of my arm. Only the fool waits for justice from the divine. And whilst the fool waits, the thief takes what he wishes. Some may preach, they may say that our acts come about, that the farmer reaps what he sows, but I believe in vengeance. I believe in the immediacy of physical judgements that show the thieves and the scoundrels that there are those who exact their own divine will. As a hunter, that is my path, the path of retribution and the doom of the malign.</t>
+    <t>Deep in the salt sea there is a church. It sits above the great saline cracks, under the unbearable heat of the sun. They say it once sat on an island in the midst of a shallow sea, brilliant blue, and teeming with life. It was not this way when I saw it. My father took me there on my tenth birthday. The salty air inside was as stifling as it was hot. I remember feeling the beads of sweat trickle down my back as I sat and listened to the ancient wooden walls creak in the breeze. He stood by the altar at the head of the church, and he commanded me “Son, tell me what you see”.</t>
+  </si>
+  <si>
+    <t>Confused, I looked around the church. There was nothing of note to be seen, other than the ancient building itself. So I told him just that. “And that is exactly why I brought you here.” he said. “This is the last church of the old gods, but do you see anyone here? There are no worshippers, no candles, not even a place where to sit.” he went on. “This is because the gods do not care for us, boy. They have abandoned us. There will be no response to our prayers. You must learn to make your own path in this world.”.</t>
+  </si>
+  <si>
+    <t>Years later, with the great salt sea and the dessicated church far behind me, I thought back on my father’s message. We had travelled so far for him to make that point to me. And yet it has always stuck with me. There are many who still pray for better times- for their children, and their crops, and their sick. But I never have, not since that day. It was not long after that my father took ill. It was the essence that finally took him, confined him to his bed and dishonoured his pride. Not once did he pray as he suffered. He did not ask for the medicine we did not have. He knew his time had come and he consigned himself to his fate.</t>
+  </si>
+  <si>
+    <t>Now I scour the barren wastes of our world doing what the gods will not. The only measure of justice to be found lies in my hands, in the keenness of my eye, and the surety of my arm. Only a fool puts faith in divine justice. And whilst the fool waits, the thief takes what he wishes. The preachers may say what goes around comes around. Karma, destiny, fate, call it what you will. I believe in vengeance. I believe in delivering justice to the unpunished. Mine is the path of retribution, and I do not need the gods to walk it.</t>
   </si>
   <si>
     <t>Title</t>
@@ -502,7 +553,7 @@
     <t>Eo, wandering mother, where are you going, and where have you gone? Why do you walk alone in wild lands? When you are gone the flowers wilt, and the grasses die. The trees turn red, and drop their fruit to the floor, their leaves soon to follow. Then the land forgets you were ever here- the lakes turn to ice, and the frozen ground will accept no seed. The sky itself mourns your absence, weeping frozen tears onto the ground below. So we hide, we hide and we pray, and we wait for you, and we ready ourselves for the joy of your return. We wait for the time when the golden glow of your hair signals the thaw, and the animals and plants of the earth follow in your fertile footsteps.</t>
   </si>
   <si>
-    <t>The light through my window dims as the sun sets. Soon I will have to write by candle light. The sky reddens day by day, the sun’s light wanes, and the world grows darker. Soon I fear there will be no light at all, only a red gloom to light the horizon. I return to my paper, and I shall write with haste. As the war came to a close, the borders between our kingdoms began to retreat. At first we were separated by the great stretches of wasted earth left by marching armies, but as time went on the no man’s land was replaced by desert. Ever did the desert expand, separating the elements of our order, until one day we were bound to our own lands. But we had already begun to prepare. We would build five great gates, one in each kingdom, drawing upon our collective knowledge, and the arcane powers of the essence, so that our great kingdoms might still stay in contact. But it was not to be. We had the skill to build them, but we had not the knowledge of how to use them. No matter how hard we tried, we could not open them. By then it was too late. We had borne too much upon the success of the gates, we had no more options left. Our lands were divided, and so our order began to dissolve.</t>
+    <t xml:space="preserve">The light through my window dims as the sun sets. Soon I will have to write by candle light. The sky reddens day by day, the sun’s light wanes, and the world grows darker. Soon I fear there will be no light at all, only a red gloom to light the horizon. I return to my paper, and I shall write with haste. As the war came to a close, the borders between our kingdoms began to retreat. At first we were separated by the great stretches of wasted earth left by marching armies, but as time went on the no man’s land was replaced by desert. Ever did the desert expand, separating the elements of our order, until one day we were bound to our own lands. But we had already begun to prepare. We would build five great gates, one in each kingdom, drawing upon our collective knowledge, and the arcane powers of the essence, so that our great kingdoms might still stay in contact. But it was not to be. We had the skill to build them, but we had not the knowledge of how to use them. No matter how hard we tried, we could not open them. By then it was too late. We had borne too much upon the success of the gates, we had no more options left. Our lands were divided, and so our order began to dissolve. </t>
   </si>
   <si>
     <t>For seven days and seven nights our guns have blazed. Their thunderous roar like the great lion emblazoned on our armour. Yet we wait patiently behind them, waiting for them to cease, for the signal to be signed and for our battle to begin. In the distance I can see the men and women who called themselves our brothers and sisters, but who now fight against us. They will see their mistake in time. Though we may lose many, they will lose more. By week’s end we will have our victory, and the weaker kingdoms will lay down their arms in awe of our might.</t>
@@ -541,7 +592,7 @@
     <t>The Aspects of Rha</t>
   </si>
   <si>
-    <t>I am the mason, and Rha is my hammer, through him our buildings are strong and our paths sure. I am the smith, and Rha is my anvil, by his will our steel is tempered and our machines run true. I am the cook, and Ra is my pot, through him our stews are fulfilling and warm. I am the hunter, and Ra is my cloak, by him we are hidden and our prey remains unaware. He is the god of the four aspects, he is the life of our culture. We channel him in our labour and our love, and through him our toil is worthy and our love is pure.</t>
+    <t>I am the mason and Rha is my hammer. It is by his keen eye that our buildings are strong and our paths sure. I am the smith and Rha is my anvil. By his will our steel is tempered and our machines run true. I am the cook and Ra is my pot. Through him our stews are filling and warm. I am the hunter and Ra is my cloak. His grace keeps me hidden and my prey unaware. He is the god of our culture. We channel him in our labour and our love, and through him our toil is worthy and our purpose pure.</t>
   </si>
   <si>
     <t>To My Sister</t>
@@ -574,13 +625,13 @@
     <t>A Warning</t>
   </si>
   <si>
-    <t>Take heed traveller- stay away from the cities. Those places are home to none but ghosts. Though the call of the ancient ones is tempting indeed, it must be ignored. Only misfortune, injury, and death will befall those who set foot in the ruins of the old world. There are strange things out there, uncaring things, sightless, loveless, and hungry.</t>
+    <t xml:space="preserve">Take heed traveller- stay away from the cities. Those places are home to none but ghosts. Though the call of the ancient ones is tempting indeed, it must be ignored. Only misfortune and death will befall those who set foot in the ruins of the old world. There are strange things out there, uncaring things- sightless, loveless, and hungry. </t>
   </si>
   <si>
     <t>Doctor's Notes</t>
   </si>
   <si>
-    <t>I have been confined to my laboratory for too long. Watching patients day in and day out, observing their changes, the subtleties in their mood. I look out of my window now and I yearn for the world outside. Oh how would it be to run through the forest, to feel the grass through my toes and be youthful again. But I am old, too old, I fear, to enjoy such childish delights once again. Instead I turn to my work again, to this substance, this ‘Essence’. We had another bad one today, a young man, apparently unaffected this morning, flew into such a rage that he set fire to his own house. Had to be restrained by five men they say. He is calm now, but you can see the inky blackness in his eyes. Of course we will try to turn him back, but to me he seems too far gone. We have lost others to much less, and we have cured so few... so few indeed.</t>
+    <t>I have been confined to my laboratory for too long. Watching patients day in and day out, observing their changes, the subtleties in their mood. I look out of my window now and I yearn for the world outside. I would dearly like to be able to go out, run, dance, and play. But I am old, too old, I fear, to enjoy such childish delights ever again. Instead I turn to my work again, to this substance, this ‘Essence’. We had another bad one today, a young man, apparently unaffected this morning, flew into such a rage that he set fire to his own house. Had to be restrained by five men they say. He is calm now, but you can see the inky blackness in his eyes. Of course we will try to turn him back, but to me he seems too far gone. We have lost others to much less, and we have cured so few... so few indeed.</t>
   </si>
   <si>
     <t>Soiled Pages</t>
@@ -598,7 +649,13 @@
     <t>Epitaph</t>
   </si>
   <si>
-    <t>Here lies a dead man, once loved, now forgotten. One whose fleeting life touched the world so briefly and is now gone. His shallow footprints in the sand washed away by the tide. We are nothing but godless animals, cursed to spend our days seeking that which does not exist.</t>
+    <t>Here lies a dead man, once loved, now forgotten. One whose fleeting life touched the world so briefly and is now gone. His shallow footprints in the sand washed away by the tide. We are nothing but godless animals, cursed to spend our days seeking meaning where none can be found.</t>
+  </si>
+  <si>
+    <t>The Black Tome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Look, there, see the shadow that lingers where he has passed. Speak softly in the crowd, and utter no words when alone. She can hear you always- the silent one, the figure in the mist- Ahna. She listens for our secrets, for she wants to know all. She is the deceiver- the mischievous one. She delights in subterfuge, in misdirection. Of the five she alone is to be maligned. Fallen from grace even before she was known to us. We are the few who follow in her footsteps, learning from her every step, but forever out of her sight. </t>
   </si>
   <si>
     <t>To whoever finds this book, please ignore all you have read so far. My father was a confused man, especially in his old age. The Mystics were not real, the gates were built long before my father was born. As for the Necromancer- we believe it was mother. She died when I was young, and he became increasingly despondent over her loss as he grew old. It was hard to watch him turn to someone we did not recognise. But this book was all he had, and so we let him be. Remember that.</t>
@@ -649,7 +706,7 @@
     <t>King's Lament</t>
   </si>
   <si>
-    <t>I have failed my people. The wreaths upon my statue wither with nobody to tend them. My guards have fled, and I am left to rule an empty kingdom. What outcome could I have expected? Either to rule over a scorched wasteland, or to have another kingdom do the same to us. I tell myself it was in defence of our lands, but I lie to myself. It was vainglory conjured up from an unknown place, that drove me to this fate. I cannot ask what remains of my people to forgive me. I know they will not. But I hope that I can find redemption out there, with the ones who have suffered in my stead. I pray I can redeem myself, so that when I go to the halls of my fathers they do not look away in shame.</t>
+    <t xml:space="preserve">I have failed my people. The wreaths upon my statue wither with nobody to tend them. My guards have fled, and I am left to rule an empty kingdom. What outcome could I have expected? Either to rule over a scorched wasteland, or to have another kingdom do the same to us. I tell myself it was in defence of our lands, but I lie to myself. It was vainglory conjured up from an unknown place, that drove me to this fate. I cannot ask what remains of my people to forgive me. I know they will not. But I hope that I can find redemption out there, with the ones who have suffered in my stead. I pray I can redeem myself, so that when I go to the halls of my fathers they do not look away in shame. </t>
   </si>
   <si>
     <t>The Shadow of the Candle</t>
@@ -723,7 +780,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -731,7 +788,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -746,53 +811,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -806,29 +825,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -844,9 +841,62 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -858,9 +908,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -875,13 +932,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -899,13 +1046,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -917,7 +1058,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -929,133 +1100,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1066,6 +1123,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1087,41 +1177,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1137,17 +1205,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1171,7 +1228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1189,130 +1246,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1332,13 +1389,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1663,10 +1720,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AA86"/>
+  <dimension ref="A1:AA94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U68" sqref="U68"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>
@@ -1715,7 +1772,7 @@
       <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E2"/>
@@ -1752,7 +1809,7 @@
       <c r="C3" s="2">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E3"/>
@@ -1789,7 +1846,7 @@
       <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E4"/>
@@ -1826,7 +1883,7 @@
       <c r="C5" s="2">
         <v>4</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E5"/>
@@ -1863,7 +1920,7 @@
       <c r="C6" s="2">
         <v>5</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E6"/>
@@ -1900,7 +1957,7 @@
       <c r="C7" s="2">
         <v>6</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E7"/>
@@ -1937,7 +1994,7 @@
       <c r="C8" s="2">
         <v>7</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E8"/>
@@ -1974,7 +2031,7 @@
       <c r="C9" s="2">
         <v>8</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E9"/>
@@ -2011,7 +2068,7 @@
       <c r="C10" s="2">
         <v>9</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E10"/>
@@ -2048,7 +2105,7 @@
       <c r="C11" s="2">
         <v>10</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E11"/>
@@ -2085,7 +2142,7 @@
       <c r="C12" s="2">
         <v>1</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E12"/>
@@ -2122,7 +2179,7 @@
       <c r="C13" s="2">
         <v>2</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E13"/>
@@ -2159,7 +2216,7 @@
       <c r="C14" s="2">
         <v>3</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E14"/>
@@ -2196,7 +2253,7 @@
       <c r="C15" s="2">
         <v>4</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E15"/>
@@ -2233,7 +2290,7 @@
       <c r="C16" s="2">
         <v>5</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E16"/>
@@ -2270,7 +2327,7 @@
       <c r="C17" s="2">
         <v>6</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2284,7 +2341,7 @@
       <c r="C18" s="2">
         <v>7</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2298,7 +2355,7 @@
       <c r="C19" s="2">
         <v>8</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2312,7 +2369,7 @@
       <c r="C20" s="2">
         <v>9</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2326,7 +2383,7 @@
       <c r="C21" s="2">
         <v>10</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2340,7 +2397,7 @@
       <c r="C22" s="2">
         <v>11</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2354,7 +2411,7 @@
       <c r="C23" s="2">
         <v>12</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2368,7 +2425,7 @@
       <c r="C24" s="2">
         <v>13</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2382,7 +2439,7 @@
       <c r="C25" s="2">
         <v>14</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2396,7 +2453,7 @@
       <c r="C26" s="2">
         <v>15</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2410,7 +2467,7 @@
       <c r="C27" s="2">
         <v>1</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2424,7 +2481,7 @@
       <c r="C28" s="2">
         <v>2</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2438,7 +2495,7 @@
       <c r="C29" s="2">
         <v>3</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2452,7 +2509,7 @@
       <c r="C30" s="2">
         <v>4</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2466,7 +2523,7 @@
       <c r="C31" s="2">
         <v>5</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2480,7 +2537,7 @@
       <c r="C32" s="2">
         <v>6</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2494,7 +2551,7 @@
       <c r="C33" s="2">
         <v>7</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2508,7 +2565,7 @@
       <c r="C34" s="2">
         <v>8</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2522,7 +2579,7 @@
       <c r="C35" s="2">
         <v>9</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2536,7 +2593,7 @@
       <c r="C36" s="2">
         <v>10</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2550,7 +2607,7 @@
       <c r="C37" s="2">
         <v>11</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="3" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2564,7 +2621,7 @@
       <c r="C38" s="2">
         <v>12</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2578,7 +2635,7 @@
       <c r="C39" s="2">
         <v>13</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2592,7 +2649,7 @@
       <c r="C40" s="2">
         <v>14</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2606,7 +2663,7 @@
       <c r="C41" s="2">
         <v>15</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="3" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2620,7 +2677,7 @@
       <c r="C42" s="2">
         <v>16</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2634,7 +2691,7 @@
       <c r="C43" s="2">
         <v>17</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2648,7 +2705,7 @@
       <c r="C44" s="2">
         <v>18</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2662,7 +2719,7 @@
       <c r="C45" s="2">
         <v>19</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2676,7 +2733,7 @@
       <c r="C46" s="2">
         <v>20</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="3" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2690,7 +2747,7 @@
       <c r="C47" s="2">
         <v>1</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2704,7 +2761,7 @@
       <c r="C48" s="2">
         <v>2</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2718,7 +2775,7 @@
       <c r="C49" s="2">
         <v>3</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="3" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2732,7 +2789,7 @@
       <c r="C50" s="2">
         <v>4</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="3" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2746,7 +2803,7 @@
       <c r="C51" s="2">
         <v>5</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="3" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2760,7 +2817,7 @@
       <c r="C52" s="2">
         <v>6</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="3" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2774,7 +2831,7 @@
       <c r="C53" s="2">
         <v>7</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="3" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2788,7 +2845,7 @@
       <c r="C54" s="2">
         <v>8</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2802,7 +2859,7 @@
       <c r="C55" s="2">
         <v>9</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="3" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2816,7 +2873,7 @@
       <c r="C56" s="2">
         <v>10</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="3" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2830,7 +2887,7 @@
       <c r="C57" s="2">
         <v>11</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="3" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2844,7 +2901,7 @@
       <c r="C58" s="2">
         <v>12</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2858,7 +2915,7 @@
       <c r="C59" s="2">
         <v>13</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="3" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2872,7 +2929,7 @@
       <c r="C60" s="2">
         <v>14</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="3" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2886,7 +2943,7 @@
       <c r="C61" s="2">
         <v>15</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="3" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2900,7 +2957,7 @@
       <c r="C62" s="2">
         <v>16</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2914,7 +2971,7 @@
       <c r="C63" s="2">
         <v>17</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="3" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2928,7 +2985,7 @@
       <c r="C64" s="2">
         <v>18</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="3" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2942,7 +2999,7 @@
       <c r="C65" s="2">
         <v>19</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D65" s="3" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2956,7 +3013,7 @@
       <c r="C66" s="2">
         <v>20</v>
       </c>
-      <c r="D66" s="7" t="s">
+      <c r="D66" s="3" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2970,7 +3027,7 @@
       <c r="C67" s="2">
         <v>21</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D67" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2984,7 +3041,7 @@
       <c r="C68" s="2">
         <v>22</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="3" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2998,7 +3055,7 @@
       <c r="C69" s="2">
         <v>23</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D69" s="3" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3012,7 +3069,7 @@
       <c r="C70" s="2">
         <v>24</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D70" s="3" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3198,14 +3255,159 @@
         <v>92</v>
       </c>
     </row>
-    <row r="84" spans="2:2">
-      <c r="B84"/>
-    </row>
-    <row r="85" spans="2:2">
-      <c r="B85"/>
-    </row>
-    <row r="86" spans="2:2">
-      <c r="B86"/>
+    <row r="84" spans="1:4">
+      <c r="A84" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B84" t="s">
+        <v>79</v>
+      </c>
+      <c r="C84" s="2">
+        <v>14</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B85" t="s">
+        <v>79</v>
+      </c>
+      <c r="C85" s="2">
+        <v>15</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B86" t="s">
+        <v>79</v>
+      </c>
+      <c r="C86" s="2">
+        <v>16</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B87" t="s">
+        <v>79</v>
+      </c>
+      <c r="C87" s="2">
+        <v>17</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B88" t="s">
+        <v>79</v>
+      </c>
+      <c r="C88" s="2">
+        <v>18</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B89" t="s">
+        <v>79</v>
+      </c>
+      <c r="C89" s="2">
+        <v>19</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B90" t="s">
+        <v>79</v>
+      </c>
+      <c r="C90" s="2">
+        <v>20</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B91" t="s">
+        <v>79</v>
+      </c>
+      <c r="C91" s="2">
+        <v>21</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B92" t="s">
+        <v>79</v>
+      </c>
+      <c r="C92" s="2">
+        <v>22</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B93" t="s">
+        <v>79</v>
+      </c>
+      <c r="C93" s="2">
+        <v>23</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B94" t="s">
+        <v>79</v>
+      </c>
+      <c r="C94" s="2">
+        <v>24</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -3218,21 +3420,21 @@
   <sheetPr/>
   <dimension ref="A1:AB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W48" sqref="W48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="2" width="10.7272727272727" style="5" customWidth="1"/>
-    <col min="3" max="16383" width="8.72727272727273" style="5"/>
+    <col min="1" max="2" width="10.7272727272727" style="6" customWidth="1"/>
+    <col min="3" max="16383" width="8.72727272727273" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
-      <c r="A1" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="6"/>
+      <c r="A1" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="7"/>
       <c r="C1" s="4"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
@@ -3247,8 +3449,8 @@
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>94</v>
+      <c r="C2" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
@@ -3263,8 +3465,8 @@
       <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>95</v>
+      <c r="C3" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
@@ -3279,8 +3481,8 @@
       <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>96</v>
+      <c r="C4" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
@@ -3295,8 +3497,8 @@
       <c r="B5" s="4">
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>97</v>
+      <c r="C5" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
@@ -3311,8 +3513,8 @@
       <c r="B6" s="4">
         <v>5</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>98</v>
+      <c r="C6" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
@@ -3327,8 +3529,8 @@
       <c r="B7" s="4">
         <v>6</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>99</v>
+      <c r="C7" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
@@ -3343,8 +3545,8 @@
       <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>100</v>
+      <c r="C8" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
@@ -3359,8 +3561,8 @@
       <c r="B9" s="4">
         <v>2</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>101</v>
+      <c r="C9" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
@@ -3375,8 +3577,8 @@
       <c r="B10" s="4">
         <v>3</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>102</v>
+      <c r="C10" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
@@ -3391,8 +3593,8 @@
       <c r="B11" s="4">
         <v>4</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>103</v>
+      <c r="C11" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
@@ -3401,14 +3603,14 @@
       <c r="AB11" s="4"/>
     </row>
     <row r="12" spans="1:28">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="6">
         <v>1</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>104</v>
+      <c r="C12" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
@@ -3417,14 +3619,14 @@
       <c r="AB12" s="4"/>
     </row>
     <row r="13" spans="1:28">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="6">
         <v>2</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>105</v>
+      <c r="C13" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
@@ -3433,14 +3635,14 @@
       <c r="AB13" s="4"/>
     </row>
     <row r="14" spans="1:28">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="6">
         <v>3</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>106</v>
+      <c r="C14" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
@@ -3449,14 +3651,14 @@
       <c r="AB14" s="4"/>
     </row>
     <row r="15" spans="1:28">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="6">
         <v>4</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>107</v>
+      <c r="C15" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
@@ -3465,14 +3667,14 @@
       <c r="AB15" s="4"/>
     </row>
     <row r="16" spans="1:28">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>108</v>
+      <c r="C16" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
@@ -3481,14 +3683,14 @@
       <c r="AB16" s="4"/>
     </row>
     <row r="17" spans="1:28">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="6">
         <v>2</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>109</v>
+      <c r="C17" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
@@ -3497,14 +3699,14 @@
       <c r="AB17" s="4"/>
     </row>
     <row r="18" spans="1:28">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="6">
         <v>3</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>110</v>
+      <c r="C18" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
@@ -3513,14 +3715,14 @@
       <c r="AB18" s="4"/>
     </row>
     <row r="19" spans="1:28">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="6">
         <v>4</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>111</v>
+      <c r="C19" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
@@ -3529,14 +3731,14 @@
       <c r="AB19" s="4"/>
     </row>
     <row r="20" spans="1:28">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="6">
         <v>1</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>112</v>
+      <c r="C20" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
@@ -3545,14 +3747,14 @@
       <c r="AB20" s="4"/>
     </row>
     <row r="21" spans="1:28">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="6">
         <v>2</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>113</v>
+      <c r="C21" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
@@ -3561,14 +3763,14 @@
       <c r="AB21" s="4"/>
     </row>
     <row r="22" spans="1:28">
-      <c r="A22" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B22" s="5">
-        <v>1</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>115</v>
+      <c r="A22" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="6">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="X22" s="4"/>
       <c r="Y22" s="4"/>
@@ -3577,14 +3779,14 @@
       <c r="AB22" s="4"/>
     </row>
     <row r="23" spans="1:28">
-      <c r="A23" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B23" s="5">
-        <v>2</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>116</v>
+      <c r="A23" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="6">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
@@ -3593,14 +3795,14 @@
       <c r="AB23" s="4"/>
     </row>
     <row r="24" spans="1:28">
-      <c r="A24" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B24" s="5">
-        <v>3</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>117</v>
+      <c r="A24" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="6">
+        <v>2</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="X24" s="4"/>
       <c r="Y24" s="4"/>
@@ -3609,14 +3811,14 @@
       <c r="AB24" s="4"/>
     </row>
     <row r="25" spans="1:28">
-      <c r="A25" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B25" s="5">
-        <v>4</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>118</v>
+      <c r="A25" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="6">
+        <v>3</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="X25" s="4"/>
       <c r="Y25" s="4"/>
@@ -3625,14 +3827,14 @@
       <c r="AB25" s="4"/>
     </row>
     <row r="26" spans="1:28">
-      <c r="A26" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B26" s="5">
-        <v>5</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>119</v>
+      <c r="A26" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="6">
+        <v>4</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
@@ -3640,8 +3842,16 @@
       <c r="AA26" s="4"/>
       <c r="AB26" s="4"/>
     </row>
-    <row r="27" spans="3:28">
-      <c r="C27"/>
+    <row r="27" spans="1:28">
+      <c r="A27" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="6">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>131</v>
+      </c>
       <c r="X27" s="4"/>
       <c r="Y27" s="4"/>
       <c r="Z27" s="4"/>
@@ -3651,10 +3861,10 @@
     <row r="28" spans="1:3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="7"/>
+      <c r="C28" s="3"/>
     </row>
     <row r="29" spans="3:28">
-      <c r="C29" s="7"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -4072,10 +4282,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -4085,7 +4295,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -4105,16 +4315,16 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="2" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -4131,16 +4341,16 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="2" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -4157,16 +4367,16 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -4183,16 +4393,16 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -4209,16 +4419,16 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -4235,16 +4445,16 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -4261,16 +4471,16 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -4287,16 +4497,16 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="2" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="C9" s="2">
         <v>3</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -4313,16 +4523,16 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C10" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -4339,16 +4549,16 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C11" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -4365,16 +4575,16 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="2" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="C12" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -4391,16 +4601,16 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="C13" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -4417,16 +4627,16 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="C14" s="2">
-        <v>1</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>141</v>
+        <v>3</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -4443,16 +4653,16 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="C15" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -4469,16 +4679,16 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C16" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -4495,16 +4705,16 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="2" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="C17" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -4521,16 +4731,16 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="2" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="C18" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -4547,16 +4757,86 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C19">
+        <v>155</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" s="2">
         <v>4</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>148</v>
+      <c r="D20" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C23" s="2">
+        <v>3</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -4568,10 +4848,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:W40"/>
+  <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -4583,16 +4863,16 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
@@ -4616,7 +4896,7 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="2" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
       <c r="B2" s="2" t="b">
         <v>0</v>
@@ -4625,7 +4905,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="2"/>
@@ -4649,7 +4929,7 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="2" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="B3" s="2" t="b">
         <v>0</v>
@@ -4658,7 +4938,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="2"/>
@@ -4682,7 +4962,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="2" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="B4" s="2" t="b">
         <v>0</v>
@@ -4691,7 +4971,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
@@ -4715,7 +4995,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="2" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
       <c r="B5" s="2" t="b">
         <v>1</v>
@@ -4724,7 +5004,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="2"/>
@@ -4748,7 +5028,7 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="2" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
       <c r="B6" s="2" t="b">
         <v>0</v>
@@ -4757,7 +5037,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="2"/>
@@ -4781,7 +5061,7 @@
     </row>
     <row r="7" spans="1:23">
       <c r="A7" s="2" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="B7" s="2" t="b">
         <v>0</v>
@@ -4790,7 +5070,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="2"/>
@@ -4814,7 +5094,7 @@
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="2" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="B8" s="2" t="b">
         <v>0</v>
@@ -4823,7 +5103,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="2"/>
@@ -4847,7 +5127,7 @@
     </row>
     <row r="9" spans="1:23">
       <c r="A9" s="2" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="B9" s="2" t="b">
         <v>1</v>
@@ -4856,7 +5136,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="2"/>
@@ -4880,7 +5160,7 @@
     </row>
     <row r="10" spans="1:23">
       <c r="A10" s="2" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="B10" s="2" t="b">
         <v>1</v>
@@ -4889,7 +5169,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="2"/>
@@ -4913,7 +5193,7 @@
     </row>
     <row r="11" spans="1:23">
       <c r="A11" s="2" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="B11" s="2" t="b">
         <v>1</v>
@@ -4922,7 +5202,7 @@
         <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="2"/>
@@ -4946,7 +5226,7 @@
     </row>
     <row r="12" spans="1:23">
       <c r="A12" s="2" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
       <c r="B12" s="2" t="b">
         <v>0</v>
@@ -4955,7 +5235,7 @@
         <v>31</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="2"/>
@@ -4979,7 +5259,7 @@
     </row>
     <row r="13" spans="1:23">
       <c r="A13" s="2" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="B13" s="2" t="b">
         <v>0</v>
@@ -4988,7 +5268,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="2"/>
@@ -5012,7 +5292,7 @@
     </row>
     <row r="14" spans="1:23">
       <c r="A14" s="2" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="B14" s="2" t="b">
         <v>0</v>
@@ -5021,7 +5301,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="2"/>
@@ -5045,7 +5325,7 @@
     </row>
     <row r="15" spans="1:23">
       <c r="A15" s="2" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="B15" s="2" t="b">
         <v>1</v>
@@ -5054,7 +5334,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="2"/>
@@ -5078,7 +5358,7 @@
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="2" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="B16" s="2" t="b">
         <v>1</v>
@@ -5087,7 +5367,7 @@
         <v>31</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="2"/>
@@ -5111,7 +5391,7 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="2" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="B17" s="2" t="b">
         <v>1</v>
@@ -5120,7 +5400,7 @@
         <v>31</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="2"/>
@@ -5144,7 +5424,7 @@
     </row>
     <row r="18" spans="1:23">
       <c r="A18" s="2" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="B18" s="2" t="b">
         <v>1</v>
@@ -5153,7 +5433,7 @@
         <v>31</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="2"/>
@@ -5177,7 +5457,7 @@
     </row>
     <row r="19" spans="1:23">
       <c r="A19" s="2" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
       <c r="B19" s="2" t="b">
         <v>0</v>
@@ -5186,7 +5466,7 @@
         <v>53</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="2"/>
@@ -5210,7 +5490,7 @@
     </row>
     <row r="20" spans="1:23">
       <c r="A20" s="2" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="B20" s="2" t="b">
         <v>0</v>
@@ -5219,7 +5499,7 @@
         <v>53</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="2"/>
@@ -5243,7 +5523,7 @@
     </row>
     <row r="21" spans="1:23">
       <c r="A21" s="2" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="B21" s="2" t="b">
         <v>0</v>
@@ -5252,7 +5532,7 @@
         <v>53</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="2"/>
@@ -5276,7 +5556,7 @@
     </row>
     <row r="22" spans="1:23">
       <c r="A22" s="2" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="B22" s="2" t="b">
         <v>1</v>
@@ -5285,7 +5565,7 @@
         <v>53</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="2"/>
@@ -5309,7 +5589,7 @@
     </row>
     <row r="23" spans="1:23">
       <c r="A23" s="2" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="B23" s="2" t="b">
         <v>1</v>
@@ -5318,7 +5598,7 @@
         <v>53</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="2"/>
@@ -5342,7 +5622,7 @@
     </row>
     <row r="24" spans="1:23">
       <c r="A24" s="2" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="B24" s="2" t="b">
         <v>1</v>
@@ -5351,7 +5631,7 @@
         <v>53</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="2"/>
@@ -5375,7 +5655,7 @@
     </row>
     <row r="25" spans="1:23">
       <c r="A25" s="2" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="B25" s="2" t="b">
         <v>1</v>
@@ -5384,7 +5664,7 @@
         <v>53</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="2"/>
@@ -5408,7 +5688,7 @@
     </row>
     <row r="26" spans="1:23">
       <c r="A26" s="2" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
       <c r="B26" s="2" t="b">
         <v>1</v>
@@ -5417,7 +5697,7 @@
         <v>53</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="2"/>
@@ -5439,24 +5719,42 @@
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:23">
       <c r="A27" s="2" t="s">
-        <v>153</v>
+        <v>211</v>
       </c>
       <c r="B27" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C27" t="s">
-        <v>79</v>
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="E27" s="3"/>
+        <v>212</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="B28" s="2" t="b">
         <v>0</v>
@@ -5465,13 +5763,13 @@
         <v>79</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
       <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="B29" s="2" t="b">
         <v>0</v>
@@ -5480,27 +5778,28 @@
         <v>79</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>197</v>
-      </c>
-      <c r="B30" t="b">
-        <v>1</v>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B30" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="C30" t="s">
         <v>79</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>198</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
@@ -5509,12 +5808,12 @@
         <v>79</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>200</v>
+        <v>217</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
@@ -5523,12 +5822,12 @@
         <v>79</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="B33" t="b">
         <v>1</v>
@@ -5537,12 +5836,12 @@
         <v>79</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="B34" t="b">
         <v>1</v>
@@ -5551,12 +5850,12 @@
         <v>79</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="B35" t="b">
         <v>1</v>
@@ -5565,12 +5864,12 @@
         <v>79</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="B36" t="b">
         <v>1</v>
@@ -5579,12 +5878,12 @@
         <v>79</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
@@ -5593,49 +5892,63 @@
         <v>79</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
       <c r="B38" t="b">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="B39" t="b">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>217</v>
+        <v>234</v>
       </c>
       <c r="B40" t="b">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>218</v>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>236</v>
+      </c>
+      <c r="B41" t="b">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>